<commit_message>
Added more items to bill of materials spreadsheet.
</commit_message>
<xml_diff>
--- a/parts/bill_of_materials.xlsx
+++ b/parts/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\laser_tunnel\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD20015-A1C3-4072-91B7-F04D72F1A368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D867B752-0FB3-4BF0-B9DC-54129A504C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3189" yWindow="1243" windowWidth="22268" windowHeight="14974" xr2:uid="{C7A15FB5-B248-4CA2-8E4B-B85C1BCDD779}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>Laser Tunnel</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>DigiKey</t>
+  </si>
+  <si>
+    <t>audio jack</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cui-devices/SJ1-3533NG/738701</t>
   </si>
 </sst>
 </file>
@@ -592,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A265784A-A2E2-4F2C-B0D4-276F819350E1}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -668,18 +674,18 @@
         <v>1.0696249999999998</v>
       </c>
       <c r="G3" s="4">
-        <f>B3+D3+F3</f>
+        <f t="shared" ref="G3:G25" si="0">B3+D3+F3</f>
         <v>11.019625</v>
       </c>
       <c r="H3" s="4">
-        <f>G3/C3</f>
+        <f t="shared" ref="H3:H25" si="1">G3/C3</f>
         <v>11.019625</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" s="4">
-        <f>H3*I3</f>
+        <f t="shared" ref="J3:J25" si="2">H3*I3</f>
         <v>11.019625</v>
       </c>
       <c r="K3" t="s">
@@ -703,22 +709,22 @@
         <v>0</v>
       </c>
       <c r="F4" s="4">
-        <f t="shared" ref="F4:F25" si="0">(B4+D4+E4)*0.1075</f>
+        <f t="shared" ref="F4:F25" si="3">(B4+D4+E4)*0.1075</f>
         <v>0.64392499999999997</v>
       </c>
       <c r="G4" s="4">
-        <f>B4+D4+F4</f>
+        <f t="shared" si="0"/>
         <v>6.6339250000000005</v>
       </c>
       <c r="H4" s="4">
-        <f>G4/C4</f>
+        <f t="shared" si="1"/>
         <v>0.66339250000000005</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" s="4">
-        <f>H4*I4</f>
+        <f t="shared" si="2"/>
         <v>0.66339250000000005</v>
       </c>
       <c r="K4" s="3" t="s">
@@ -739,22 +745,22 @@
         <v>0</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G5" s="4">
-        <f>B5+D5+F5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H5" s="4">
-        <f>G5/C5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" s="4">
-        <f>H5*I5</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -772,22 +778,22 @@
         <v>0</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.85892500000000005</v>
       </c>
       <c r="G6" s="4">
-        <f>B6+D6+F6</f>
+        <f t="shared" si="0"/>
         <v>8.8489249999999995</v>
       </c>
       <c r="H6" s="4">
-        <f>G6/C6</f>
+        <f t="shared" si="1"/>
         <v>0.17697849999999998</v>
       </c>
       <c r="I6">
         <v>3</v>
       </c>
       <c r="J6" s="4">
-        <f>H6*I6</f>
+        <f t="shared" si="2"/>
         <v>0.5309355</v>
       </c>
       <c r="K6" t="s">
@@ -808,22 +814,22 @@
         <v>0</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G7" s="4">
-        <f>B7+D7+F7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7" s="4">
-        <f>G7/C7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I7">
         <v>3</v>
       </c>
       <c r="J7" s="4">
-        <f>H7*I7</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -841,22 +847,22 @@
         <v>0</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.64392499999999997</v>
       </c>
       <c r="G8" s="4">
-        <f>B8+D8+F8</f>
+        <f t="shared" si="0"/>
         <v>6.6339250000000005</v>
       </c>
       <c r="H8" s="4">
-        <f>G8/C8</f>
+        <f t="shared" si="1"/>
         <v>4.4226166666666671E-2</v>
       </c>
       <c r="I8">
         <v>3</v>
       </c>
       <c r="J8" s="4">
-        <f>H8*I8</f>
+        <f t="shared" si="2"/>
         <v>0.1326785</v>
       </c>
       <c r="K8" t="s">
@@ -877,22 +883,22 @@
         <v>0</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.0414249999999998</v>
       </c>
       <c r="G9" s="4">
-        <f>B9+D9+F9</f>
+        <f t="shared" si="0"/>
         <v>21.031424999999999</v>
       </c>
       <c r="H9" s="4">
-        <f>G9/C9</f>
+        <f t="shared" si="1"/>
         <v>7.0104749999999996</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" s="4">
-        <f>H9*I9</f>
+        <f t="shared" si="2"/>
         <v>7.0104749999999996</v>
       </c>
       <c r="K9" t="s">
@@ -913,22 +919,22 @@
         <v>0</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.396425</v>
       </c>
       <c r="G10" s="4">
-        <f>B10+D10+F10</f>
+        <f t="shared" si="0"/>
         <v>14.386425000000001</v>
       </c>
       <c r="H10" s="4">
-        <f>G10/C10</f>
+        <f t="shared" si="1"/>
         <v>2.8772850000000001</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" s="4">
-        <f>H10*I10</f>
+        <f t="shared" si="2"/>
         <v>2.8772850000000001</v>
       </c>
       <c r="K10" t="s">
@@ -949,22 +955,22 @@
         <v>0</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.64392499999999997</v>
       </c>
       <c r="G11" s="4">
-        <f>B11+D11+F11</f>
+        <f t="shared" si="0"/>
         <v>6.6339250000000005</v>
       </c>
       <c r="H11" s="4">
-        <f>G11/C11</f>
+        <f t="shared" si="1"/>
         <v>0.1326785</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="J11" s="4">
-        <f>H11*I11</f>
+        <f t="shared" si="2"/>
         <v>0.26535700000000001</v>
       </c>
       <c r="K11" t="s">
@@ -985,22 +991,22 @@
         <v>0</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.85892500000000005</v>
       </c>
       <c r="G12" s="4">
-        <f>B12+D12+F12</f>
+        <f t="shared" si="0"/>
         <v>8.8489249999999995</v>
       </c>
       <c r="H12" s="4">
-        <f>G12/C12</f>
+        <f t="shared" si="1"/>
         <v>0.44244624999999999</v>
       </c>
       <c r="I12">
         <v>2</v>
       </c>
       <c r="J12" s="4">
-        <f>H12*I12</f>
+        <f t="shared" si="2"/>
         <v>0.88489249999999997</v>
       </c>
       <c r="K12" t="s">
@@ -1012,32 +1018,36 @@
         <v>34</v>
       </c>
       <c r="B13" s="1">
-        <v>9.99</v>
+        <v>0.88</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
+      <c r="E13" s="4">
+        <f>B13*0.1</f>
+        <v>8.8000000000000009E-2</v>
+      </c>
       <c r="F13" s="4">
-        <f t="shared" si="0"/>
-        <v>1.073925</v>
+        <f t="shared" si="3"/>
+        <v>0.10406</v>
       </c>
       <c r="G13" s="4">
-        <f>B13+D13+F13</f>
-        <v>11.063925000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.98406000000000005</v>
       </c>
       <c r="H13" s="4">
-        <f>G13/C13</f>
-        <v>1.1063925000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.98406000000000005</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" s="4">
-        <f>H13*I13</f>
-        <v>1.1063925000000001</v>
+        <f t="shared" si="2"/>
+        <v>0.98406000000000005</v>
       </c>
       <c r="K13" t="s">
         <v>33</v>
@@ -1060,22 +1070,22 @@
         <v>0</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.5576749999999999</v>
       </c>
       <c r="G14" s="4">
-        <f>B14+D14+F14</f>
+        <f t="shared" si="0"/>
         <v>16.047675000000002</v>
       </c>
       <c r="H14" s="4">
-        <f>G14/C14</f>
+        <f t="shared" si="1"/>
         <v>0.26746125000000004</v>
       </c>
       <c r="I14">
         <v>2</v>
       </c>
       <c r="J14" s="4">
-        <f>H14*I14</f>
+        <f t="shared" si="2"/>
         <v>0.53492250000000008</v>
       </c>
       <c r="K14" t="s">
@@ -1096,22 +1106,22 @@
         <v>0</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.80517499999999997</v>
       </c>
       <c r="G15" s="4">
-        <f>B15+D15+F15</f>
+        <f t="shared" si="0"/>
         <v>8.2951750000000004</v>
       </c>
       <c r="H15" s="4">
-        <f>G15/C15</f>
+        <f t="shared" si="1"/>
         <v>0.16590350000000001</v>
       </c>
       <c r="I15">
         <v>2</v>
       </c>
       <c r="J15" s="4">
-        <f>H15*I15</f>
+        <f t="shared" si="2"/>
         <v>0.33180700000000002</v>
       </c>
       <c r="K15" t="s">
@@ -1132,22 +1142,22 @@
         <v>0</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.75142500000000001</v>
       </c>
       <c r="G16" s="4">
-        <f>B16+D16+F16</f>
+        <f t="shared" si="0"/>
         <v>7.7414250000000004</v>
       </c>
       <c r="H16" s="4">
-        <f>G16/C16</f>
+        <f t="shared" si="1"/>
         <v>7.7414250000000004E-2</v>
       </c>
       <c r="I16">
         <v>2</v>
       </c>
       <c r="J16" s="4">
-        <f>H16*I16</f>
+        <f t="shared" si="2"/>
         <v>0.15482850000000001</v>
       </c>
       <c r="K16" t="s">
@@ -1168,22 +1178,22 @@
         <v>0</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.64392499999999997</v>
       </c>
       <c r="G17" s="4">
-        <f>B17+D17+F17</f>
+        <f t="shared" si="0"/>
         <v>6.6339250000000005</v>
       </c>
       <c r="H17" s="4">
-        <f>G17/C17</f>
+        <f t="shared" si="1"/>
         <v>0.1326785</v>
       </c>
       <c r="I17">
         <v>2</v>
       </c>
       <c r="J17" s="4">
-        <f>H17*I17</f>
+        <f t="shared" si="2"/>
         <v>0.26535700000000001</v>
       </c>
       <c r="K17" t="s">
@@ -1204,22 +1214,22 @@
         <v>0</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.0414249999999998</v>
       </c>
       <c r="G18" s="4">
-        <f>B18+D18+F18</f>
+        <f t="shared" si="0"/>
         <v>21.031424999999999</v>
       </c>
       <c r="H18" s="4">
-        <f>G18/C18</f>
+        <f t="shared" si="1"/>
         <v>4.2062849999999994</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" s="4">
-        <f>H18*I18</f>
+        <f t="shared" si="2"/>
         <v>4.2062849999999994</v>
       </c>
       <c r="K18" t="s">
@@ -1240,22 +1250,22 @@
         <v>0</v>
       </c>
       <c r="F19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.6646750000000003</v>
       </c>
       <c r="G19" s="4">
-        <f>B19+D19+F19</f>
+        <f t="shared" si="0"/>
         <v>37.754675000000006</v>
       </c>
       <c r="H19" s="4">
-        <f>G19/C19</f>
+        <f t="shared" si="1"/>
         <v>3.1462229166666673</v>
       </c>
       <c r="I19">
         <v>1</v>
       </c>
       <c r="J19" s="4">
-        <f>H19*I19</f>
+        <f t="shared" si="2"/>
         <v>3.1462229166666673</v>
       </c>
       <c r="K19" s="3" t="s">
@@ -1283,22 +1293,22 @@
         <v>0.76400000000000001</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.90342999999999996</v>
       </c>
       <c r="G20" s="4">
-        <f>B20+D20+F20</f>
+        <f t="shared" si="0"/>
         <v>8.543429999999999</v>
       </c>
       <c r="H20" s="4">
-        <f>G20/C20</f>
+        <f t="shared" si="1"/>
         <v>0.85434299999999985</v>
       </c>
       <c r="I20">
         <v>2</v>
       </c>
       <c r="J20" s="4">
-        <f>H20*I20</f>
+        <f t="shared" si="2"/>
         <v>1.7086859999999997</v>
       </c>
       <c r="K20" s="3" t="s">
@@ -1326,22 +1336,22 @@
         <v>0.89000000000000012</v>
       </c>
       <c r="F21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.0524250000000002</v>
       </c>
       <c r="G21" s="4">
-        <f>B21+D21+F21</f>
+        <f t="shared" si="0"/>
         <v>9.9524249999999999</v>
       </c>
       <c r="H21" s="4">
-        <f>G21/C21</f>
+        <f t="shared" si="1"/>
         <v>0.49762125000000001</v>
       </c>
       <c r="I21">
         <v>1</v>
       </c>
       <c r="J21" s="4">
-        <f>H21*I21</f>
+        <f t="shared" si="2"/>
         <v>0.49762125000000001</v>
       </c>
       <c r="K21" t="s">
@@ -1365,22 +1375,22 @@
         <v>0</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.39990000000000003</v>
       </c>
       <c r="G22" s="4">
-        <f>B22+D22+F22</f>
+        <f t="shared" si="0"/>
         <v>4.1199000000000003</v>
       </c>
       <c r="H22" s="4">
-        <f>G22/C22</f>
+        <f t="shared" si="1"/>
         <v>4.5776666666666674E-2</v>
       </c>
       <c r="I22">
         <v>2</v>
       </c>
       <c r="J22" s="4">
-        <f>H22*I22</f>
+        <f t="shared" si="2"/>
         <v>9.1553333333333348E-2</v>
       </c>
       <c r="K22" t="s">
@@ -1404,22 +1414,22 @@
         <v>0</v>
       </c>
       <c r="F23" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.19350000000000001</v>
       </c>
       <c r="G23" s="4">
-        <f>B23+D23+F23</f>
+        <f t="shared" si="0"/>
         <v>1.9935</v>
       </c>
       <c r="H23" s="4">
-        <f>G23/C23</f>
+        <f t="shared" si="1"/>
         <v>3.9870000000000003E-2</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23" s="4">
-        <f>H23*I23</f>
+        <f t="shared" si="2"/>
         <v>3.9870000000000003E-2</v>
       </c>
       <c r="K23" t="s">
@@ -1443,22 +1453,22 @@
         <v>0</v>
       </c>
       <c r="F24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.23220000000000002</v>
       </c>
       <c r="G24" s="4">
-        <f>B24+D24+F24</f>
+        <f t="shared" si="0"/>
         <v>2.3922000000000003</v>
       </c>
       <c r="H24" s="4">
-        <f>G24/C24</f>
+        <f t="shared" si="1"/>
         <v>4.7844000000000005E-2</v>
       </c>
       <c r="I24">
         <v>1</v>
       </c>
       <c r="J24" s="4">
-        <f>H24*I24</f>
+        <f t="shared" si="2"/>
         <v>4.7844000000000005E-2</v>
       </c>
       <c r="K24" t="s">
@@ -1482,22 +1492,22 @@
         <v>0</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.19350000000000001</v>
       </c>
       <c r="G25" s="4">
-        <f>B25+D25+F25</f>
+        <f t="shared" si="0"/>
         <v>1.9935</v>
       </c>
       <c r="H25" s="4">
-        <f>G25/C25</f>
+        <f t="shared" si="1"/>
         <v>3.9870000000000003E-2</v>
       </c>
       <c r="I25">
         <v>1</v>
       </c>
       <c r="J25" s="4">
-        <f>H25*I25</f>
+        <f t="shared" si="2"/>
         <v>3.9870000000000003E-2</v>
       </c>
       <c r="K25" t="s">
@@ -1505,28 +1515,68 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B26" s="1"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="J26" s="4"/>
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="1">
+        <v>11.69</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
+        <f>B25*0.1</f>
+        <v>0.18000000000000002</v>
+      </c>
+      <c r="F26" s="4">
+        <f t="shared" ref="F26" si="4">(B26+D26+E26)*0.1075</f>
+        <v>1.276025</v>
+      </c>
+      <c r="G26" s="4">
+        <f t="shared" ref="G26" si="5">B26+D26+F26</f>
+        <v>12.966025</v>
+      </c>
+      <c r="H26" s="4">
+        <f t="shared" ref="H26" si="6">G26/C26</f>
+        <v>1.2966025000000001</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26" s="4">
+        <f t="shared" ref="J26" si="7">H26*I26</f>
+        <v>1.2966025000000001</v>
+      </c>
+      <c r="K26" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
+      <c r="B27" s="1"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B28" s="4">
         <f>SUM(B3:B26)</f>
-        <v>199.92999999999998</v>
-      </c>
-      <c r="I27" s="5">
+        <v>202.51</v>
+      </c>
+      <c r="I28" s="5">
         <f>SUM(I3:I26)</f>
-        <v>37</v>
-      </c>
-      <c r="J27" s="4">
+        <v>38</v>
+      </c>
+      <c r="J28" s="4">
         <f>SUM(J3:J26)</f>
-        <v>35.555900999999999</v>
+        <v>36.730170999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made final(?) part selections and updated the BOM.
</commit_message>
<xml_diff>
--- a/parts/bill_of_materials.xlsx
+++ b/parts/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\laser_tunnel\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D867B752-0FB3-4BF0-B9DC-54129A504C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B7BBC4-733C-4862-80F0-0B2B81D6C3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3189" yWindow="1243" windowWidth="22268" windowHeight="14974" xr2:uid="{C7A15FB5-B248-4CA2-8E4B-B85C1BCDD779}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Laser Tunnel</t>
   </si>
@@ -79,27 +79,12 @@
     <t>https://www.amazon.com/gp/product/B07H3VF3BF</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B07KP4KQ5M</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/gp/product/B07PVY4D52</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B07ZYNWJ1S</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/gp/product/B081SYT5F5</t>
-  </si>
-  <si>
     <t>screw terminal block (2-pin)</t>
   </si>
   <si>
-    <t>PCB protoboard</t>
-  </si>
-  <si>
-    <t>M4 washer</t>
-  </si>
-  <si>
     <t>M4 hex nut</t>
   </si>
   <si>
@@ -109,15 +94,6 @@
     <t>12-terminal header socket</t>
   </si>
   <si>
-    <t>Totals</t>
-  </si>
-  <si>
-    <t>3D-printed mirror holder</t>
-  </si>
-  <si>
-    <t>3D-printed bracket</t>
-  </si>
-  <si>
     <t>12V power adapter</t>
   </si>
   <si>
@@ -133,45 +109,21 @@
     <t>https://www.homedepot.com/p/Sterilite-6-Qt-Storage-Box-16426A60/308820126</t>
   </si>
   <si>
-    <t>https://www.amazon.com/DIKAVS-Breadboard-friendly-2-1mm-Barrel-Jack/dp/B074LK7G86</t>
-  </si>
-  <si>
     <t>2.1mmx5.5mm DC barrel jack</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/tensility-international-corp/54-00133/9685442</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/mechatronics-fan-group/G8020H12B1-6-RSR/8120048</t>
   </si>
   <si>
-    <t>M4 rubber washer (suppress vibes)</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/uxcell-Rubber-Washers-Inner-Diameter/dp/B07MBHWYKJ</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/Adhesive-0-78inch-Diameter-Fastener-organizing/dp/B08CL1Y348</t>
   </si>
   <si>
     <t>pair of hook-and-loop dots</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/nte-electronics-inc/500E-0079/11651214</t>
-  </si>
-  <si>
     <t>10 kOhm trimpot</t>
   </si>
   <si>
-    <t>https://www.amazon.com/MCIGICM-Breadboard-Trim-Potentiometer-Arduino/dp/B07S69443J</t>
-  </si>
-  <si>
-    <t>4-pin male fan header (Molex 0470531000)</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/molex/0470531000/2421261?s=N4IgTCBcDaILYHsA2BTAHgAgCwHYAMArAMwCMe5IAugL5A</t>
-  </si>
-  <si>
     <t>Purchase Price</t>
   </si>
   <si>
@@ -211,7 +163,52 @@
     <t>audio jack</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/cui-devices/SJ1-3533NG/738701</t>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>3D Printed Parts</t>
+  </si>
+  <si>
+    <t>bracket</t>
+  </si>
+  <si>
+    <t>mirror holders</t>
+  </si>
+  <si>
+    <t>4-pin fan header</t>
+  </si>
+  <si>
+    <t>180 Ohm resistor</t>
+  </si>
+  <si>
+    <t>push button switch</t>
+  </si>
+  <si>
+    <t>Amazon Total:</t>
+  </si>
+  <si>
+    <t>3D Printed Total:</t>
+  </si>
+  <si>
+    <t>DigiKey Total:</t>
+  </si>
+  <si>
+    <t>Grand Totals:</t>
+  </si>
+  <si>
+    <t>PCBway</t>
+  </si>
+  <si>
+    <t>PCBway Total:</t>
+  </si>
+  <si>
+    <t>DFPlayer Mini</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B07BDD8BF3</t>
+  </si>
+  <si>
+    <t>LED</t>
   </si>
 </sst>
 </file>
@@ -221,7 +218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +247,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -273,7 +278,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -282,6 +287,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -598,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A265784A-A2E2-4F2C-B0D4-276F819350E1}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -611,7 +618,7 @@
     <col min="3" max="3" width="12.23046875" customWidth="1"/>
     <col min="4" max="5" width="8.69140625" customWidth="1"/>
     <col min="6" max="6" width="9.3046875" customWidth="1"/>
-    <col min="7" max="7" width="7.765625" customWidth="1"/>
+    <col min="7" max="7" width="9.23046875" customWidth="1"/>
     <col min="9" max="9" width="8.3046875" customWidth="1"/>
     <col min="10" max="10" width="10.53515625" customWidth="1"/>
   </cols>
@@ -626,142 +633,114 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>9.9499999999999993</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <f>(B3+D3+E3)*0.1075</f>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <f>(B4+D4+E4)*0.1075</f>
         <v>1.0696249999999998</v>
       </c>
-      <c r="G3" s="4">
-        <f t="shared" ref="G3:G25" si="0">B3+D3+F3</f>
+      <c r="G4" s="4">
+        <f t="shared" ref="G4:G14" si="0">B4+D4+F4</f>
         <v>11.019625</v>
       </c>
-      <c r="H3" s="4">
-        <f t="shared" ref="H3:H25" si="1">G3/C3</f>
+      <c r="H4" s="4">
+        <f t="shared" ref="H4:H14" si="1">G4/C4</f>
         <v>11.019625</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" s="4">
-        <f t="shared" ref="J3:J25" si="2">H3*I3</f>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" ref="J4:J14" si="2">H4*I4</f>
         <v>11.019625</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K4" t="s">
         <v>7</v>
       </c>
-      <c r="L3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>5.99</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>10</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <f t="shared" ref="F4:F25" si="3">(B4+D4+E4)*0.1075</f>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" ref="F5:F14" si="3">(B5+D5+E5)*0.1075</f>
         <v>0.64392499999999997</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G5" s="4">
         <f t="shared" si="0"/>
         <v>6.6339250000000005</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H5" s="4">
         <f t="shared" si="1"/>
         <v>0.66339250000000005</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
         <f t="shared" si="2"/>
         <v>0.66339250000000005</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
@@ -802,688 +781,529 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>5.99</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.64392499999999997</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.6339250000000005</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.4226166666666671E-2</v>
       </c>
       <c r="I7">
         <v>3</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1326785</v>
+      </c>
+      <c r="K7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1">
-        <v>5.99</v>
+        <v>18.989999999999998</v>
       </c>
       <c r="C8">
-        <v>150</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="3"/>
-        <v>0.64392499999999997</v>
+        <v>2.0414249999999998</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="0"/>
-        <v>6.6339250000000005</v>
+        <v>21.031424999999999</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="1"/>
-        <v>4.4226166666666671E-2</v>
+        <v>7.0104749999999996</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="2"/>
-        <v>0.1326785</v>
+        <v>7.0104749999999996</v>
       </c>
       <c r="K8" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1">
-        <v>18.989999999999998</v>
+        <v>12.99</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="3"/>
-        <v>2.0414249999999998</v>
+        <v>1.396425</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
-        <v>21.031424999999999</v>
+        <v>14.386425000000001</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="1"/>
-        <v>7.0104749999999996</v>
+        <v>2.8772850000000001</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="2"/>
-        <v>7.0104749999999996</v>
-      </c>
-      <c r="K9" t="s">
-        <v>11</v>
+        <v>2.8772850000000001</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
-        <v>12.99</v>
+        <v>5.99</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="3"/>
-        <v>1.396425</v>
+        <v>0.64392499999999997</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="0"/>
-        <v>14.386425000000001</v>
+        <v>6.6339250000000005</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="1"/>
-        <v>2.8772850000000001</v>
+        <v>0.1326785</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="2"/>
-        <v>2.8772850000000001</v>
+        <v>0.26535700000000001</v>
       </c>
       <c r="K10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
-        <v>5.99</v>
+        <v>14.49</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="3"/>
-        <v>0.64392499999999997</v>
+        <v>1.5576749999999999</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="0"/>
-        <v>6.6339250000000005</v>
+        <v>16.047675000000002</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="1"/>
-        <v>0.1326785</v>
+        <v>0.26746125000000004</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="2"/>
-        <v>0.26535700000000001</v>
+        <v>0.53492250000000008</v>
       </c>
       <c r="K11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1">
-        <v>7.99</v>
+        <v>7.49</v>
       </c>
       <c r="C12">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="3"/>
-        <v>0.85892500000000005</v>
+        <v>0.80517499999999997</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="0"/>
-        <v>8.8489249999999995</v>
+        <v>8.2951750000000004</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="1"/>
-        <v>0.44244624999999999</v>
+        <v>0.16590350000000001</v>
       </c>
       <c r="I12">
         <v>2</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="2"/>
-        <v>0.88489249999999997</v>
+        <v>0.33180700000000002</v>
       </c>
       <c r="K12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
-        <v>0.88</v>
+        <v>18.989999999999998</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>0</v>
-      </c>
-      <c r="E13" s="4">
-        <f>B13*0.1</f>
-        <v>8.8000000000000009E-2</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" si="3"/>
-        <v>0.10406</v>
+        <v>2.0414249999999998</v>
       </c>
       <c r="G13" s="4">
         <f t="shared" si="0"/>
-        <v>0.98406000000000005</v>
+        <v>21.031424999999999</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="1"/>
-        <v>0.98406000000000005</v>
+        <v>4.2062849999999994</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="2"/>
-        <v>0.98406000000000005</v>
+        <v>4.2062849999999994</v>
       </c>
       <c r="K13" t="s">
-        <v>33</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1">
-        <v>14.49</v>
+        <v>34.090000000000003</v>
       </c>
       <c r="C14">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="F14" s="4">
         <f t="shared" si="3"/>
-        <v>1.5576749999999999</v>
+        <v>3.6646750000000003</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="0"/>
-        <v>16.047675000000002</v>
+        <v>37.754675000000006</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" si="1"/>
-        <v>0.26746125000000004</v>
+        <v>3.1462229166666673</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="2"/>
-        <v>0.53492250000000008</v>
-      </c>
-      <c r="K14" t="s">
-        <v>13</v>
+        <v>3.1462229166666673</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>22</v>
+      <c r="A15" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="B15" s="1">
-        <v>7.49</v>
-      </c>
-      <c r="C15">
-        <v>50</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" si="3"/>
-        <v>0.80517499999999997</v>
-      </c>
-      <c r="G15" s="4">
-        <f t="shared" si="0"/>
-        <v>8.2951750000000004</v>
-      </c>
-      <c r="H15" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16590350000000001</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15" s="4">
-        <f t="shared" si="2"/>
-        <v>0.33180700000000002</v>
-      </c>
-      <c r="K15" t="s">
-        <v>14</v>
-      </c>
+        <f>SUM(B4:B14)</f>
+        <v>142.94999999999999</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="1">
+        <f>SUM(G4:G14)</f>
+        <v>158.317125</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="7">
+        <f>SUM(I4:I14)</f>
+        <v>18</v>
+      </c>
+      <c r="J15" s="1">
+        <f>SUM(J4:J14)</f>
+        <v>30.718985916666668</v>
+      </c>
+      <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="1">
-        <v>6.99</v>
-      </c>
-      <c r="C16">
-        <v>100</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
-        <f t="shared" si="3"/>
-        <v>0.75142500000000001</v>
-      </c>
-      <c r="G16" s="4">
-        <f t="shared" si="0"/>
-        <v>7.7414250000000004</v>
-      </c>
-      <c r="H16" s="4">
-        <f t="shared" si="1"/>
-        <v>7.7414250000000004E-2</v>
-      </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
-      <c r="J16" s="4">
-        <f t="shared" si="2"/>
-        <v>0.15482850000000001</v>
-      </c>
-      <c r="K16" t="s">
-        <v>15</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="1">
-        <v>5.99</v>
-      </c>
-      <c r="C17">
-        <v>50</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="F17" s="4">
-        <f t="shared" si="3"/>
-        <v>0.64392499999999997</v>
-      </c>
-      <c r="G17" s="4">
-        <f t="shared" si="0"/>
-        <v>6.6339250000000005</v>
-      </c>
-      <c r="H17" s="4">
-        <f t="shared" si="1"/>
-        <v>0.1326785</v>
-      </c>
-      <c r="I17">
-        <v>2</v>
-      </c>
-      <c r="J17" s="4">
-        <f t="shared" si="2"/>
-        <v>0.26535700000000001</v>
-      </c>
-      <c r="K17" t="s">
-        <v>38</v>
-      </c>
+      <c r="A17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1">
-        <v>18.989999999999998</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="3"/>
-        <v>2.0414249999999998</v>
+        <f>(B18+D18+E18)*0.1075</f>
+        <v>0</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="0"/>
-        <v>21.031424999999999</v>
+        <f>B18+D18+F18</f>
+        <v>0</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="1"/>
-        <v>4.2062849999999994</v>
+        <f>G18/C18</f>
+        <v>0</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" s="4">
-        <f t="shared" si="2"/>
-        <v>4.2062849999999994</v>
-      </c>
-      <c r="K18" t="s">
-        <v>29</v>
+        <f>H18*I18</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B19" s="1">
-        <v>34.090000000000003</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="F19" s="4">
-        <f t="shared" si="3"/>
-        <v>3.6646750000000003</v>
+        <f>(B19+D19+E19)*0.1075</f>
+        <v>0</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" si="0"/>
-        <v>37.754675000000006</v>
+        <f>B19+D19+F19</f>
+        <v>0</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="1"/>
-        <v>3.1462229166666673</v>
+        <f>G19/C19</f>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J19" s="4">
-        <f t="shared" si="2"/>
-        <v>3.1462229166666673</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L19" t="s">
-        <v>32</v>
+        <f>H19*I19</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>42</v>
+      <c r="A20" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="B20" s="1">
-        <v>7.64</v>
-      </c>
-      <c r="C20">
-        <v>10</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4">
-        <f>B20*0.1</f>
-        <v>0.76400000000000001</v>
-      </c>
-      <c r="F20" s="4">
-        <f t="shared" si="3"/>
-        <v>0.90342999999999996</v>
-      </c>
-      <c r="G20" s="4">
-        <f t="shared" si="0"/>
-        <v>8.543429999999999</v>
-      </c>
-      <c r="H20" s="4">
-        <f t="shared" si="1"/>
-        <v>0.85434299999999985</v>
-      </c>
-      <c r="I20">
-        <v>2</v>
-      </c>
-      <c r="J20" s="4">
-        <f t="shared" si="2"/>
-        <v>1.7086859999999997</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L20" s="3" t="s">
+        <f>SUM(B18:B19)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="1">
+        <f>SUM(G18:G19)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="7">
+        <f>SUM(I18:I19)</f>
+        <v>4</v>
+      </c>
+      <c r="J20" s="1">
+        <f>SUM(J18:J19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B21" s="1"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A22" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="1">
-        <v>8.9</v>
-      </c>
-      <c r="C21">
-        <v>20</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" s="4">
-        <f>B21*0.1</f>
-        <v>0.89000000000000012</v>
-      </c>
-      <c r="F21" s="4">
-        <f t="shared" si="3"/>
-        <v>1.0524250000000002</v>
-      </c>
-      <c r="G21" s="4">
-        <f t="shared" si="0"/>
-        <v>9.9524249999999999</v>
-      </c>
-      <c r="H21" s="4">
-        <f t="shared" si="1"/>
-        <v>0.49762125000000001</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21" s="4">
-        <f t="shared" si="2"/>
-        <v>0.49762125000000001</v>
-      </c>
-      <c r="K21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="1">
-        <v>3.72</v>
-      </c>
-      <c r="C22">
-        <v>90</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0</v>
-      </c>
-      <c r="F22" s="4">
-        <f t="shared" si="3"/>
-        <v>0.39990000000000003</v>
-      </c>
-      <c r="G22" s="4">
-        <f t="shared" si="0"/>
-        <v>4.1199000000000003</v>
-      </c>
-      <c r="H22" s="4">
-        <f t="shared" si="1"/>
-        <v>4.5776666666666674E-2</v>
-      </c>
-      <c r="I22">
-        <v>2</v>
-      </c>
-      <c r="J22" s="4">
-        <f t="shared" si="2"/>
-        <v>9.1553333333333348E-2</v>
-      </c>
-      <c r="K22" t="s">
-        <v>57</v>
-      </c>
+      <c r="B22" s="1"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B23" s="1">
-        <v>1.8</v>
+        <v>0.53</v>
       </c>
       <c r="C23">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23" s="4">
-        <v>0</v>
+        <f>B23*0.1</f>
+        <v>5.3000000000000005E-2</v>
       </c>
       <c r="F23" s="4">
-        <f t="shared" si="3"/>
-        <v>0.19350000000000001</v>
+        <f t="shared" ref="F23" si="4">(B23+D23+E23)*0.1075</f>
+        <v>6.2672500000000006E-2</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" si="0"/>
-        <v>1.9935</v>
+        <f t="shared" ref="G23" si="5">B23+D23+F23</f>
+        <v>0.59267250000000005</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="1"/>
-        <v>3.9870000000000003E-2</v>
+        <f t="shared" ref="H23" si="6">G23/C23</f>
+        <v>0.59267250000000005</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23" s="4">
-        <f t="shared" si="2"/>
-        <v>3.9870000000000003E-2</v>
-      </c>
-      <c r="K23" t="s">
-        <v>57</v>
+        <f t="shared" ref="J23" si="7">H23*I23</f>
+        <v>0.59267250000000005</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="B24" s="1">
-        <v>2.16</v>
+        <v>1.7</v>
       </c>
       <c r="C24">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24" s="4">
-        <v>0</v>
+        <f>B24*0.1</f>
+        <v>0.17</v>
       </c>
       <c r="F24" s="4">
-        <f t="shared" si="3"/>
-        <v>0.23220000000000002</v>
+        <f>(B24+D24+E24)*0.1075</f>
+        <v>0.20102499999999998</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" si="0"/>
-        <v>2.3922000000000003</v>
+        <f>B24+D24+F24</f>
+        <v>1.901025</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="1"/>
-        <v>4.7844000000000005E-2</v>
+        <f>G24/C24</f>
+        <v>0.95051249999999998</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J24" s="4">
-        <f t="shared" si="2"/>
-        <v>4.7844000000000005E-2</v>
-      </c>
-      <c r="K24" t="s">
-        <v>57</v>
+        <f>H24*I24</f>
+        <v>1.901025</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1">
-        <v>1.8</v>
+        <v>0.81</v>
       </c>
       <c r="C25">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1492,102 +1312,458 @@
         <v>0</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" si="3"/>
-        <v>0.19350000000000001</v>
+        <f>(B25+D25+E25)*0.1075</f>
+        <v>8.7075E-2</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="0"/>
-        <v>1.9935</v>
+        <f>B25+D25+F25</f>
+        <v>0.89707500000000007</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="1"/>
-        <v>3.9870000000000003E-2</v>
+        <f>G25/C25</f>
+        <v>0.89707500000000007</v>
       </c>
       <c r="I25">
         <v>1</v>
       </c>
       <c r="J25" s="4">
-        <f t="shared" si="2"/>
-        <v>3.9870000000000003E-2</v>
-      </c>
-      <c r="K25" t="s">
-        <v>57</v>
-      </c>
+        <f>H25*I25</f>
+        <v>0.89707500000000007</v>
+      </c>
+      <c r="L25" s="3"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B26" s="1">
-        <v>11.69</v>
+        <v>1.38</v>
       </c>
       <c r="C26">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26" s="4">
-        <f>B25*0.1</f>
-        <v>0.18000000000000002</v>
+        <f>B30*0.1</f>
+        <v>0.03</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" ref="F26" si="4">(B26+D26+E26)*0.1075</f>
-        <v>1.276025</v>
+        <f t="shared" ref="F26" si="8">(B26+D26+E26)*0.1075</f>
+        <v>0.15157499999999999</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" ref="G26" si="5">B26+D26+F26</f>
-        <v>12.966025</v>
+        <f t="shared" ref="G26" si="9">B26+D26+F26</f>
+        <v>1.5315749999999999</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" ref="H26" si="6">G26/C26</f>
-        <v>1.2966025000000001</v>
+        <f t="shared" ref="H26" si="10">G26/C26</f>
+        <v>1.5315749999999999</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
       <c r="J26" s="4">
-        <f t="shared" ref="J26" si="7">H26*I26</f>
-        <v>1.2966025000000001</v>
-      </c>
-      <c r="K26" t="s">
-        <v>59</v>
+        <f t="shared" ref="J26" si="11">H26*I26</f>
+        <v>1.5315749999999999</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B27" s="1"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="J27" s="4"/>
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <f>(B27+D27+E27)*0.1075</f>
+        <v>4.7300000000000002E-2</v>
+      </c>
+      <c r="G27" s="4">
+        <f>B27+D27+F27</f>
+        <v>0.48730000000000001</v>
+      </c>
+      <c r="H27" s="4">
+        <f>G27/C27</f>
+        <v>0.48730000000000001</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27" s="4">
+        <f>H27*I27</f>
+        <v>0.48730000000000001</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="4">
-        <f>SUM(B3:B26)</f>
-        <v>202.51</v>
-      </c>
-      <c r="I28" s="5">
-        <f>SUM(I3:I26)</f>
+        <v>39</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <f>(B28+D28+E28)*0.1075</f>
+        <v>2.1500000000000002E-2</v>
+      </c>
+      <c r="G28" s="4">
+        <f>B28+D28+F28</f>
+        <v>0.2215</v>
+      </c>
+      <c r="H28" s="4">
+        <f>G28/C28</f>
+        <v>0.11075</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28" s="4">
+        <f>H28*I28</f>
+        <v>0.2215</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
         <v>38</v>
       </c>
-      <c r="J28" s="4">
-        <f>SUM(J3:J26)</f>
-        <v>36.730170999999999</v>
+      <c r="B29" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <f>(B29+D29+E29)*0.1075</f>
+        <v>2.1500000000000002E-2</v>
+      </c>
+      <c r="G29" s="4">
+        <f>B29+D29+F29</f>
+        <v>0.2215</v>
+      </c>
+      <c r="H29" s="4">
+        <f>G29/C29</f>
+        <v>0.11075</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29" s="4">
+        <f>H29*I29</f>
+        <v>0.2215</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <f>(B30+D30+E30)*0.1075</f>
+        <v>3.2250000000000001E-2</v>
+      </c>
+      <c r="G30" s="4">
+        <f>B30+D30+F30</f>
+        <v>0.33224999999999999</v>
+      </c>
+      <c r="H30" s="4">
+        <f>G30/C30</f>
+        <v>0.11075</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="J30" s="4">
+        <f>H30*I30</f>
+        <v>0.33224999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4">
+        <f>(B31+D31+E31)*0.1075</f>
+        <v>1.0750000000000001E-2</v>
+      </c>
+      <c r="G31" s="4">
+        <f>B31+D31+F31</f>
+        <v>0.11075</v>
+      </c>
+      <c r="H31" s="4">
+        <f>G31/C31</f>
+        <v>0.11075</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31" s="4">
+        <f>H31*I31</f>
+        <v>0.11075</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1.56</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4">
+        <f>B32*0.1</f>
+        <v>0.15600000000000003</v>
+      </c>
+      <c r="F32" s="4">
+        <f>(B32+D32+E32)*0.1075</f>
+        <v>0.18447000000000002</v>
+      </c>
+      <c r="G32" s="4">
+        <f>B32+D32+F32</f>
+        <v>1.7444700000000002</v>
+      </c>
+      <c r="H32" s="4">
+        <f>G32/C32</f>
+        <v>0.87223500000000009</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32" s="4">
+        <f>H32*I32</f>
+        <v>1.7444700000000002</v>
+      </c>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4">
+        <f>B33*0.1</f>
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="F33" s="4">
+        <f>(B33+D33+E33)*0.1075</f>
+        <v>1.5372500000000001E-2</v>
+      </c>
+      <c r="G33" s="4">
+        <f>B33+D33+F33</f>
+        <v>0.14537250000000002</v>
+      </c>
+      <c r="H33" s="4">
+        <f>G33/C33</f>
+        <v>0.14537250000000002</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33" s="4">
+        <f>H33*I33</f>
+        <v>0.14537250000000002</v>
+      </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4">
+        <f>B34*0.1</f>
+        <v>0.03</v>
+      </c>
+      <c r="F34" s="4">
+        <f>(B34+D34+E34)*0.1075</f>
+        <v>3.5474999999999993E-2</v>
+      </c>
+      <c r="G34" s="4">
+        <f>B34+D34+F34</f>
+        <v>0.33547499999999997</v>
+      </c>
+      <c r="H34" s="4">
+        <f>G34/C34</f>
+        <v>0.33547499999999997</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34" s="4">
+        <f>H34*I34</f>
+        <v>0.33547499999999997</v>
+      </c>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="1">
+        <f>SUM(B23:B34)</f>
+        <v>7.65</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="1">
+        <f>SUM(G23:G34)</f>
+        <v>8.5209650000000021</v>
+      </c>
+      <c r="H35" s="4"/>
+      <c r="I35">
+        <f>SUM(I23:I34)</f>
+        <v>18</v>
+      </c>
+      <c r="J35" s="4">
+        <f>SUM(J23:J34)</f>
+        <v>8.5209650000000021</v>
+      </c>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A36" s="6"/>
+      <c r="B36" s="1"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A37" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A38" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A39" s="6"/>
+      <c r="B39" s="1"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A40" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="4">
+        <f>B15+B20+B35+B38</f>
+        <v>150.6</v>
+      </c>
+      <c r="G40" s="4">
+        <f>G15+G20+G35+G38</f>
+        <v>166.83808999999999</v>
+      </c>
+      <c r="I40" s="5">
+        <f>I15+I20+I35+I38</f>
+        <v>40</v>
+      </c>
+      <c r="J40" s="1">
+        <f>J15+J20+J35+J38</f>
+        <v>39.239950916666672</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K4" r:id="rId1" xr:uid="{ACAC5234-DDA0-4969-B5FE-D166D7000F40}"/>
-    <hyperlink ref="K19" r:id="rId2" xr:uid="{71225EA3-939E-4F2C-8578-429F24215C0C}"/>
-    <hyperlink ref="L13" r:id="rId3" xr:uid="{F056419B-B686-40FF-89F9-86DF9119F0A3}"/>
-    <hyperlink ref="K20" r:id="rId4" xr:uid="{9446B96F-FFED-41E0-80E8-03E074521A78}"/>
-    <hyperlink ref="L20" r:id="rId5" xr:uid="{23DB0E81-46EB-402F-93A6-7BE6E7BA250A}"/>
+    <hyperlink ref="K5" r:id="rId1" xr:uid="{ACAC5234-DDA0-4969-B5FE-D166D7000F40}"/>
+    <hyperlink ref="K14" r:id="rId2" xr:uid="{71225EA3-939E-4F2C-8578-429F24215C0C}"/>
+    <hyperlink ref="K9" r:id="rId3" xr:uid="{AED873F4-67F0-430A-8DE3-7AABA9CDF44E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Moved the header sockets to the DigiKey list.
</commit_message>
<xml_diff>
--- a/parts/bill_of_materials.xlsx
+++ b/parts/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\laser_tunnel\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B7BBC4-733C-4862-80F0-0B2B81D6C3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891227A6-8872-44E5-9CBE-85B5E76A6E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3189" yWindow="1243" windowWidth="22268" windowHeight="14974" xr2:uid="{C7A15FB5-B248-4CA2-8E4B-B85C1BCDD779}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Laser Tunnel</t>
   </si>
@@ -79,9 +79,6 @@
     <t>https://www.amazon.com/gp/product/B07H3VF3BF</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B07PVY4D52</t>
-  </si>
-  <si>
     <t>screw terminal block (2-pin)</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>M4x35mm machine screw</t>
   </si>
   <si>
-    <t>12-terminal header socket</t>
-  </si>
-  <si>
     <t>12V power adapter</t>
   </si>
   <si>
@@ -209,6 +203,15 @@
   </si>
   <si>
     <t>LED</t>
+  </si>
+  <si>
+    <t>PCB fabrication</t>
+  </si>
+  <si>
+    <t>8-pin header socket for DFPlayer</t>
+  </si>
+  <si>
+    <t>12-pin header socket for Pro Mini</t>
   </si>
 </sst>
 </file>
@@ -278,7 +281,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -289,6 +292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -605,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A265784A-A2E2-4F2C-B0D4-276F819350E1}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -633,31 +637,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
         <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
       </c>
       <c r="K2" t="s">
         <v>4</v>
@@ -665,7 +669,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
@@ -678,7 +682,7 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="4">
@@ -686,25 +690,25 @@
         <v>1.0696249999999998</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" ref="G4:G14" si="0">B4+D4+F4</f>
+        <f t="shared" ref="G4:G13" si="0">B4+D4+F4</f>
         <v>11.019625</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" ref="H4:H14" si="1">G4/C4</f>
+        <f t="shared" ref="H4:H13" si="1">G4/C4</f>
         <v>11.019625</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" s="4">
-        <f t="shared" ref="J4:J14" si="2">H4*I4</f>
+        <f t="shared" ref="J4:J13" si="2">H4*I4</f>
         <v>11.019625</v>
       </c>
       <c r="K4" t="s">
         <v>7</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
@@ -717,11 +721,11 @@
       <c r="C5">
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>0</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" ref="F5:F14" si="3">(B5+D5+E5)*0.1075</f>
+        <f t="shared" ref="F5:F13" si="3">(B5+D5+E5)*0.1075</f>
         <v>0.64392499999999997</v>
       </c>
       <c r="G5" s="4">
@@ -753,7 +757,7 @@
       <c r="C6">
         <v>50</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>0</v>
       </c>
       <c r="F6" s="4">
@@ -781,7 +785,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
         <v>5.99</v>
@@ -789,7 +793,7 @@
       <c r="C7">
         <v>150</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="F7" s="4">
@@ -812,7 +816,7 @@
         <v>0.1326785</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
@@ -825,7 +829,7 @@
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>0</v>
       </c>
       <c r="F8" s="4">
@@ -853,7 +857,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="1">
         <v>12.99</v>
@@ -861,7 +865,7 @@
       <c r="C9">
         <v>5</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>0</v>
       </c>
       <c r="F9" s="4">
@@ -884,115 +888,115 @@
         <v>2.8772850000000001</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
-        <v>5.99</v>
+        <v>14.49</v>
       </c>
       <c r="C10">
-        <v>50</v>
-      </c>
-      <c r="D10">
+        <v>60</v>
+      </c>
+      <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="3"/>
-        <v>0.64392499999999997</v>
+        <v>1.5576749999999999</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="0"/>
-        <v>6.6339250000000005</v>
+        <v>16.047675000000002</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="1"/>
-        <v>0.1326785</v>
+        <v>0.26746125000000004</v>
       </c>
       <c r="I10">
         <v>2</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="2"/>
-        <v>0.26535700000000001</v>
+        <v>0.53492250000000008</v>
       </c>
       <c r="K10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1">
-        <v>14.49</v>
+        <v>7.49</v>
       </c>
       <c r="C11">
-        <v>60</v>
-      </c>
-      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="3"/>
-        <v>1.5576749999999999</v>
+        <v>0.80517499999999997</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="0"/>
-        <v>16.047675000000002</v>
+        <v>8.2951750000000004</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="1"/>
-        <v>0.26746125000000004</v>
+        <v>0.16590350000000001</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="2"/>
-        <v>0.53492250000000008</v>
+        <v>0.33180700000000002</v>
       </c>
       <c r="K11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1">
-        <v>7.49</v>
+        <v>18.989999999999998</v>
       </c>
       <c r="C12">
-        <v>50</v>
-      </c>
-      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="3"/>
-        <v>0.80517499999999997</v>
+        <v>2.0414249999999998</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="0"/>
-        <v>8.2951750000000004</v>
+        <v>21.031424999999999</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="1"/>
-        <v>0.16590350000000001</v>
+        <v>4.2062849999999994</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="2"/>
-        <v>0.33180700000000002</v>
+        <v>4.2062849999999994</v>
       </c>
       <c r="K12" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
@@ -1000,101 +1004,76 @@
         <v>20</v>
       </c>
       <c r="B13" s="1">
-        <v>18.989999999999998</v>
+        <v>34.090000000000003</v>
       </c>
       <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1">
         <v>0</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" si="3"/>
-        <v>2.0414249999999998</v>
+        <v>3.6646750000000003</v>
       </c>
       <c r="G13" s="4">
         <f t="shared" si="0"/>
-        <v>21.031424999999999</v>
+        <v>37.754675000000006</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="1"/>
-        <v>4.2062849999999994</v>
+        <v>3.1462229166666673</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="2"/>
-        <v>4.2062849999999994</v>
-      </c>
-      <c r="K13" t="s">
+        <v>3.1462229166666673</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="L13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>22</v>
+      <c r="A14" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B14" s="1">
-        <v>34.090000000000003</v>
-      </c>
-      <c r="C14">
-        <v>12</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="3"/>
-        <v>3.6646750000000003</v>
-      </c>
-      <c r="G14" s="4">
-        <f t="shared" si="0"/>
-        <v>37.754675000000006</v>
-      </c>
-      <c r="H14" s="4">
-        <f t="shared" si="1"/>
-        <v>3.1462229166666673</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14" s="4">
-        <f t="shared" si="2"/>
-        <v>3.1462229166666673</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" t="s">
-        <v>24</v>
-      </c>
+        <f>SUM(B4:B13)</f>
+        <v>136.95999999999998</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="1">
+        <f>SUM(G4:G13)</f>
+        <v>151.6832</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="7">
+        <f>SUM(I4:I13)</f>
+        <v>16</v>
+      </c>
+      <c r="J14" s="1">
+        <f>SUM(J4:J13)</f>
+        <v>30.453628916666666</v>
+      </c>
+      <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A15" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="1">
-        <f>SUM(B4:B14)</f>
-        <v>142.94999999999999</v>
-      </c>
+      <c r="B15" s="1"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="1">
-        <f>SUM(G4:G14)</f>
-        <v>158.317125</v>
-      </c>
+      <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="7">
-        <f>SUM(I4:I14)</f>
-        <v>18</v>
-      </c>
-      <c r="J15" s="1">
-        <f>SUM(J4:J14)</f>
-        <v>30.718985916666668</v>
-      </c>
-      <c r="K15" s="3"/>
+      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A16" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="B16" s="1"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1103,19 +1082,41 @@
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <f>(B17+D17+E17)*0.1075</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <f>B17+D17+F17</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <f>G17/C17</f>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17" s="4">
+        <f>H17*I17</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -1123,7 +1124,7 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>0</v>
       </c>
       <c r="F18" s="4">
@@ -1139,7 +1140,7 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J18" s="4">
         <f>H18*I18</f>
@@ -1147,62 +1148,40 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>46</v>
+      <c r="A19" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="F19" s="4">
-        <f>(B19+D19+E19)*0.1075</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="4">
-        <f>B19+D19+F19</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="4">
-        <f>G19/C19</f>
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>3</v>
-      </c>
-      <c r="J19" s="4">
-        <f>H19*I19</f>
+        <f>SUM(B17:B18)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="1">
+        <f>SUM(G17:G18)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="7">
+        <f>SUM(I17:I18)</f>
+        <v>4</v>
+      </c>
+      <c r="J19" s="1">
+        <f>SUM(J17:J18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A20" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="1">
-        <f>SUM(B18:B19)</f>
-        <v>0</v>
-      </c>
+      <c r="B20" s="1"/>
+      <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="1">
-        <f>SUM(G18:G19)</f>
-        <v>0</v>
-      </c>
+      <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="7">
-        <f>SUM(I18:I19)</f>
-        <v>4</v>
-      </c>
-      <c r="J20" s="1">
-        <f>SUM(J18:J19)</f>
-        <v>0</v>
-      </c>
+      <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A21" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="B21" s="1"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1211,162 +1190,187 @@
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A22" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4">
+        <f>B22*0.1</f>
+        <v>5.3000000000000005E-2</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" ref="F22" si="4">(B22+D22+E22)*0.1075</f>
+        <v>6.2672500000000006E-2</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" ref="G22" si="5">B22+D22+F22</f>
+        <v>0.59267250000000005</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" ref="H22" si="6">G22/C22</f>
+        <v>0.59267250000000005</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" ref="J22" si="7">H22*I22</f>
+        <v>0.59267250000000005</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1">
-        <v>0.53</v>
+        <v>1.7</v>
       </c>
       <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
         <v>0</v>
       </c>
       <c r="E23" s="4">
         <f>B23*0.1</f>
-        <v>5.3000000000000005E-2</v>
+        <v>0.17</v>
       </c>
       <c r="F23" s="4">
-        <f t="shared" ref="F23" si="4">(B23+D23+E23)*0.1075</f>
-        <v>6.2672500000000006E-2</v>
+        <f>(B23+D23+E23)*0.1075</f>
+        <v>0.20102499999999998</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" ref="G23" si="5">B23+D23+F23</f>
-        <v>0.59267250000000005</v>
+        <f>B23+D23+F23</f>
+        <v>1.901025</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" ref="H23" si="6">G23/C23</f>
-        <v>0.59267250000000005</v>
+        <f>G23/C23</f>
+        <v>0.95051249999999998</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J23" s="4">
-        <f t="shared" ref="J23" si="7">H23*I23</f>
-        <v>0.59267250000000005</v>
+        <f>H23*I23</f>
+        <v>1.901025</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>1.7</v>
+        <v>0.81</v>
       </c>
       <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" s="4">
-        <f>B24*0.1</f>
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="F24" s="4">
         <f>(B24+D24+E24)*0.1075</f>
-        <v>0.20102499999999998</v>
+        <v>8.7075E-2</v>
       </c>
       <c r="G24" s="4">
         <f>B24+D24+F24</f>
-        <v>1.901025</v>
+        <v>0.89707500000000007</v>
       </c>
       <c r="H24" s="4">
         <f>G24/C24</f>
-        <v>0.95051249999999998</v>
+        <v>0.89707500000000007</v>
       </c>
       <c r="I24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J24" s="4">
         <f>H24*I24</f>
-        <v>1.901025</v>
-      </c>
+        <v>0.89707500000000007</v>
+      </c>
+      <c r="L24" s="3"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B25" s="1">
-        <v>0.81</v>
+        <v>1.38</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>0</v>
       </c>
       <c r="E25" s="4">
-        <v>0</v>
+        <f>B29*0.1</f>
+        <v>0.03</v>
       </c>
       <c r="F25" s="4">
-        <f>(B25+D25+E25)*0.1075</f>
-        <v>8.7075E-2</v>
+        <f t="shared" ref="F25" si="8">(B25+D25+E25)*0.1075</f>
+        <v>0.15157499999999999</v>
       </c>
       <c r="G25" s="4">
-        <f>B25+D25+F25</f>
-        <v>0.89707500000000007</v>
+        <f t="shared" ref="G25" si="9">B25+D25+F25</f>
+        <v>1.5315749999999999</v>
       </c>
       <c r="H25" s="4">
-        <f>G25/C25</f>
-        <v>0.89707500000000007</v>
+        <f t="shared" ref="H25" si="10">G25/C25</f>
+        <v>1.5315749999999999</v>
       </c>
       <c r="I25">
         <v>1</v>
       </c>
       <c r="J25" s="4">
-        <f>H25*I25</f>
-        <v>0.89707500000000007</v>
-      </c>
-      <c r="L25" s="3"/>
+        <f t="shared" ref="J25" si="11">H25*I25</f>
+        <v>1.5315749999999999</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1">
-        <v>1.38</v>
+        <v>0.44</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>0</v>
       </c>
       <c r="E26" s="4">
-        <f>B30*0.1</f>
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" ref="F26" si="8">(B26+D26+E26)*0.1075</f>
-        <v>0.15157499999999999</v>
+        <f t="shared" ref="F26:F33" si="12">(B26+D26+E26)*0.1075</f>
+        <v>4.7300000000000002E-2</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" ref="G26" si="9">B26+D26+F26</f>
-        <v>1.5315749999999999</v>
+        <f t="shared" ref="G26:G33" si="13">B26+D26+F26</f>
+        <v>0.48730000000000001</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" ref="H26" si="10">G26/C26</f>
-        <v>1.5315749999999999</v>
+        <f t="shared" ref="H26:H33" si="14">G26/C26</f>
+        <v>0.48730000000000001</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
       <c r="J26" s="4">
-        <f t="shared" ref="J26" si="11">H26*I26</f>
-        <v>1.5315749999999999</v>
+        <f t="shared" ref="J26:J33" si="15">H26*I26</f>
+        <v>0.48730000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.4">
@@ -1374,40 +1378,40 @@
         <v>37</v>
       </c>
       <c r="B27" s="1">
-        <v>0.44</v>
+        <v>0.2</v>
       </c>
       <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
         <v>0</v>
       </c>
       <c r="E27" s="4">
         <v>0</v>
       </c>
       <c r="F27" s="4">
-        <f>(B27+D27+E27)*0.1075</f>
-        <v>4.7300000000000002E-2</v>
+        <f t="shared" si="12"/>
+        <v>2.1500000000000002E-2</v>
       </c>
       <c r="G27" s="4">
-        <f>B27+D27+F27</f>
-        <v>0.48730000000000001</v>
+        <f t="shared" si="13"/>
+        <v>0.2215</v>
       </c>
       <c r="H27" s="4">
-        <f>G27/C27</f>
-        <v>0.48730000000000001</v>
+        <f t="shared" si="14"/>
+        <v>0.11075</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J27" s="4">
-        <f>H27*I27</f>
-        <v>0.48730000000000001</v>
+        <f t="shared" si="15"/>
+        <v>0.2215</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B28" s="1">
         <v>0.2</v>
@@ -1415,29 +1419,29 @@
       <c r="C28">
         <v>2</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>0</v>
       </c>
       <c r="E28" s="4">
         <v>0</v>
       </c>
       <c r="F28" s="4">
-        <f>(B28+D28+E28)*0.1075</f>
+        <f t="shared" si="12"/>
         <v>2.1500000000000002E-2</v>
       </c>
       <c r="G28" s="4">
-        <f>B28+D28+F28</f>
+        <f t="shared" si="13"/>
         <v>0.2215</v>
       </c>
       <c r="H28" s="4">
-        <f>G28/C28</f>
+        <f t="shared" si="14"/>
         <v>0.11075</v>
       </c>
       <c r="I28">
         <v>2</v>
       </c>
       <c r="J28" s="4">
-        <f>H28*I28</f>
+        <f t="shared" si="15"/>
         <v>0.2215</v>
       </c>
     </row>
@@ -1446,267 +1450,291 @@
         <v>38</v>
       </c>
       <c r="B29" s="1">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1">
         <v>0</v>
       </c>
       <c r="E29" s="4">
         <v>0</v>
       </c>
       <c r="F29" s="4">
-        <f>(B29+D29+E29)*0.1075</f>
-        <v>2.1500000000000002E-2</v>
+        <f t="shared" si="12"/>
+        <v>3.2250000000000001E-2</v>
       </c>
       <c r="G29" s="4">
-        <f>B29+D29+F29</f>
-        <v>0.2215</v>
+        <f t="shared" si="13"/>
+        <v>0.33224999999999999</v>
       </c>
       <c r="H29" s="4">
-        <f>G29/C29</f>
+        <f t="shared" si="14"/>
         <v>0.11075</v>
       </c>
       <c r="I29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J29" s="4">
-        <f>H29*I29</f>
-        <v>0.2215</v>
+        <f t="shared" si="15"/>
+        <v>0.33224999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B30" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C30">
-        <v>3</v>
-      </c>
-      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" s="4">
         <v>0</v>
       </c>
       <c r="F30" s="4">
-        <f>(B30+D30+E30)*0.1075</f>
-        <v>3.2250000000000001E-2</v>
+        <f t="shared" si="12"/>
+        <v>1.0750000000000001E-2</v>
       </c>
       <c r="G30" s="4">
-        <f>B30+D30+F30</f>
-        <v>0.33224999999999999</v>
+        <f t="shared" si="13"/>
+        <v>0.11075</v>
       </c>
       <c r="H30" s="4">
-        <f>G30/C30</f>
+        <f t="shared" si="14"/>
         <v>0.11075</v>
       </c>
       <c r="I30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J30" s="4">
-        <f>H30*I30</f>
-        <v>0.33224999999999999</v>
+        <f t="shared" si="15"/>
+        <v>0.11075</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1">
-        <v>0.1</v>
+        <v>1.56</v>
       </c>
       <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
         <v>0</v>
       </c>
       <c r="E31" s="4">
-        <v>0</v>
+        <f>B31*0.1</f>
+        <v>0.15600000000000003</v>
       </c>
       <c r="F31" s="4">
-        <f>(B31+D31+E31)*0.1075</f>
-        <v>1.0750000000000001E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.18447000000000002</v>
       </c>
       <c r="G31" s="4">
-        <f>B31+D31+F31</f>
-        <v>0.11075</v>
+        <f t="shared" si="13"/>
+        <v>1.7444700000000002</v>
       </c>
       <c r="H31" s="4">
-        <f>G31/C31</f>
-        <v>0.11075</v>
+        <f t="shared" si="14"/>
+        <v>0.87223500000000009</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J31" s="4">
-        <f>H31*I31</f>
-        <v>0.11075</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>1.7444700000000002</v>
+      </c>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B32" s="1">
-        <v>1.56</v>
+        <v>0.13</v>
       </c>
       <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
         <v>0</v>
       </c>
       <c r="E32" s="4">
         <f>B32*0.1</f>
-        <v>0.15600000000000003</v>
+        <v>1.3000000000000001E-2</v>
       </c>
       <c r="F32" s="4">
-        <f>(B32+D32+E32)*0.1075</f>
-        <v>0.18447000000000002</v>
+        <f t="shared" si="12"/>
+        <v>1.5372500000000001E-2</v>
       </c>
       <c r="G32" s="4">
-        <f>B32+D32+F32</f>
-        <v>1.7444700000000002</v>
+        <f t="shared" si="13"/>
+        <v>0.14537250000000002</v>
       </c>
       <c r="H32" s="4">
-        <f>G32/C32</f>
-        <v>0.87223500000000009</v>
+        <f t="shared" si="14"/>
+        <v>0.14537250000000002</v>
       </c>
       <c r="I32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J32" s="4">
-        <f>H32*I32</f>
-        <v>1.7444700000000002</v>
+        <f t="shared" si="15"/>
+        <v>0.14537250000000002</v>
       </c>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B33" s="1">
-        <v>0.13</v>
+        <v>0.39</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>0</v>
       </c>
       <c r="E33" s="4">
-        <f>B33*0.1</f>
-        <v>1.3000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="F33" s="4">
-        <f>(B33+D33+E33)*0.1075</f>
-        <v>1.5372500000000001E-2</v>
+        <f t="shared" si="12"/>
+        <v>4.1925000000000004E-2</v>
       </c>
       <c r="G33" s="4">
-        <f>B33+D33+F33</f>
-        <v>0.14537250000000002</v>
+        <f t="shared" si="13"/>
+        <v>0.431925</v>
       </c>
       <c r="H33" s="4">
-        <f>G33/C33</f>
-        <v>0.14537250000000002</v>
+        <f t="shared" si="14"/>
+        <v>0.431925</v>
       </c>
       <c r="I33">
         <v>1</v>
       </c>
       <c r="J33" s="4">
-        <f>H33*I33</f>
-        <v>0.14537250000000002</v>
+        <f t="shared" si="15"/>
+        <v>0.431925</v>
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B34" s="1">
-        <v>0.3</v>
+        <v>1.56</v>
       </c>
       <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1">
         <v>0</v>
       </c>
       <c r="E34" s="4">
-        <f>B34*0.1</f>
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="F34" s="4">
         <f>(B34+D34+E34)*0.1075</f>
-        <v>3.5474999999999993E-2</v>
+        <v>0.16770000000000002</v>
       </c>
       <c r="G34" s="4">
         <f>B34+D34+F34</f>
-        <v>0.33547499999999997</v>
+        <v>1.7277</v>
       </c>
       <c r="H34" s="4">
         <f>G34/C34</f>
-        <v>0.33547499999999997</v>
+        <v>0.86385000000000001</v>
       </c>
       <c r="I34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J34" s="4">
         <f>H34*I34</f>
-        <v>0.33547499999999997</v>
-      </c>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A35" s="6" t="s">
-        <v>52</v>
+        <v>1.7277</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>58</v>
       </c>
       <c r="B35" s="1">
-        <f>SUM(B23:B34)</f>
-        <v>7.65</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="1">
-        <f>SUM(G23:G34)</f>
-        <v>8.5209650000000021</v>
-      </c>
-      <c r="H35" s="4"/>
+        <v>1.3</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0</v>
+      </c>
+      <c r="F35" s="4">
+        <f t="shared" ref="F35" si="16">(B35+D35+E35)*0.1075</f>
+        <v>0.13975000000000001</v>
+      </c>
+      <c r="G35" s="4">
+        <f t="shared" ref="G35" si="17">B35+D35+F35</f>
+        <v>1.4397500000000001</v>
+      </c>
+      <c r="H35" s="4">
+        <f t="shared" ref="H35" si="18">G35/C35</f>
+        <v>0.71987500000000004</v>
+      </c>
       <c r="I35">
-        <f>SUM(I23:I34)</f>
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="J35" s="4">
-        <f>SUM(J23:J34)</f>
-        <v>8.5209650000000021</v>
+        <f t="shared" ref="J35" si="19">H35*I35</f>
+        <v>1.4397500000000001</v>
       </c>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A36" s="6"/>
-      <c r="B36" s="1"/>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A36" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="1">
+        <f>SUM(B22:B35)</f>
+        <v>10.600000000000001</v>
+      </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="1"/>
+      <c r="G36" s="1">
+        <f>SUM(G22:G35)</f>
+        <v>11.784865000000002</v>
+      </c>
       <c r="H36" s="4"/>
-      <c r="J36" s="4"/>
+      <c r="I36">
+        <f>SUM(I22:I35)</f>
+        <v>22</v>
+      </c>
+      <c r="J36" s="4">
+        <f>SUM(J22:J35)</f>
+        <v>11.784865000000002</v>
+      </c>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A37" s="6" t="s">
-        <v>54</v>
-      </c>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A37" s="6"/>
       <c r="B37" s="1"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -1716,51 +1744,116 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B38" s="1"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="G38" s="1"/>
       <c r="H38" s="4"/>
       <c r="J38" s="4"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A39" s="6"/>
-      <c r="B39" s="1"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="J39" s="4"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A39" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="1">
+        <f>23.49*0.99</f>
+        <v>23.255099999999999</v>
+      </c>
+      <c r="C39">
+        <v>15</v>
+      </c>
+      <c r="D39" s="1">
+        <v>22.04</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0</v>
+      </c>
+      <c r="G39" s="4">
+        <f t="shared" ref="G39" si="20">B39+D39+F39</f>
+        <v>45.295099999999998</v>
+      </c>
+      <c r="H39" s="4">
+        <f t="shared" ref="H39" si="21">G39/C39</f>
+        <v>3.019673333333333</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39" s="4">
+        <f t="shared" ref="J39" si="22">H39*I39</f>
+        <v>3.019673333333333</v>
+      </c>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="4">
-        <f>B15+B20+B35+B38</f>
-        <v>150.6</v>
-      </c>
-      <c r="G40" s="4">
-        <f>G15+G20+G35+G38</f>
-        <v>166.83808999999999</v>
-      </c>
-      <c r="I40" s="5">
-        <f>I15+I20+I35+I38</f>
-        <v>40</v>
+      <c r="B40" s="1">
+        <f>SUM(B39:B39)</f>
+        <v>23.255099999999999</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="1">
+        <f>SUM(G39:G39)</f>
+        <v>45.295099999999998</v>
+      </c>
+      <c r="H40" s="4"/>
+      <c r="I40">
+        <f>SUM(I39:I39)</f>
+        <v>1</v>
       </c>
       <c r="J40" s="1">
-        <f>J15+J20+J35+J38</f>
-        <v>39.239950916666672</v>
+        <f>SUM(J39:J39)</f>
+        <v>3.019673333333333</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A41" s="6"/>
+      <c r="B41" s="1"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A42" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="4">
+        <f>B14+B19+B36+B40</f>
+        <v>170.81509999999997</v>
+      </c>
+      <c r="G42" s="4">
+        <f>G14+G19+G36+G40</f>
+        <v>208.76316499999999</v>
+      </c>
+      <c r="I42" s="5">
+        <f>I14+I19+I36+I40</f>
+        <v>43</v>
+      </c>
+      <c r="J42" s="1">
+        <f>J14+J19+J36+J40</f>
+        <v>45.25816725</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K5" r:id="rId1" xr:uid="{ACAC5234-DDA0-4969-B5FE-D166D7000F40}"/>
-    <hyperlink ref="K14" r:id="rId2" xr:uid="{71225EA3-939E-4F2C-8578-429F24215C0C}"/>
+    <hyperlink ref="K13" r:id="rId2" xr:uid="{71225EA3-939E-4F2C-8578-429F24215C0C}"/>
     <hyperlink ref="K9" r:id="rId3" xr:uid="{AED873F4-67F0-430A-8DE3-7AABA9CDF44E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Broke up bill of materials by supplier.  Added some missing items.
</commit_message>
<xml_diff>
--- a/parts/bill_of_materials.xlsx
+++ b/parts/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\laser_tunnel\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891227A6-8872-44E5-9CBE-85B5E76A6E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22314A68-3FF2-4A0A-9529-3AFAE928971A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3189" yWindow="1243" windowWidth="22268" windowHeight="14974" xr2:uid="{C7A15FB5-B248-4CA2-8E4B-B85C1BCDD779}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Laser Tunnel</t>
   </si>
@@ -212,6 +212,15 @@
   </si>
   <si>
     <t>12-pin header socket for Pro Mini</t>
+  </si>
+  <si>
+    <t>shunt jumper</t>
+  </si>
+  <si>
+    <t>shipping???</t>
+  </si>
+  <si>
+    <t>See Laser-Tunnel list on DigiKey</t>
   </si>
 </sst>
 </file>
@@ -281,7 +290,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -289,10 +298,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -609,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A265784A-A2E2-4F2C-B0D4-276F819350E1}">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -668,7 +681,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1039,24 +1052,24 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="7">
         <f>SUM(B4:B13)</f>
         <v>136.95999999999998</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="1">
+      <c r="G14" s="7">
         <f>SUM(G4:G13)</f>
         <v>151.6832</v>
       </c>
       <c r="H14" s="4"/>
-      <c r="I14" s="7">
+      <c r="I14" s="12">
         <f>SUM(I4:I13)</f>
         <v>16</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="7">
         <f>SUM(J4:J13)</f>
         <v>30.453628916666666</v>
       </c>
@@ -1071,7 +1084,7 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="1"/>
@@ -1148,24 +1161,24 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="7">
         <f>SUM(B17:B18)</f>
         <v>0</v>
       </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="1">
+      <c r="G19" s="7">
         <f>SUM(G17:G18)</f>
         <v>0</v>
       </c>
       <c r="H19" s="4"/>
-      <c r="I19" s="7">
+      <c r="I19" s="12">
         <f>SUM(I17:I18)</f>
         <v>4</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="7">
         <f>SUM(J17:J18)</f>
         <v>0</v>
       </c>
@@ -1179,7 +1192,7 @@
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="1"/>
@@ -1188,124 +1201,125 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="J21" s="4"/>
+      <c r="K21" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>45</v>
+      <c r="A22" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="B22" s="1">
-        <v>0.53</v>
+        <v>0</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="1">
-        <v>0</v>
+      <c r="D22">
+        <v>4.99</v>
       </c>
       <c r="E22" s="4">
-        <f>B22*0.1</f>
-        <v>5.3000000000000005E-2</v>
+        <v>0</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" ref="F22" si="4">(B22+D22+E22)*0.1075</f>
-        <v>6.2672500000000006E-2</v>
+        <v>0</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" ref="G22" si="5">B22+D22+F22</f>
-        <v>0.59267250000000005</v>
+        <f t="shared" ref="G22:G23" si="4">B22+D22+F22</f>
+        <v>4.99</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" ref="H22" si="6">G22/C22</f>
-        <v>0.59267250000000005</v>
+        <f t="shared" ref="H22" si="5">G22/C22</f>
+        <v>4.99</v>
       </c>
       <c r="I22">
         <v>1</v>
       </c>
       <c r="J22" s="4">
-        <f t="shared" ref="J22" si="7">H22*I22</f>
-        <v>0.59267250000000005</v>
+        <f t="shared" ref="J22" si="6">H22*I22</f>
+        <v>4.99</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1">
-        <v>1.7</v>
+        <v>0.53</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
       <c r="E23" s="4">
         <f>B23*0.1</f>
-        <v>0.17</v>
+        <v>5.3000000000000005E-2</v>
       </c>
       <c r="F23" s="4">
-        <f>(B23+D23+E23)*0.1075</f>
-        <v>0.20102499999999998</v>
+        <f t="shared" ref="F23" si="7">(B23+D23+E23)*0.1075</f>
+        <v>6.2672500000000006E-2</v>
       </c>
       <c r="G23" s="4">
-        <f>B23+D23+F23</f>
-        <v>1.901025</v>
+        <f t="shared" si="4"/>
+        <v>0.59267250000000005</v>
       </c>
       <c r="H23" s="4">
-        <f>G23/C23</f>
-        <v>0.95051249999999998</v>
+        <f t="shared" ref="H23" si="8">G23/C23</f>
+        <v>0.59267250000000005</v>
       </c>
       <c r="I23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J23" s="4">
-        <f>H23*I23</f>
-        <v>1.901025</v>
+        <f t="shared" ref="J23" si="9">H23*I23</f>
+        <v>0.59267250000000005</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1">
-        <v>0.81</v>
+        <v>1.7</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" s="4">
-        <v>0</v>
+        <f>B24*0.1</f>
+        <v>0.17</v>
       </c>
       <c r="F24" s="4">
         <f>(B24+D24+E24)*0.1075</f>
-        <v>8.7075E-2</v>
+        <v>0.20102499999999998</v>
       </c>
       <c r="G24" s="4">
         <f>B24+D24+F24</f>
-        <v>0.89707500000000007</v>
+        <v>1.901025</v>
       </c>
       <c r="H24" s="4">
         <f>G24/C24</f>
-        <v>0.89707500000000007</v>
+        <v>0.95051249999999998</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J24" s="4">
         <f>H24*I24</f>
-        <v>0.89707500000000007</v>
-      </c>
-      <c r="L24" s="3"/>
+        <v>1.901025</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1">
-        <v>1.38</v>
+        <v>0.81</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1314,35 +1328,35 @@
         <v>0</v>
       </c>
       <c r="E25" s="4">
-        <f>B29*0.1</f>
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" ref="F25" si="8">(B25+D25+E25)*0.1075</f>
-        <v>0.15157499999999999</v>
+        <f>(B25+D25+E25)*0.1075</f>
+        <v>8.7075E-2</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" ref="G25" si="9">B25+D25+F25</f>
-        <v>1.5315749999999999</v>
+        <f>B25+D25+F25</f>
+        <v>0.89707500000000007</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" ref="H25" si="10">G25/C25</f>
-        <v>1.5315749999999999</v>
+        <f>G25/C25</f>
+        <v>0.89707500000000007</v>
       </c>
       <c r="I25">
         <v>1</v>
       </c>
       <c r="J25" s="4">
-        <f t="shared" ref="J25" si="11">H25*I25</f>
-        <v>1.5315749999999999</v>
-      </c>
+        <f>H25*I25</f>
+        <v>0.89707500000000007</v>
+      </c>
+      <c r="L25" s="3"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B26" s="1">
-        <v>0.44</v>
+        <v>1.38</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1351,330 +1365,331 @@
         <v>0</v>
       </c>
       <c r="E26" s="4">
-        <v>0</v>
+        <f>B30*0.1</f>
+        <v>0.03</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" ref="F26:F33" si="12">(B26+D26+E26)*0.1075</f>
-        <v>4.7300000000000002E-2</v>
+        <f t="shared" ref="F26" si="10">(B26+D26+E26)*0.1075</f>
+        <v>0.15157499999999999</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" ref="G26:G33" si="13">B26+D26+F26</f>
-        <v>0.48730000000000001</v>
+        <f t="shared" ref="G26" si="11">B26+D26+F26</f>
+        <v>1.5315749999999999</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" ref="H26:H33" si="14">G26/C26</f>
-        <v>0.48730000000000001</v>
+        <f t="shared" ref="H26" si="12">G26/C26</f>
+        <v>1.5315749999999999</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
       <c r="J26" s="4">
-        <f t="shared" ref="J26:J33" si="15">H26*I26</f>
-        <v>0.48730000000000001</v>
+        <f t="shared" ref="J26" si="13">H26*I26</f>
+        <v>1.5315749999999999</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" ref="F27:F34" si="14">(B27+D27+E27)*0.1075</f>
+        <v>4.7300000000000002E-2</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" ref="G27:G34" si="15">B27+D27+F27</f>
+        <v>0.48730000000000001</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" ref="H27:H34" si="16">G27/C27</f>
+        <v>0.48730000000000001</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" ref="J27:J34" si="17">H27*I27</f>
+        <v>0.48730000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B28" s="1">
         <v>0.2</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>2</v>
       </c>
-      <c r="D27" s="1">
-        <v>0</v>
-      </c>
-      <c r="E27" s="4">
-        <v>0</v>
-      </c>
-      <c r="F27" s="4">
-        <f t="shared" si="12"/>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="14"/>
         <v>2.1500000000000002E-2</v>
       </c>
-      <c r="G27" s="4">
-        <f t="shared" si="13"/>
-        <v>0.2215</v>
-      </c>
-      <c r="H27" s="4">
-        <f t="shared" si="14"/>
-        <v>0.11075</v>
-      </c>
-      <c r="I27">
-        <v>2</v>
-      </c>
-      <c r="J27" s="4">
+      <c r="G28" s="4">
         <f t="shared" si="15"/>
         <v>0.2215</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28" s="1">
-        <v>0</v>
-      </c>
-      <c r="E28" s="4">
-        <v>0</v>
-      </c>
-      <c r="F28" s="4">
-        <f t="shared" si="12"/>
-        <v>2.1500000000000002E-2</v>
-      </c>
-      <c r="G28" s="4">
-        <f t="shared" si="13"/>
-        <v>0.2215</v>
-      </c>
       <c r="H28" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.11075</v>
       </c>
       <c r="I28">
         <v>2</v>
       </c>
       <c r="J28" s="4">
+        <f t="shared" si="17"/>
+        <v>0.2215</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" si="14"/>
+        <v>2.1500000000000002E-2</v>
+      </c>
+      <c r="G29" s="4">
         <f t="shared" si="15"/>
         <v>0.2215</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
+      <c r="H29" s="4">
+        <f t="shared" si="16"/>
+        <v>0.11075</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29" s="4">
+        <f t="shared" si="17"/>
+        <v>0.2215</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B30" s="1">
         <v>0.3</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>3</v>
       </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-      <c r="E29" s="4">
-        <v>0</v>
-      </c>
-      <c r="F29" s="4">
-        <f t="shared" si="12"/>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <f t="shared" si="14"/>
         <v>3.2250000000000001E-2</v>
       </c>
-      <c r="G29" s="4">
-        <f t="shared" si="13"/>
-        <v>0.33224999999999999</v>
-      </c>
-      <c r="H29" s="4">
-        <f t="shared" si="14"/>
-        <v>0.11075</v>
-      </c>
-      <c r="I29">
-        <v>3</v>
-      </c>
-      <c r="J29" s="4">
+      <c r="G30" s="4">
         <f t="shared" si="15"/>
         <v>0.33224999999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
+      <c r="H30" s="4">
+        <f t="shared" si="16"/>
+        <v>0.11075</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" si="17"/>
+        <v>0.33224999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B31" s="1">
         <v>0.1</v>
       </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-      <c r="E30" s="4">
-        <v>0</v>
-      </c>
-      <c r="F30" s="4">
-        <f t="shared" si="12"/>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4">
+        <f t="shared" si="14"/>
         <v>1.0750000000000001E-2</v>
       </c>
-      <c r="G30" s="4">
-        <f t="shared" si="13"/>
-        <v>0.11075</v>
-      </c>
-      <c r="H30" s="4">
-        <f t="shared" si="14"/>
-        <v>0.11075</v>
-      </c>
-      <c r="I30">
-        <v>1</v>
-      </c>
-      <c r="J30" s="4">
+      <c r="G31" s="4">
         <f t="shared" si="15"/>
         <v>0.11075</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
+      <c r="H31" s="4">
+        <f t="shared" si="16"/>
+        <v>0.11075</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31" s="4">
+        <f t="shared" si="17"/>
+        <v>0.11075</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B32" s="1">
         <v>1.56</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>2</v>
       </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31" s="4">
-        <f>B31*0.1</f>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4">
+        <f>B32*0.1</f>
         <v>0.15600000000000003</v>
       </c>
-      <c r="F31" s="4">
-        <f t="shared" si="12"/>
+      <c r="F32" s="4">
+        <f t="shared" si="14"/>
         <v>0.18447000000000002</v>
       </c>
-      <c r="G31" s="4">
-        <f t="shared" si="13"/>
-        <v>1.7444700000000002</v>
-      </c>
-      <c r="H31" s="4">
-        <f t="shared" si="14"/>
-        <v>0.87223500000000009</v>
-      </c>
-      <c r="I31">
-        <v>2</v>
-      </c>
-      <c r="J31" s="4">
+      <c r="G32" s="4">
         <f t="shared" si="15"/>
         <v>1.7444700000000002</v>
       </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
+      <c r="H32" s="4">
+        <f t="shared" si="16"/>
+        <v>0.87223500000000009</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32" s="4">
+        <f t="shared" si="17"/>
+        <v>1.7444700000000002</v>
+      </c>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B33" s="1">
         <v>0.13</v>
       </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="E32" s="4">
-        <f>B32*0.1</f>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4">
+        <f>B33*0.1</f>
         <v>1.3000000000000001E-2</v>
       </c>
-      <c r="F32" s="4">
-        <f t="shared" si="12"/>
+      <c r="F33" s="4">
+        <f t="shared" si="14"/>
         <v>1.5372500000000001E-2</v>
       </c>
-      <c r="G32" s="4">
-        <f t="shared" si="13"/>
-        <v>0.14537250000000002</v>
-      </c>
-      <c r="H32" s="4">
-        <f t="shared" si="14"/>
-        <v>0.14537250000000002</v>
-      </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-      <c r="J32" s="4">
+      <c r="G33" s="4">
         <f t="shared" si="15"/>
         <v>0.14537250000000002</v>
       </c>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
+      <c r="H33" s="4">
+        <f t="shared" si="16"/>
+        <v>0.14537250000000002</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33" s="4">
+        <f t="shared" si="17"/>
+        <v>0.14537250000000002</v>
+      </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B34" s="1">
         <v>0.39</v>
       </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-      <c r="E33" s="4">
-        <v>0</v>
-      </c>
-      <c r="F33" s="4">
-        <f t="shared" si="12"/>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4">
+        <f t="shared" si="14"/>
         <v>4.1925000000000004E-2</v>
       </c>
-      <c r="G33" s="4">
-        <f t="shared" si="13"/>
-        <v>0.431925</v>
-      </c>
-      <c r="H33" s="4">
-        <f t="shared" si="14"/>
-        <v>0.431925</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33" s="4">
+      <c r="G34" s="4">
         <f t="shared" si="15"/>
         <v>0.431925</v>
       </c>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="1">
-        <v>1.56</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34" s="1">
-        <v>0</v>
-      </c>
-      <c r="E34" s="4">
-        <v>0</v>
-      </c>
-      <c r="F34" s="4">
-        <f>(B34+D34+E34)*0.1075</f>
-        <v>0.16770000000000002</v>
-      </c>
-      <c r="G34" s="4">
-        <f>B34+D34+F34</f>
-        <v>1.7277</v>
-      </c>
       <c r="H34" s="4">
-        <f>G34/C34</f>
-        <v>0.86385000000000001</v>
+        <f t="shared" si="16"/>
+        <v>0.431925</v>
       </c>
       <c r="I34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J34" s="4">
-        <f>H34*I34</f>
-        <v>1.7277</v>
-      </c>
+        <f t="shared" si="17"/>
+        <v>0.431925</v>
+      </c>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B35" s="1">
-        <v>1.3</v>
+        <v>1.56</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -1686,168 +1701,242 @@
         <v>0</v>
       </c>
       <c r="F35" s="4">
-        <f t="shared" ref="F35" si="16">(B35+D35+E35)*0.1075</f>
-        <v>0.13975000000000001</v>
+        <f>(B35+D35+E35)*0.1075</f>
+        <v>0.16770000000000002</v>
       </c>
       <c r="G35" s="4">
-        <f t="shared" ref="G35" si="17">B35+D35+F35</f>
-        <v>1.4397500000000001</v>
+        <f>B35+D35+F35</f>
+        <v>1.7277</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" ref="H35" si="18">G35/C35</f>
-        <v>0.71987500000000004</v>
+        <f>G35/C35</f>
+        <v>0.86385000000000001</v>
       </c>
       <c r="I35">
         <v>2</v>
       </c>
       <c r="J35" s="4">
-        <f t="shared" ref="J35" si="19">H35*I35</f>
+        <f>H35*I35</f>
+        <v>1.7277</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="4">
+        <v>0</v>
+      </c>
+      <c r="F36" s="4">
+        <f t="shared" ref="F36" si="18">(B36+D36+E36)*0.1075</f>
+        <v>0.13975000000000001</v>
+      </c>
+      <c r="G36" s="4">
+        <f t="shared" ref="G36" si="19">B36+D36+F36</f>
         <v>1.4397500000000001</v>
       </c>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A36" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="1">
-        <f>SUM(B22:B35)</f>
-        <v>10.600000000000001</v>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="1">
-        <f>SUM(G22:G35)</f>
-        <v>11.784865000000002</v>
-      </c>
-      <c r="H36" s="4"/>
+      <c r="H36" s="4">
+        <f t="shared" ref="H36" si="20">G36/C36</f>
+        <v>0.71987500000000004</v>
+      </c>
       <c r="I36">
-        <f>SUM(I22:I35)</f>
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="J36" s="4">
-        <f>SUM(J22:J35)</f>
-        <v>11.784865000000002</v>
+        <f t="shared" ref="J36" si="21">H36*I36</f>
+        <v>1.4397500000000001</v>
       </c>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A37" s="6"/>
-      <c r="B37" s="1"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="4"/>
-      <c r="J37" s="4"/>
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4">
+        <f t="shared" ref="F37" si="22">(B37+D37+E37)*0.1075</f>
+        <v>1.0750000000000001E-2</v>
+      </c>
+      <c r="G37" s="4">
+        <f t="shared" ref="G37" si="23">B37+D37+F37</f>
+        <v>0.11075</v>
+      </c>
+      <c r="H37" s="4">
+        <f t="shared" ref="H37" si="24">G37/C37</f>
+        <v>0.11075</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37" s="4">
+        <f t="shared" ref="J37" si="25">H37*I37</f>
+        <v>0.11075</v>
+      </c>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A38" s="6" t="s">
+    <row r="38" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="7">
+        <f>SUM(B22:B37)</f>
+        <v>10.700000000000001</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="7">
+        <f>SUM(G22:G37)</f>
+        <v>16.885614999999998</v>
+      </c>
+      <c r="H38" s="8"/>
+      <c r="I38" s="5">
+        <f>SUM(I22:I37)</f>
+        <v>24</v>
+      </c>
+      <c r="J38" s="10">
+        <f>SUM(J22:J37)</f>
+        <v>16.885614999999998</v>
+      </c>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A39" s="5"/>
+      <c r="B39" s="1"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A40" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A39" s="8" t="s">
+      <c r="B40" s="1"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A41" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B41" s="1">
         <f>23.49*0.99</f>
         <v>23.255099999999999</v>
       </c>
-      <c r="C39">
+      <c r="C41">
         <v>15</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D41" s="1">
         <v>22.04</v>
       </c>
-      <c r="E39" s="4">
-        <v>0</v>
-      </c>
-      <c r="F39" s="4">
-        <v>0</v>
-      </c>
-      <c r="G39" s="4">
-        <f t="shared" ref="G39" si="20">B39+D39+F39</f>
+      <c r="E41" s="4">
+        <v>0</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0</v>
+      </c>
+      <c r="G41" s="4">
+        <f t="shared" ref="G41" si="26">B41+D41+F41</f>
         <v>45.295099999999998</v>
       </c>
-      <c r="H39" s="4">
-        <f t="shared" ref="H39" si="21">G39/C39</f>
+      <c r="H41" s="4">
+        <f t="shared" ref="H41" si="27">G41/C41</f>
         <v>3.019673333333333</v>
       </c>
-      <c r="I39">
-        <v>1</v>
-      </c>
-      <c r="J39" s="4">
-        <f t="shared" ref="J39" si="22">H39*I39</f>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41" s="4">
+        <f t="shared" ref="J41" si="28">H41*I41</f>
         <v>3.019673333333333</v>
       </c>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="1"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A40" s="6" t="s">
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="1"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A42" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="1">
-        <f>SUM(B39:B39)</f>
+      <c r="B42" s="7">
+        <f>SUM(B41:B41)</f>
         <v>23.255099999999999</v>
       </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="1">
-        <f>SUM(G39:G39)</f>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="7">
+        <f>SUM(G41:G41)</f>
         <v>45.295099999999998</v>
       </c>
-      <c r="H40" s="4"/>
-      <c r="I40">
-        <f>SUM(I39:I39)</f>
-        <v>1</v>
-      </c>
-      <c r="J40" s="1">
-        <f>SUM(J39:J39)</f>
+      <c r="H42" s="4"/>
+      <c r="I42" s="5">
+        <f>SUM(I41:I41)</f>
+        <v>1</v>
+      </c>
+      <c r="J42" s="7">
+        <f>SUM(J41:J41)</f>
         <v>3.019673333333333</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A41" s="6"/>
-      <c r="B41" s="1"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="J41" s="4"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A42" s="6" t="s">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A43" s="5"/>
+      <c r="B43" s="1"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="J43" s="4"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A44" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="4">
-        <f>B14+B19+B36+B40</f>
-        <v>170.81509999999997</v>
-      </c>
-      <c r="G42" s="4">
-        <f>G14+G19+G36+G40</f>
-        <v>208.76316499999999</v>
-      </c>
-      <c r="I42" s="5">
-        <f>I14+I19+I36+I40</f>
-        <v>43</v>
-      </c>
-      <c r="J42" s="1">
-        <f>J14+J19+J36+J40</f>
-        <v>45.25816725</v>
+      <c r="B44" s="10">
+        <f>B14+B19+B38+B42</f>
+        <v>170.91509999999997</v>
+      </c>
+      <c r="G44" s="10">
+        <f>G14+G19+G38+G42</f>
+        <v>213.86391499999999</v>
+      </c>
+      <c r="I44" s="11">
+        <f>I14+I19+I38+I42</f>
+        <v>45</v>
+      </c>
+      <c r="J44" s="7">
+        <f>J14+J19+J38+J42</f>
+        <v>50.35891724999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated bill of materials spreadsheet.
</commit_message>
<xml_diff>
--- a/parts/bill_of_materials.xlsx
+++ b/parts/bill_of_materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\laser_tunnel\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22314A68-3FF2-4A0A-9529-3AFAE928971A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382CD39D-E3FF-4507-8F06-9F473F80D266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3189" yWindow="1243" windowWidth="22268" windowHeight="14974" xr2:uid="{C7A15FB5-B248-4CA2-8E4B-B85C1BCDD779}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C7A15FB5-B248-4CA2-8E4B-B85C1BCDD779}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Laser Tunnel</t>
   </si>
@@ -142,9 +142,6 @@
     <t>2N3904 transistor</t>
   </si>
   <si>
-    <t>330 Ohm resistor</t>
-  </si>
-  <si>
     <t>1 kOhm resistor</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>4-pin fan header</t>
   </si>
   <si>
-    <t>180 Ohm resistor</t>
-  </si>
-  <si>
     <t>push button switch</t>
   </si>
   <si>
@@ -202,9 +196,6 @@
     <t>https://www.amazon.com/dp/B07BDD8BF3</t>
   </si>
   <si>
-    <t>LED</t>
-  </si>
-  <si>
     <t>PCB fabrication</t>
   </si>
   <si>
@@ -221,6 +212,42 @@
   </si>
   <si>
     <t>See Laser-Tunnel list on DigiKey</t>
+  </si>
+  <si>
+    <t>Kits Needed:</t>
+  </si>
+  <si>
+    <t>Extended Qty</t>
+  </si>
+  <si>
+    <t>On Hand</t>
+  </si>
+  <si>
+    <t>Qty Needed</t>
+  </si>
+  <si>
+    <t>Purchase Units</t>
+  </si>
+  <si>
+    <t>Purchase Cost</t>
+  </si>
+  <si>
+    <t>10 Ohm resistor</t>
+  </si>
+  <si>
+    <t>1.2kOhm resistor</t>
+  </si>
+  <si>
+    <t>2.2kOhm resistor</t>
+  </si>
+  <si>
+    <t>5-pin header socket for optional outputs</t>
+  </si>
+  <si>
+    <t>Schottky diode</t>
+  </si>
+  <si>
+    <t>0.01uF capacitor</t>
   </si>
 </sst>
 </file>
@@ -622,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A265784A-A2E2-4F2C-B0D4-276F819350E1}">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -638,14 +665,21 @@
     <col min="7" max="7" width="9.23046875" customWidth="1"/>
     <col min="9" max="9" width="8.3046875" customWidth="1"/>
     <col min="10" max="10" width="10.53515625" customWidth="1"/>
+    <col min="17" max="17" width="11.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -679,13 +713,28 @@
       <c r="K2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -723,8 +772,27 @@
       <c r="L4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M4">
+        <f>$C$1*I4</f>
+        <v>20</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>M4-N4</f>
+        <v>20</v>
+      </c>
+      <c r="P4">
+        <f>_xlfn.CEILING.MATH(O4/C4)</f>
+        <v>20</v>
+      </c>
+      <c r="Q4" s="4">
+        <f>P4*G4</f>
+        <v>220.39249999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -759,8 +827,27 @@
       <c r="K5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M5">
+        <f t="shared" ref="M5:M13" si="4">$C$1*I5</f>
+        <v>20</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5:O13" si="5">M5-N5</f>
+        <v>20</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P13" si="6">_xlfn.CEILING.MATH(O5/C5)</f>
+        <v>2</v>
+      </c>
+      <c r="Q5" s="4">
+        <f t="shared" ref="Q5:Q13" si="7">P5*G5</f>
+        <v>13.267850000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -795,8 +882,27 @@
       <c r="K6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="Q6" s="4">
+        <f t="shared" si="7"/>
+        <v>17.697849999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -831,8 +937,27 @@
       <c r="K7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q7" s="4">
+        <f t="shared" si="7"/>
+        <v>6.6339250000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -867,10 +992,29 @@
       <c r="K8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="Q8" s="4">
+        <f t="shared" si="7"/>
+        <v>147.21997499999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1">
         <v>12.99</v>
@@ -901,10 +1045,29 @@
         <v>2.8772850000000001</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+        <v>53</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="Q9" s="4">
+        <f t="shared" si="7"/>
+        <v>57.545700000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -939,8 +1102,27 @@
       <c r="K10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M10">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q10" s="4">
+        <f t="shared" si="7"/>
+        <v>16.047675000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -975,8 +1157,27 @@
       <c r="K11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M11">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q11" s="4">
+        <f t="shared" si="7"/>
+        <v>8.2951750000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1011,8 +1212,27 @@
       <c r="K12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M12">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="7"/>
+        <v>84.125699999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1050,10 +1270,29 @@
       <c r="L13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="7"/>
+        <v>75.509350000000012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" s="7">
         <f>SUM(B4:B13)</f>
@@ -1074,8 +1313,12 @@
         <v>30.453628916666666</v>
       </c>
       <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="Q14" s="7">
+        <f>SUM(Q4:Q13)</f>
+        <v>646.73569999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -1083,9 +1326,9 @@
       <c r="H15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1"/>
       <c r="E16" s="4"/>
@@ -1094,9 +1337,9 @@
       <c r="H16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -1127,9 +1370,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -1160,9 +1403,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" s="7">
         <f>SUM(B17:B18)</f>
@@ -1183,7 +1426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1191,9 +1434,9 @@
       <c r="H20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1"/>
       <c r="E21" s="4"/>
@@ -1202,12 +1445,12 @@
       <c r="H21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A22" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -1225,24 +1468,43 @@
         <v>0</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" ref="G22:G23" si="4">B22+D22+F22</f>
+        <f t="shared" ref="G22:G23" si="8">B22+D22+F22</f>
         <v>4.99</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" ref="H22" si="5">G22/C22</f>
+        <f t="shared" ref="H22" si="9">G22/C22</f>
         <v>4.99</v>
       </c>
       <c r="I22">
         <v>1</v>
       </c>
       <c r="J22" s="4">
-        <f t="shared" ref="J22" si="6">H22*I22</f>
+        <f t="shared" ref="J22" si="10">H22*I22</f>
         <v>4.99</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M22">
+        <f t="shared" ref="M22:M35" si="11">$C$1*I22</f>
+        <v>20</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f t="shared" ref="O22:O35" si="12">M22-N22</f>
+        <v>20</v>
+      </c>
+      <c r="P22">
+        <f t="shared" ref="P22:P35" si="13">_xlfn.CEILING.MATH(O22/C22)</f>
+        <v>20</v>
+      </c>
+      <c r="Q22" s="4">
+        <f t="shared" ref="Q22:Q35" si="14">P22*G22</f>
+        <v>99.800000000000011</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1">
         <v>0.53</v>
@@ -1258,26 +1520,45 @@
         <v>5.3000000000000005E-2</v>
       </c>
       <c r="F23" s="4">
-        <f t="shared" ref="F23" si="7">(B23+D23+E23)*0.1075</f>
+        <f t="shared" ref="F23" si="15">(B23+D23+E23)*0.1075</f>
         <v>6.2672500000000006E-2</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.59267250000000005</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" ref="H23" si="8">G23/C23</f>
+        <f t="shared" ref="H23" si="16">G23/C23</f>
         <v>0.59267250000000005</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23" s="4">
-        <f t="shared" ref="J23" si="9">H23*I23</f>
+        <f t="shared" ref="J23" si="17">H23*I23</f>
         <v>0.59267250000000005</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M23">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="Q23" s="4">
+        <f t="shared" si="14"/>
+        <v>11.85345</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1313,8 +1594,27 @@
         <f>H24*I24</f>
         <v>1.901025</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M24">
+        <f t="shared" si="11"/>
+        <v>40</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="12"/>
+        <v>40</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="Q24" s="4">
+        <f t="shared" si="14"/>
+        <v>38.020499999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1350,10 +1650,29 @@
         <v>0.89707500000000007</v>
       </c>
       <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M25">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="Q25" s="4">
+        <f t="shared" si="14"/>
+        <v>17.941500000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1">
         <v>1.38</v>
@@ -1365,30 +1684,49 @@
         <v>0</v>
       </c>
       <c r="E26" s="4">
-        <f>B30*0.1</f>
+        <f>B29*0.1</f>
         <v>0.03</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" ref="F26" si="10">(B26+D26+E26)*0.1075</f>
+        <f t="shared" ref="F26" si="18">(B26+D26+E26)*0.1075</f>
         <v>0.15157499999999999</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" ref="G26" si="11">B26+D26+F26</f>
+        <f t="shared" ref="G26" si="19">B26+D26+F26</f>
         <v>1.5315749999999999</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" ref="H26" si="12">G26/C26</f>
+        <f t="shared" ref="H26" si="20">G26/C26</f>
         <v>1.5315749999999999</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
       <c r="J26" s="4">
-        <f t="shared" ref="J26" si="13">H26*I26</f>
+        <f t="shared" ref="J26" si="21">H26*I26</f>
         <v>1.5315749999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M26">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="Q26" s="4">
+        <f t="shared" si="14"/>
+        <v>30.631499999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1405,70 +1743,108 @@
         <v>0</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" ref="F27:F34" si="14">(B27+D27+E27)*0.1075</f>
+        <f t="shared" ref="F27:F30" si="22">(B27+D27+E27)*0.1075</f>
         <v>4.7300000000000002E-2</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" ref="G27:G34" si="15">B27+D27+F27</f>
+        <f t="shared" ref="G27:G30" si="23">B27+D27+F27</f>
         <v>0.48730000000000001</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" ref="H27:H34" si="16">G27/C27</f>
+        <f t="shared" ref="H27:H30" si="24">G27/C27</f>
         <v>0.48730000000000001</v>
       </c>
       <c r="I27">
         <v>1</v>
       </c>
       <c r="J27" s="4">
-        <f t="shared" ref="J27:J34" si="17">H27*I27</f>
+        <f t="shared" ref="J27:J30" si="25">H27*I27</f>
         <v>0.48730000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M27">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="Q27" s="4">
+        <f t="shared" si="14"/>
+        <v>9.7460000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="22"/>
+        <v>1.0750000000000001E-2</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" si="23"/>
+        <v>0.11075</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="24"/>
+        <v>0.11075</v>
+      </c>
+      <c r="I28">
+        <v>9</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="25"/>
+        <v>0.99675000000000002</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="11"/>
+        <v>180</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="12"/>
+        <v>180</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="13"/>
+        <v>180</v>
+      </c>
+      <c r="Q28" s="4">
+        <f t="shared" si="14"/>
+        <v>19.934999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28" s="1">
-        <v>0</v>
-      </c>
-      <c r="E28" s="4">
-        <v>0</v>
-      </c>
-      <c r="F28" s="4">
-        <f t="shared" si="14"/>
-        <v>2.1500000000000002E-2</v>
-      </c>
-      <c r="G28" s="4">
-        <f t="shared" si="15"/>
-        <v>0.2215</v>
-      </c>
-      <c r="H28" s="4">
-        <f t="shared" si="16"/>
-        <v>0.11075</v>
-      </c>
-      <c r="I28">
-        <v>2</v>
-      </c>
-      <c r="J28" s="4">
-        <f t="shared" si="17"/>
-        <v>0.2215</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
       <c r="B29" s="1">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
@@ -1477,34 +1853,53 @@
         <v>0</v>
       </c>
       <c r="F29" s="4">
-        <f t="shared" si="14"/>
-        <v>2.1500000000000002E-2</v>
+        <f t="shared" si="22"/>
+        <v>3.2250000000000001E-2</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" si="15"/>
-        <v>0.2215</v>
+        <f t="shared" si="23"/>
+        <v>0.33224999999999999</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>0.11075</v>
       </c>
       <c r="I29">
         <v>2</v>
       </c>
       <c r="J29" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>0.2215</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M29">
+        <f t="shared" si="11"/>
+        <v>40</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="12"/>
+        <v>40</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="Q29" s="4">
+        <f t="shared" si="14"/>
+        <v>4.6514999999999995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B30" s="1">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
@@ -1513,28 +1908,47 @@
         <v>0</v>
       </c>
       <c r="F30" s="4">
+        <f t="shared" si="22"/>
+        <v>5.3749999999999999E-2</v>
+      </c>
+      <c r="G30" s="4">
+        <f t="shared" si="23"/>
+        <v>0.55374999999999996</v>
+      </c>
+      <c r="H30" s="4">
+        <f t="shared" si="24"/>
+        <v>0.11074999999999999</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" si="25"/>
+        <v>0.55374999999999996</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="11"/>
+        <v>100</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="12"/>
+        <v>100</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="Q30" s="4">
         <f t="shared" si="14"/>
-        <v>3.2250000000000001E-2</v>
-      </c>
-      <c r="G30" s="4">
-        <f t="shared" si="15"/>
-        <v>0.33224999999999999</v>
-      </c>
-      <c r="H30" s="4">
-        <f t="shared" si="16"/>
-        <v>0.11075</v>
-      </c>
-      <c r="I30">
-        <v>3</v>
-      </c>
-      <c r="J30" s="4">
-        <f t="shared" si="17"/>
-        <v>0.33224999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
+        <v>11.074999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B31" s="1">
         <v>0.1</v>
@@ -1549,67 +1963,102 @@
         <v>0</v>
       </c>
       <c r="F31" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="F31" si="26">(B31+D31+E31)*0.1075</f>
         <v>1.0750000000000001E-2</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="G31" si="27">B31+D31+F31</f>
         <v>0.11075</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="H31" si="28">G31/C31</f>
         <v>0.11075</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J31" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="J31" si="29">H31*I31</f>
+        <v>0.55374999999999996</v>
+      </c>
+      <c r="M31">
+        <f t="shared" ref="M31" si="30">$C$1*I31</f>
+        <v>100</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" ref="O31" si="31">M31-N31</f>
+        <v>100</v>
+      </c>
+      <c r="P31">
+        <f t="shared" ref="P31" si="32">_xlfn.CEILING.MATH(O31/C31)</f>
+        <v>100</v>
+      </c>
+      <c r="Q31" s="4">
+        <f t="shared" ref="Q31" si="33">P31*G31</f>
+        <v>11.074999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" ref="F32" si="34">(B32+D32+E32)*0.1075</f>
+        <v>1.0750000000000001E-2</v>
+      </c>
+      <c r="G32" s="4">
+        <f t="shared" ref="G32" si="35">B32+D32+F32</f>
         <v>0.11075</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="1">
-        <v>1.56</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="E32" s="4">
-        <f>B32*0.1</f>
-        <v>0.15600000000000003</v>
-      </c>
-      <c r="F32" s="4">
-        <f t="shared" si="14"/>
-        <v>0.18447000000000002</v>
-      </c>
-      <c r="G32" s="4">
-        <f t="shared" si="15"/>
-        <v>1.7444700000000002</v>
-      </c>
       <c r="H32" s="4">
-        <f t="shared" si="16"/>
-        <v>0.87223500000000009</v>
+        <f t="shared" ref="H32" si="36">G32/C32</f>
+        <v>0.11075</v>
       </c>
       <c r="I32">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J32" s="4">
-        <f t="shared" si="17"/>
-        <v>1.7444700000000002</v>
-      </c>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
+        <f t="shared" ref="J32" si="37">H32*I32</f>
+        <v>0.55374999999999996</v>
+      </c>
+      <c r="M32">
+        <f t="shared" ref="M32" si="38">$C$1*I32</f>
+        <v>100</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <f t="shared" ref="O32" si="39">M32-N32</f>
+        <v>100</v>
+      </c>
+      <c r="P32">
+        <f t="shared" ref="P32" si="40">_xlfn.CEILING.MATH(O32/C32)</f>
+        <v>100</v>
+      </c>
+      <c r="Q32" s="4">
+        <f t="shared" ref="Q32" si="41">P32*G32</f>
+        <v>11.074999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B33" s="1">
         <v>0.13</v>
@@ -1625,36 +2074,55 @@
         <v>1.3000000000000001E-2</v>
       </c>
       <c r="F33" s="4">
-        <f t="shared" si="14"/>
+        <f>(B33+D33+E33)*0.1075</f>
         <v>1.5372500000000001E-2</v>
       </c>
       <c r="G33" s="4">
-        <f t="shared" si="15"/>
+        <f>B33+D33+F33</f>
         <v>0.14537250000000002</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="16"/>
+        <f>G33/C33</f>
         <v>0.14537250000000002</v>
       </c>
       <c r="I33">
         <v>1</v>
       </c>
       <c r="J33" s="4">
-        <f t="shared" si="17"/>
+        <f>H33*I33</f>
         <v>0.14537250000000002</v>
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M33">
+        <f>$C$1*I33</f>
+        <v>20</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f>M33-N33</f>
+        <v>20</v>
+      </c>
+      <c r="P33">
+        <f>_xlfn.CEILING.MATH(O33/C33)</f>
+        <v>20</v>
+      </c>
+      <c r="Q33" s="4">
+        <f>P33*G33</f>
+        <v>2.9074500000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>56</v>
       </c>
       <c r="B34" s="1">
-        <v>0.39</v>
+        <v>1.56</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
@@ -1663,33 +2131,50 @@
         <v>0</v>
       </c>
       <c r="F34" s="4">
+        <f>(B34+D34+E34)*0.1075</f>
+        <v>0.16770000000000002</v>
+      </c>
+      <c r="G34" s="4">
+        <f>B34+D34+F34</f>
+        <v>1.7277</v>
+      </c>
+      <c r="H34" s="4">
+        <f>G34/C34</f>
+        <v>0.86385000000000001</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+      <c r="J34" s="4">
+        <f>H34*I34</f>
+        <v>1.7277</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="11"/>
+        <v>40</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="12"/>
+        <v>40</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="Q34" s="4">
         <f t="shared" si="14"/>
-        <v>4.1925000000000004E-2</v>
-      </c>
-      <c r="G34" s="4">
-        <f t="shared" si="15"/>
-        <v>0.431925</v>
-      </c>
-      <c r="H34" s="4">
-        <f t="shared" si="16"/>
-        <v>0.431925</v>
-      </c>
-      <c r="I34">
-        <v>1</v>
-      </c>
-      <c r="J34" s="4">
-        <f t="shared" si="17"/>
-        <v>0.431925</v>
-      </c>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+        <v>34.554000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B35" s="1">
-        <v>1.56</v>
+        <v>1.3</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -1701,34 +2186,55 @@
         <v>0</v>
       </c>
       <c r="F35" s="4">
-        <f>(B35+D35+E35)*0.1075</f>
-        <v>0.16770000000000002</v>
+        <f t="shared" ref="F35" si="42">(B35+D35+E35)*0.1075</f>
+        <v>0.13975000000000001</v>
       </c>
       <c r="G35" s="4">
-        <f>B35+D35+F35</f>
-        <v>1.7277</v>
+        <f t="shared" ref="G35" si="43">B35+D35+F35</f>
+        <v>1.4397500000000001</v>
       </c>
       <c r="H35" s="4">
-        <f>G35/C35</f>
-        <v>0.86385000000000001</v>
+        <f t="shared" ref="H35" si="44">G35/C35</f>
+        <v>0.71987500000000004</v>
       </c>
       <c r="I35">
         <v>2</v>
       </c>
       <c r="J35" s="4">
-        <f>H35*I35</f>
-        <v>1.7277</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+        <f t="shared" ref="J35" si="45">H35*I35</f>
+        <v>1.4397500000000001</v>
+      </c>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35">
+        <f t="shared" si="11"/>
+        <v>40</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="12"/>
+        <v>40</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="Q35" s="4">
+        <f t="shared" si="14"/>
+        <v>28.795000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B36" s="1">
-        <v>1.3</v>
+        <v>0.47</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
@@ -1737,30 +2243,49 @@
         <v>0</v>
       </c>
       <c r="F36" s="4">
-        <f t="shared" ref="F36" si="18">(B36+D36+E36)*0.1075</f>
-        <v>0.13975000000000001</v>
+        <f t="shared" ref="F36" si="46">(B36+D36+E36)*0.1075</f>
+        <v>5.0524999999999994E-2</v>
       </c>
       <c r="G36" s="4">
-        <f t="shared" ref="G36" si="19">B36+D36+F36</f>
-        <v>1.4397500000000001</v>
+        <f t="shared" ref="G36" si="47">B36+D36+F36</f>
+        <v>0.52052500000000002</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" ref="H36" si="20">G36/C36</f>
-        <v>0.71987500000000004</v>
+        <f t="shared" ref="H36" si="48">G36/C36</f>
+        <v>0.52052500000000002</v>
       </c>
       <c r="I36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J36" s="4">
-        <f t="shared" ref="J36" si="21">H36*I36</f>
-        <v>1.4397500000000001</v>
+        <f t="shared" ref="J36" si="49">H36*I36</f>
+        <v>0.52052500000000002</v>
       </c>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M36">
+        <f t="shared" ref="M36" si="50">$C$1*I36</f>
+        <v>20</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <f t="shared" ref="O36" si="51">M36-N36</f>
+        <v>20</v>
+      </c>
+      <c r="P36">
+        <f t="shared" ref="P36" si="52">_xlfn.CEILING.MATH(O36/C36)</f>
+        <v>20</v>
+      </c>
+      <c r="Q36" s="4">
+        <f t="shared" ref="Q36" si="53">P36*G36</f>
+        <v>10.410500000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B37" s="1">
         <v>0.1</v>
@@ -1775,168 +2300,388 @@
         <v>0</v>
       </c>
       <c r="F37" s="4">
-        <f t="shared" ref="F37" si="22">(B37+D37+E37)*0.1075</f>
+        <f t="shared" ref="F37:F38" si="54">(B37+D37+E37)*0.1075</f>
         <v>1.0750000000000001E-2</v>
       </c>
       <c r="G37" s="4">
-        <f t="shared" ref="G37" si="23">B37+D37+F37</f>
+        <f t="shared" ref="G37:G38" si="55">B37+D37+F37</f>
         <v>0.11075</v>
       </c>
       <c r="H37" s="4">
-        <f t="shared" ref="H37" si="24">G37/C37</f>
+        <f t="shared" ref="H37:H38" si="56">G37/C37</f>
         <v>0.11075</v>
       </c>
       <c r="I37">
         <v>1</v>
       </c>
       <c r="J37" s="4">
-        <f t="shared" ref="J37" si="25">H37*I37</f>
+        <f t="shared" ref="J37:J38" si="57">H37*I37</f>
         <v>0.11075</v>
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
-    </row>
-    <row r="38" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="7">
-        <f>SUM(B22:B37)</f>
-        <v>10.700000000000001</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="7">
-        <f>SUM(G22:G37)</f>
-        <v>16.885614999999998</v>
-      </c>
-      <c r="H38" s="8"/>
-      <c r="I38" s="5">
-        <f>SUM(I22:I37)</f>
-        <v>24</v>
-      </c>
-      <c r="J38" s="10">
-        <f>SUM(J22:J37)</f>
-        <v>16.885614999999998</v>
-      </c>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A39" s="5"/>
-      <c r="B39" s="1"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A40" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="4"/>
-      <c r="J40" s="4"/>
+      <c r="M37">
+        <f>$C$1*I37</f>
+        <v>20</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <f>M37-N37</f>
+        <v>20</v>
+      </c>
+      <c r="P37">
+        <f>_xlfn.CEILING.MATH(O37/C37)</f>
+        <v>20</v>
+      </c>
+      <c r="Q37" s="4">
+        <f>P37*G37</f>
+        <v>2.2149999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2.14</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0</v>
+      </c>
+      <c r="F38" s="4">
+        <f t="shared" si="54"/>
+        <v>0.23005</v>
+      </c>
+      <c r="G38" s="4">
+        <f t="shared" si="55"/>
+        <v>2.37005</v>
+      </c>
+      <c r="H38" s="4">
+        <f t="shared" si="56"/>
+        <v>0.23700499999999999</v>
+      </c>
+      <c r="I38">
+        <v>10</v>
+      </c>
+      <c r="J38" s="4">
+        <f t="shared" si="57"/>
+        <v>2.37005</v>
+      </c>
+      <c r="M38">
+        <f t="shared" ref="M38" si="58">$C$1*I38</f>
+        <v>200</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <f t="shared" ref="O38" si="59">M38-N38</f>
+        <v>200</v>
+      </c>
+      <c r="P38">
+        <f t="shared" ref="P38" si="60">_xlfn.CEILING.MATH(O38/C38)</f>
+        <v>20</v>
+      </c>
+      <c r="Q38" s="4">
+        <f t="shared" ref="Q38" si="61">P38*G38</f>
+        <v>47.400999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0</v>
+      </c>
+      <c r="F39" s="4">
+        <f t="shared" ref="F39" si="62">(B39+D39+E39)*0.1075</f>
+        <v>0.12362499999999998</v>
+      </c>
+      <c r="G39" s="4">
+        <f t="shared" ref="G39" si="63">B39+D39+F39</f>
+        <v>1.273625</v>
+      </c>
+      <c r="H39" s="4">
+        <f t="shared" ref="H39" si="64">G39/C39</f>
+        <v>0.25472499999999998</v>
+      </c>
+      <c r="I39">
+        <v>5</v>
+      </c>
+      <c r="J39" s="4">
+        <f t="shared" ref="J39" si="65">H39*I39</f>
+        <v>1.273625</v>
+      </c>
+      <c r="M39">
+        <f t="shared" ref="M39" si="66">$C$1*I39</f>
+        <v>100</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <f t="shared" ref="O39" si="67">M39-N39</f>
+        <v>100</v>
+      </c>
+      <c r="P39">
+        <f t="shared" ref="P39" si="68">_xlfn.CEILING.MATH(O39/C39)</f>
+        <v>20</v>
+      </c>
+      <c r="Q39" s="4">
+        <f t="shared" ref="Q39" si="69">P39*G39</f>
+        <v>25.4725</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1.42</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="4">
+        <f>B40*0.1</f>
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="F40" s="4">
+        <f>(B40+D40+E40)*0.1075</f>
+        <v>0.16791499999999998</v>
+      </c>
+      <c r="G40" s="4">
+        <f>B40+D40+F40</f>
+        <v>1.587915</v>
+      </c>
+      <c r="H40" s="4">
+        <f>G40/C40</f>
+        <v>0.79395749999999998</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+      <c r="J40" s="4">
+        <f>H40*I40</f>
+        <v>1.587915</v>
+      </c>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A41" s="6" t="s">
+      <c r="M40">
+        <f>$C$1*I40</f>
+        <v>40</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <f>M40-N40</f>
+        <v>40</v>
+      </c>
+      <c r="P40">
+        <f>_xlfn.CEILING.MATH(O40/C40)</f>
+        <v>20</v>
+      </c>
+      <c r="Q40" s="4">
+        <f>P40*G40</f>
+        <v>31.758299999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="7">
+        <f>SUM(B22:B40)</f>
+        <v>14.23</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="7">
+        <f>SUM(G22:G40)</f>
+        <v>20.793584999999997</v>
+      </c>
+      <c r="H41" s="8"/>
+      <c r="I41" s="5">
+        <f>SUM(I22:I40)</f>
         <v>57</v>
       </c>
-      <c r="B41" s="1">
-        <f>23.49*0.99</f>
-        <v>23.255099999999999</v>
-      </c>
-      <c r="C41">
-        <v>15</v>
-      </c>
-      <c r="D41" s="1">
-        <v>22.04</v>
-      </c>
-      <c r="E41" s="4">
-        <v>0</v>
-      </c>
-      <c r="F41" s="4">
-        <v>0</v>
-      </c>
-      <c r="G41" s="4">
-        <f t="shared" ref="G41" si="26">B41+D41+F41</f>
-        <v>45.295099999999998</v>
-      </c>
-      <c r="H41" s="4">
-        <f t="shared" ref="H41" si="27">G41/C41</f>
-        <v>3.019673333333333</v>
-      </c>
-      <c r="I41">
-        <v>1</v>
-      </c>
-      <c r="J41" s="4">
-        <f t="shared" ref="J41" si="28">H41*I41</f>
-        <v>3.019673333333333</v>
-      </c>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="1"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A42" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B42" s="7">
-        <f>SUM(B41:B41)</f>
-        <v>23.255099999999999</v>
-      </c>
+      <c r="J41" s="10">
+        <f>SUM(J22:J40)</f>
+        <v>22.454834999999999</v>
+      </c>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="Q41" s="10">
+        <f>SUM(Q22:Q40)</f>
+        <v>449.31820000000005</v>
+      </c>
+      <c r="S41" s="1">
+        <v>218.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A42" s="5"/>
+      <c r="B42" s="1"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="7">
-        <f>SUM(G41:G41)</f>
-        <v>45.295099999999998</v>
-      </c>
+      <c r="G42" s="1"/>
       <c r="H42" s="4"/>
-      <c r="I42" s="5">
-        <f>SUM(I41:I41)</f>
-        <v>1</v>
-      </c>
-      <c r="J42" s="7">
-        <f>SUM(J41:J41)</f>
-        <v>3.019673333333333</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A43" s="5"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A43" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="B43" s="1"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+      <c r="G43" s="1"/>
       <c r="H43" s="4"/>
       <c r="J43" s="4"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A44" s="5" t="s">
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A44" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="1">
+        <v>30.66</v>
+      </c>
+      <c r="C44">
+        <f>$C$1</f>
+        <v>20</v>
+      </c>
+      <c r="D44" s="1">
+        <v>29.89</v>
+      </c>
+      <c r="E44" s="4">
+        <v>0</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="4">
+        <f t="shared" ref="G44" si="70">B44+D44+F44</f>
+        <v>60.55</v>
+      </c>
+      <c r="H44" s="4">
+        <f t="shared" ref="H44" si="71">G44/C44</f>
+        <v>3.0274999999999999</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44" s="4">
+        <f t="shared" ref="J44" si="72">H44*I44</f>
+        <v>3.0274999999999999</v>
+      </c>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44">
+        <f t="shared" ref="M44" si="73">$C$1*I44</f>
+        <v>20</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <f t="shared" ref="O44" si="74">M44-N44</f>
+        <v>20</v>
+      </c>
+      <c r="P44">
+        <f t="shared" ref="P44" si="75">_xlfn.CEILING.MATH(O44/C44)</f>
+        <v>1</v>
+      </c>
+      <c r="Q44" s="4">
+        <f t="shared" ref="Q44" si="76">P44*G44</f>
+        <v>60.55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A45" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="10">
-        <f>B14+B19+B38+B42</f>
-        <v>170.91509999999997</v>
-      </c>
-      <c r="G44" s="10">
-        <f>G14+G19+G38+G42</f>
-        <v>213.86391499999999</v>
-      </c>
-      <c r="I44" s="11">
-        <f>I14+I19+I38+I42</f>
-        <v>45</v>
-      </c>
-      <c r="J44" s="7">
-        <f>J14+J19+J38+J42</f>
-        <v>50.35891724999999</v>
+      <c r="B45" s="7">
+        <f>SUM(B44:B44)</f>
+        <v>30.66</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="7">
+        <f>SUM(G44:G44)</f>
+        <v>60.55</v>
+      </c>
+      <c r="H45" s="4"/>
+      <c r="I45" s="5">
+        <f>SUM(I44:I44)</f>
+        <v>1</v>
+      </c>
+      <c r="J45" s="7">
+        <f>SUM(J44:J44)</f>
+        <v>3.0274999999999999</v>
+      </c>
+      <c r="Q45" s="7">
+        <f>SUM(Q44:Q44)</f>
+        <v>60.55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A46" s="5"/>
+      <c r="B46" s="1"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="J46" s="4"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A47" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="10">
+        <f>B14+B19+B41+B45</f>
+        <v>181.84999999999997</v>
+      </c>
+      <c r="G47" s="10">
+        <f>G14+G19+G41+G45</f>
+        <v>233.02678500000002</v>
+      </c>
+      <c r="I47" s="11">
+        <f>I14+I19+I41+I45</f>
+        <v>78</v>
+      </c>
+      <c r="J47" s="7">
+        <f>J14+J19+J41+J45</f>
+        <v>55.935963916666665</v>
+      </c>
+      <c r="Q47" s="7">
+        <f>Q14+Q19+Q41+Q45</f>
+        <v>1156.6038999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted Qty On Hand column after taking inventory.
Digi-Key order has been placed.  They haven't given me a final total yet,
so I still cannot compute the final kit price, but the quantity price
breaks probably saved about $6 per kit.
</commit_message>
<xml_diff>
--- a/parts/bill_of_materials.xlsx
+++ b/parts/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\laser_tunnel\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D939F89-716B-4704-99BF-CCEAEF3EB788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD140A74-FAF0-411A-97F3-179429EB834C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C7A15FB5-B248-4CA2-8E4B-B85C1BCDD779}"/>
   </bookViews>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A265784A-A2E2-4F2C-B0D4-276F819350E1}">
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -678,7 +678,7 @@
     <col min="13" max="13" width="12.23046875" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
     <col min="16" max="16" width="12.84375" customWidth="1"/>
-    <col min="17" max="17" width="11.765625" customWidth="1"/>
+    <col min="17" max="17" width="12.765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
@@ -786,7 +786,7 @@
         <v>7</v>
       </c>
       <c r="M4">
-        <f>$D$1*J4</f>
+        <f t="shared" ref="M4:M12" si="3">$D$1*J4</f>
         <v>20</v>
       </c>
       <c r="N4">
@@ -797,11 +797,11 @@
         <v>19</v>
       </c>
       <c r="P4">
-        <f>_xlfn.CEILING.MATH(O4/D4)</f>
+        <f t="shared" ref="P4:P12" si="4">_xlfn.CEILING.MATH(O4/D4)</f>
         <v>19</v>
       </c>
       <c r="Q4" s="4">
-        <f>P4*H4</f>
+        <f t="shared" ref="Q4:Q12" si="5">P4*H4</f>
         <v>209.37287499999999</v>
       </c>
     </row>
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" ref="G5:G12" si="3">(C5+E5+F5)*0.1075</f>
+        <f t="shared" ref="G5:G12" si="6">(C5+E5+F5)*0.1075</f>
         <v>0.64392499999999997</v>
       </c>
       <c r="H5" s="4">
@@ -841,22 +841,22 @@
         <v>8</v>
       </c>
       <c r="M5">
-        <f>$D$1*J5</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="N5">
         <v>8</v>
       </c>
       <c r="O5">
-        <f t="shared" ref="O5:O12" si="4">MAX(0, M5-N5)</f>
+        <f t="shared" ref="O5:O12" si="7">MAX(0, M5-N5)</f>
         <v>12</v>
       </c>
       <c r="P5">
-        <f>_xlfn.CEILING.MATH(O5/D5)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="Q5" s="4">
-        <f>P5*H5</f>
+        <f t="shared" si="5"/>
         <v>13.267850000000001</v>
       </c>
     </row>
@@ -874,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.85892500000000005</v>
       </c>
       <c r="H6" s="4">
@@ -896,22 +896,22 @@
         <v>9</v>
       </c>
       <c r="M6">
-        <f>$D$1*J6</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="N6">
         <v>50</v>
       </c>
       <c r="O6">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="P6">
-        <f>_xlfn.CEILING.MATH(O6/D6)</f>
         <v>1</v>
       </c>
       <c r="Q6" s="4">
-        <f>P6*H6</f>
+        <f t="shared" si="5"/>
         <v>8.8489249999999995</v>
       </c>
     </row>
@@ -929,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.64392499999999997</v>
       </c>
       <c r="H7" s="4">
@@ -951,22 +951,22 @@
         <v>22</v>
       </c>
       <c r="M7">
-        <f>$D$1*J7</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7">
+        <f t="shared" si="7"/>
+        <v>60</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-      <c r="P7">
-        <f>_xlfn.CEILING.MATH(O7/D7)</f>
         <v>1</v>
       </c>
       <c r="Q7" s="4">
-        <f>P7*H7</f>
+        <f t="shared" si="5"/>
         <v>6.6339250000000005</v>
       </c>
     </row>
@@ -984,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.0414249999999998</v>
       </c>
       <c r="H8" s="4">
@@ -1006,22 +1006,22 @@
         <v>10</v>
       </c>
       <c r="M8">
-        <f>$D$1*J8</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="N8">
         <v>3</v>
       </c>
       <c r="O8">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="4"/>
-        <v>17</v>
-      </c>
-      <c r="P8">
-        <f>_xlfn.CEILING.MATH(O8/D8)</f>
         <v>6</v>
       </c>
       <c r="Q8" s="4">
-        <f>P8*H8</f>
+        <f t="shared" si="5"/>
         <v>126.18854999999999</v>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.396425</v>
       </c>
       <c r="H9" s="4">
@@ -1061,22 +1061,22 @@
         <v>49</v>
       </c>
       <c r="M9">
-        <f>$D$1*J9</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="N9">
         <v>6</v>
       </c>
       <c r="O9">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="P9">
-        <f>_xlfn.CEILING.MATH(O9/D9)</f>
         <v>3</v>
       </c>
       <c r="Q9" s="4">
-        <f>P9*H9</f>
+        <f t="shared" si="5"/>
         <v>43.159275000000001</v>
       </c>
     </row>
@@ -1094,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.5576749999999999</v>
       </c>
       <c r="H10" s="4">
@@ -1116,22 +1116,22 @@
         <v>12</v>
       </c>
       <c r="M10">
-        <f>$D$1*J10</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="N10">
         <v>60</v>
       </c>
       <c r="O10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P10">
-        <f>_xlfn.CEILING.MATH(O10/D10)</f>
-        <v>0</v>
-      </c>
       <c r="Q10" s="4">
-        <f>P10*H10</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.80517499999999997</v>
       </c>
       <c r="H11" s="4">
@@ -1171,22 +1171,22 @@
         <v>13</v>
       </c>
       <c r="M11">
-        <f>$D$1*J11</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="N11">
         <v>50</v>
       </c>
       <c r="O11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P11">
-        <f>_xlfn.CEILING.MATH(O11/D11)</f>
-        <v>0</v>
-      </c>
       <c r="Q11" s="4">
-        <f>P11*H11</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1204,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.0414249999999998</v>
       </c>
       <c r="H12" s="4">
@@ -1226,22 +1226,22 @@
         <v>18</v>
       </c>
       <c r="M12">
-        <f>$D$1*J12</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="P12">
-        <f>_xlfn.CEILING.MATH(O12/D12)</f>
         <v>4</v>
       </c>
       <c r="Q12" s="4">
-        <f>P12*H12</f>
+        <f t="shared" si="5"/>
         <v>84.125699999999995</v>
       </c>
     </row>
@@ -1269,19 +1269,19 @@
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="12">
-        <f t="shared" ref="M13:P13" si="5">SUM(M4:M12)</f>
+        <f t="shared" ref="M13:P13" si="8">SUM(M4:M12)</f>
         <v>300</v>
       </c>
       <c r="N13" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>178</v>
       </c>
       <c r="O13" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>152</v>
       </c>
       <c r="P13" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>36</v>
       </c>
       <c r="Q13" s="7">
@@ -1319,22 +1319,22 @@
         <v>0</v>
       </c>
       <c r="G16" s="4">
-        <f t="shared" ref="G16" si="6">(C16+E16+F16)*0.1075</f>
+        <f t="shared" ref="G16" si="9">(C16+E16+F16)*0.1075</f>
         <v>0.19134999999999999</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" ref="H16" si="7">C16+E16+G16</f>
+        <f t="shared" ref="H16" si="10">C16+E16+G16</f>
         <v>1.9713499999999999</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" ref="I16" si="8">H16/D16</f>
+        <f t="shared" ref="I16" si="11">H16/D16</f>
         <v>1.9713499999999999</v>
       </c>
       <c r="J16">
         <v>1</v>
       </c>
       <c r="K16" s="4">
-        <f t="shared" ref="K16" si="9">I16*J16</f>
+        <f t="shared" ref="K16" si="12">I16*J16</f>
         <v>1.9713499999999999</v>
       </c>
       <c r="L16" s="3" t="s">
@@ -1348,7 +1348,7 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <f t="shared" ref="O16" si="10">MAX(0, M16-N16)</f>
+        <f t="shared" ref="O16" si="13">MAX(0, M16-N16)</f>
         <v>20</v>
       </c>
       <c r="P16">
@@ -1385,19 +1385,19 @@
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="12">
-        <f t="shared" ref="M17:P17" si="11">SUM(M16:M16)</f>
+        <f t="shared" ref="M17:P17" si="14">SUM(M16:M16)</f>
         <v>20</v>
       </c>
       <c r="N17" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O17" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>20</v>
       </c>
       <c r="P17" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>20</v>
       </c>
       <c r="Q17" s="7">
@@ -1457,22 +1457,22 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" ref="M20:M23" si="12">$D$1*J20</f>
+        <f t="shared" ref="M20:M23" si="15">$D$1*J20</f>
         <v>20</v>
       </c>
       <c r="N20">
         <v>0</v>
       </c>
       <c r="O20">
-        <f t="shared" ref="O20:O23" si="13">MAX(0, M20-N20)</f>
+        <f t="shared" ref="O20:O23" si="16">MAX(0, M20-N20)</f>
         <v>20</v>
       </c>
       <c r="P20">
-        <f t="shared" ref="P20:P23" si="14">_xlfn.CEILING.MATH(O20/D20)</f>
+        <f t="shared" ref="P20:P23" si="17">_xlfn.CEILING.MATH(O20/D20)</f>
         <v>20</v>
       </c>
       <c r="Q20" s="4">
-        <f t="shared" ref="Q20:Q23" si="15">P20*H20</f>
+        <f t="shared" ref="Q20:Q23" si="18">P20*H20</f>
         <v>0</v>
       </c>
     </row>
@@ -1509,22 +1509,22 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>20</v>
       </c>
       <c r="N21">
         <v>0</v>
       </c>
       <c r="O21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>20</v>
       </c>
       <c r="P21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="Q21" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -1561,22 +1561,22 @@
         <v>0</v>
       </c>
       <c r="M22">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>20</v>
       </c>
       <c r="N22">
         <v>0</v>
       </c>
       <c r="O22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>20</v>
       </c>
       <c r="P22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="Q22" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -1613,22 +1613,22 @@
         <v>0</v>
       </c>
       <c r="M23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>20</v>
       </c>
       <c r="N23">
         <v>0</v>
       </c>
       <c r="O23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>20</v>
       </c>
       <c r="P23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="Q23" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -1655,19 +1655,19 @@
         <v>0</v>
       </c>
       <c r="M24" s="12">
-        <f t="shared" ref="M24:P24" si="16">SUM(M20:M23)</f>
+        <f t="shared" ref="M24:P24" si="19">SUM(M20:M23)</f>
         <v>80</v>
       </c>
       <c r="N24" s="12">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O24" s="12">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>80</v>
       </c>
       <c r="P24" s="12">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>80</v>
       </c>
       <c r="Q24" s="7">
@@ -1715,41 +1715,41 @@
         <v>5.3000000000000005E-2</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" ref="G27" si="17">(C27+E27+F27)*0.1075</f>
+        <f t="shared" ref="G27" si="20">(C27+E27+F27)*0.1075</f>
         <v>6.2672500000000006E-2</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" ref="H27" si="18">C27+E27+G27</f>
+        <f t="shared" ref="H27" si="21">C27+E27+G27</f>
         <v>0.59267250000000005</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" ref="I27" si="19">H27/D27</f>
+        <f t="shared" ref="I27" si="22">H27/D27</f>
         <v>0.59267250000000005</v>
       </c>
       <c r="J27">
         <v>1</v>
       </c>
       <c r="K27" s="4">
-        <f t="shared" ref="K27" si="20">I27*J27</f>
+        <f t="shared" ref="K27" si="23">I27*J27</f>
         <v>0.59267250000000005</v>
       </c>
       <c r="M27">
-        <f>$D$1*J27</f>
+        <f t="shared" ref="M27:M44" si="24">$D$1*J27</f>
         <v>20</v>
       </c>
       <c r="N27">
         <v>20</v>
       </c>
       <c r="O27">
-        <f t="shared" ref="O27:O44" si="21">MAX(0, M27-N27)</f>
+        <f t="shared" ref="O27:O44" si="25">MAX(0, M27-N27)</f>
         <v>0</v>
       </c>
       <c r="P27">
-        <f>_xlfn.CEILING.MATH(O27/D27)</f>
+        <f t="shared" ref="P27:P44" si="26">_xlfn.CEILING.MATH(O27/D27)</f>
         <v>0</v>
       </c>
       <c r="Q27" s="4">
-        <f>P27*H27</f>
+        <f t="shared" ref="Q27:Q44" si="27">P27*H27</f>
         <v>0</v>
       </c>
     </row>
@@ -1790,22 +1790,22 @@
         <v>1.901025</v>
       </c>
       <c r="M28">
-        <f>$D$1*J28</f>
+        <f t="shared" si="24"/>
         <v>40</v>
       </c>
       <c r="N28">
         <v>0</v>
       </c>
       <c r="O28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>40</v>
       </c>
       <c r="P28">
-        <f>_xlfn.CEILING.MATH(O28/D28)</f>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="Q28" s="4">
-        <f>P28*H28</f>
+        <f t="shared" si="27"/>
         <v>38.020499999999998</v>
       </c>
     </row>
@@ -1845,23 +1845,23 @@
         <v>0.89707500000000007</v>
       </c>
       <c r="M29">
-        <f>$D$1*J29</f>
+        <f t="shared" si="24"/>
         <v>20</v>
       </c>
       <c r="N29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O29">
-        <f t="shared" si="21"/>
-        <v>20</v>
+        <f t="shared" si="25"/>
+        <v>10</v>
       </c>
       <c r="P29">
-        <f>_xlfn.CEILING.MATH(O29/D29)</f>
-        <v>20</v>
+        <f t="shared" si="26"/>
+        <v>10</v>
       </c>
       <c r="Q29" s="4">
-        <f>P29*H29</f>
-        <v>17.941500000000001</v>
+        <f t="shared" si="27"/>
+        <v>8.9707500000000007</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.4">
@@ -1882,42 +1882,42 @@
         <v>0.03</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" ref="G30" si="22">(C30+E30+F30)*0.1075</f>
+        <f t="shared" ref="G30" si="28">(C30+E30+F30)*0.1075</f>
         <v>0.15157499999999999</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" ref="H30" si="23">C30+E30+G30</f>
+        <f t="shared" ref="H30" si="29">C30+E30+G30</f>
         <v>1.5315749999999999</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" ref="I30" si="24">H30/D30</f>
+        <f t="shared" ref="I30" si="30">H30/D30</f>
         <v>1.5315749999999999</v>
       </c>
       <c r="J30">
         <v>1</v>
       </c>
       <c r="K30" s="4">
-        <f t="shared" ref="K30" si="25">I30*J30</f>
+        <f t="shared" ref="K30" si="31">I30*J30</f>
         <v>1.5315749999999999</v>
       </c>
       <c r="M30">
-        <f>$D$1*J30</f>
+        <f t="shared" si="24"/>
         <v>20</v>
       </c>
       <c r="N30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O30">
-        <f t="shared" si="21"/>
-        <v>20</v>
+        <f t="shared" si="25"/>
+        <v>10</v>
       </c>
       <c r="P30">
-        <f>_xlfn.CEILING.MATH(O30/D30)</f>
-        <v>20</v>
+        <f t="shared" si="26"/>
+        <v>10</v>
       </c>
       <c r="Q30" s="4">
-        <f>P30*H30</f>
-        <v>30.631499999999999</v>
+        <f t="shared" si="27"/>
+        <v>15.31575</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.4">
@@ -1937,41 +1937,41 @@
         <v>0</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" ref="G31:G34" si="26">(C31+E31+F31)*0.1075</f>
+        <f t="shared" ref="G31:G34" si="32">(C31+E31+F31)*0.1075</f>
         <v>4.7300000000000002E-2</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" ref="H31:H34" si="27">C31+E31+G31</f>
+        <f t="shared" ref="H31:H34" si="33">C31+E31+G31</f>
         <v>0.48730000000000001</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" ref="I31:I34" si="28">H31/D31</f>
+        <f t="shared" ref="I31:I34" si="34">H31/D31</f>
         <v>0.48730000000000001</v>
       </c>
       <c r="J31">
         <v>1</v>
       </c>
       <c r="K31" s="4">
-        <f t="shared" ref="K31:K34" si="29">I31*J31</f>
+        <f t="shared" ref="K31:K34" si="35">I31*J31</f>
         <v>0.48730000000000001</v>
       </c>
       <c r="M31">
-        <f>$D$1*J31</f>
+        <f t="shared" si="24"/>
         <v>20</v>
       </c>
       <c r="N31">
         <v>0</v>
       </c>
       <c r="O31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>20</v>
       </c>
       <c r="P31">
-        <f>_xlfn.CEILING.MATH(O31/D31)</f>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="Q31" s="4">
-        <f>P31*H31</f>
+        <f t="shared" si="27"/>
         <v>9.7460000000000004</v>
       </c>
     </row>
@@ -1992,41 +1992,41 @@
         <v>0</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>1.0750000000000001E-2</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0.11075</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>0.11075</v>
       </c>
       <c r="J32">
         <v>9</v>
       </c>
       <c r="K32" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>0.99675000000000002</v>
       </c>
       <c r="M32">
-        <f>$D$1*J32</f>
+        <f t="shared" si="24"/>
         <v>180</v>
       </c>
       <c r="N32">
         <v>0</v>
       </c>
       <c r="O32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>180</v>
       </c>
       <c r="P32">
-        <f>_xlfn.CEILING.MATH(O32/D32)</f>
+        <f t="shared" si="26"/>
         <v>180</v>
       </c>
       <c r="Q32" s="4">
-        <f>P32*H32</f>
+        <f t="shared" si="27"/>
         <v>19.934999999999999</v>
       </c>
     </row>
@@ -2047,41 +2047,41 @@
         <v>0</v>
       </c>
       <c r="G33" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>3.2250000000000001E-2</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0.33224999999999999</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>0.11075</v>
       </c>
       <c r="J33">
         <v>2</v>
       </c>
       <c r="K33" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>0.2215</v>
       </c>
       <c r="M33">
-        <f>$D$1*J33</f>
+        <f t="shared" si="24"/>
         <v>40</v>
       </c>
       <c r="N33">
         <v>0</v>
       </c>
       <c r="O33">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>40</v>
       </c>
       <c r="P33">
-        <f>_xlfn.CEILING.MATH(O33/D33)</f>
+        <f t="shared" si="26"/>
         <v>14</v>
       </c>
       <c r="Q33" s="4">
-        <f>P33*H33</f>
+        <f t="shared" si="27"/>
         <v>4.6514999999999995</v>
       </c>
     </row>
@@ -2102,41 +2102,41 @@
         <v>0</v>
       </c>
       <c r="G34" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>5.3749999999999999E-2</v>
       </c>
       <c r="H34" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0.55374999999999996</v>
       </c>
       <c r="I34" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>0.11074999999999999</v>
       </c>
       <c r="J34">
         <v>5</v>
       </c>
       <c r="K34" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>0.55374999999999996</v>
       </c>
       <c r="M34">
-        <f>$D$1*J34</f>
+        <f t="shared" si="24"/>
         <v>100</v>
       </c>
       <c r="N34">
         <v>0</v>
       </c>
       <c r="O34">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>100</v>
       </c>
       <c r="P34">
-        <f>_xlfn.CEILING.MATH(O34/D34)</f>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="Q34" s="4">
-        <f>P34*H34</f>
+        <f t="shared" si="27"/>
         <v>11.074999999999999</v>
       </c>
     </row>
@@ -2157,41 +2157,41 @@
         <v>0</v>
       </c>
       <c r="G35" s="4">
-        <f t="shared" ref="G35" si="30">(C35+E35+F35)*0.1075</f>
+        <f t="shared" ref="G35" si="36">(C35+E35+F35)*0.1075</f>
         <v>1.0750000000000001E-2</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" ref="H35" si="31">C35+E35+G35</f>
+        <f t="shared" ref="H35" si="37">C35+E35+G35</f>
         <v>0.11075</v>
       </c>
       <c r="I35" s="4">
-        <f t="shared" ref="I35" si="32">H35/D35</f>
+        <f t="shared" ref="I35" si="38">H35/D35</f>
         <v>0.11075</v>
       </c>
       <c r="J35">
         <v>5</v>
       </c>
       <c r="K35" s="4">
-        <f t="shared" ref="K35" si="33">I35*J35</f>
+        <f t="shared" ref="K35" si="39">I35*J35</f>
         <v>0.55374999999999996</v>
       </c>
       <c r="M35">
-        <f>$D$1*J35</f>
+        <f t="shared" si="24"/>
         <v>100</v>
       </c>
       <c r="N35">
         <v>0</v>
       </c>
       <c r="O35">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>100</v>
       </c>
       <c r="P35">
-        <f>_xlfn.CEILING.MATH(O35/D35)</f>
+        <f t="shared" si="26"/>
         <v>100</v>
       </c>
       <c r="Q35" s="4">
-        <f>P35*H35</f>
+        <f t="shared" si="27"/>
         <v>11.074999999999999</v>
       </c>
     </row>
@@ -2212,41 +2212,41 @@
         <v>0</v>
       </c>
       <c r="G36" s="4">
-        <f t="shared" ref="G36" si="34">(C36+E36+F36)*0.1075</f>
+        <f t="shared" ref="G36" si="40">(C36+E36+F36)*0.1075</f>
         <v>1.0750000000000001E-2</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" ref="H36" si="35">C36+E36+G36</f>
+        <f t="shared" ref="H36" si="41">C36+E36+G36</f>
         <v>0.11075</v>
       </c>
       <c r="I36" s="4">
-        <f t="shared" ref="I36" si="36">H36/D36</f>
+        <f t="shared" ref="I36" si="42">H36/D36</f>
         <v>0.11075</v>
       </c>
       <c r="J36">
         <v>5</v>
       </c>
       <c r="K36" s="4">
-        <f t="shared" ref="K36" si="37">I36*J36</f>
+        <f t="shared" ref="K36" si="43">I36*J36</f>
         <v>0.55374999999999996</v>
       </c>
       <c r="M36">
-        <f>$D$1*J36</f>
+        <f t="shared" si="24"/>
         <v>100</v>
       </c>
       <c r="N36">
         <v>0</v>
       </c>
       <c r="O36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>100</v>
       </c>
       <c r="P36">
-        <f>_xlfn.CEILING.MATH(O36/D36)</f>
+        <f t="shared" si="26"/>
         <v>100</v>
       </c>
       <c r="Q36" s="4">
-        <f>P36*H36</f>
+        <f t="shared" si="27"/>
         <v>11.074999999999999</v>
       </c>
     </row>
@@ -2288,23 +2288,23 @@
       </c>
       <c r="L37" s="3"/>
       <c r="M37">
-        <f>$D$1*J37</f>
+        <f t="shared" si="24"/>
         <v>20</v>
       </c>
       <c r="N37">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O37">
-        <f t="shared" si="21"/>
-        <v>20</v>
+        <f t="shared" si="25"/>
+        <v>10</v>
       </c>
       <c r="P37">
-        <f>_xlfn.CEILING.MATH(O37/D37)</f>
-        <v>20</v>
+        <f t="shared" si="26"/>
+        <v>10</v>
       </c>
       <c r="Q37" s="4">
-        <f>P37*H37</f>
-        <v>2.9074500000000003</v>
+        <f t="shared" si="27"/>
+        <v>1.4537250000000002</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.4">
@@ -2343,22 +2343,22 @@
         <v>1.7277</v>
       </c>
       <c r="M38">
-        <f>$D$1*J38</f>
+        <f t="shared" si="24"/>
         <v>40</v>
       </c>
       <c r="N38">
         <v>50</v>
       </c>
       <c r="O38">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="P38">
-        <f>_xlfn.CEILING.MATH(O38/D38)</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="Q38" s="4">
-        <f>P38*H38</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -2379,42 +2379,42 @@
         <v>0</v>
       </c>
       <c r="G39" s="4">
-        <f t="shared" ref="G39" si="38">(C39+E39+F39)*0.1075</f>
+        <f t="shared" ref="G39" si="44">(C39+E39+F39)*0.1075</f>
         <v>0.13975000000000001</v>
       </c>
       <c r="H39" s="4">
-        <f t="shared" ref="H39" si="39">C39+E39+G39</f>
+        <f t="shared" ref="H39" si="45">C39+E39+G39</f>
         <v>1.4397500000000001</v>
       </c>
       <c r="I39" s="4">
-        <f t="shared" ref="I39" si="40">H39/D39</f>
+        <f t="shared" ref="I39" si="46">H39/D39</f>
         <v>0.71987500000000004</v>
       </c>
       <c r="J39">
         <v>2</v>
       </c>
       <c r="K39" s="4">
-        <f t="shared" ref="K39" si="41">I39*J39</f>
+        <f t="shared" ref="K39" si="47">I39*J39</f>
         <v>1.4397500000000001</v>
       </c>
       <c r="L39" s="3"/>
       <c r="M39">
-        <f>$D$1*J39</f>
+        <f t="shared" si="24"/>
         <v>40</v>
       </c>
       <c r="N39">
         <v>0</v>
       </c>
       <c r="O39">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>40</v>
       </c>
       <c r="P39">
-        <f>_xlfn.CEILING.MATH(O39/D39)</f>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="Q39" s="4">
-        <f>P39*H39</f>
+        <f t="shared" si="27"/>
         <v>28.795000000000002</v>
       </c>
     </row>
@@ -2435,42 +2435,42 @@
         <v>0</v>
       </c>
       <c r="G40" s="4">
-        <f t="shared" ref="G40" si="42">(C40+E40+F40)*0.1075</f>
+        <f t="shared" ref="G40" si="48">(C40+E40+F40)*0.1075</f>
         <v>5.0524999999999994E-2</v>
       </c>
       <c r="H40" s="4">
-        <f t="shared" ref="H40" si="43">C40+E40+G40</f>
+        <f t="shared" ref="H40" si="49">C40+E40+G40</f>
         <v>0.52052500000000002</v>
       </c>
       <c r="I40" s="4">
-        <f t="shared" ref="I40" si="44">H40/D40</f>
+        <f t="shared" ref="I40" si="50">H40/D40</f>
         <v>0.52052500000000002</v>
       </c>
       <c r="J40">
         <v>1</v>
       </c>
       <c r="K40" s="4">
-        <f t="shared" ref="K40" si="45">I40*J40</f>
+        <f t="shared" ref="K40" si="51">I40*J40</f>
         <v>0.52052500000000002</v>
       </c>
       <c r="L40" s="3"/>
       <c r="M40">
-        <f>$D$1*J40</f>
+        <f t="shared" si="24"/>
         <v>20</v>
       </c>
       <c r="N40">
         <v>0</v>
       </c>
       <c r="O40">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>20</v>
       </c>
       <c r="P40">
-        <f>_xlfn.CEILING.MATH(O40/D40)</f>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="Q40" s="4">
-        <f>P40*H40</f>
+        <f t="shared" si="27"/>
         <v>10.410500000000001</v>
       </c>
     </row>
@@ -2491,43 +2491,43 @@
         <v>0</v>
       </c>
       <c r="G41" s="4">
-        <f t="shared" ref="G41:G42" si="46">(C41+E41+F41)*0.1075</f>
+        <f t="shared" ref="G41:G42" si="52">(C41+E41+F41)*0.1075</f>
         <v>1.0750000000000001E-2</v>
       </c>
       <c r="H41" s="4">
-        <f t="shared" ref="H41:H42" si="47">C41+E41+G41</f>
+        <f t="shared" ref="H41:H42" si="53">C41+E41+G41</f>
         <v>0.11075</v>
       </c>
       <c r="I41" s="4">
-        <f t="shared" ref="I41:I42" si="48">H41/D41</f>
+        <f t="shared" ref="I41:I42" si="54">H41/D41</f>
         <v>0.11075</v>
       </c>
       <c r="J41">
         <v>1</v>
       </c>
       <c r="K41" s="4">
-        <f t="shared" ref="K41:K42" si="49">I41*J41</f>
+        <f t="shared" ref="K41:K42" si="55">I41*J41</f>
         <v>0.11075</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41">
-        <f>$D$1*J41</f>
+        <f t="shared" si="24"/>
         <v>20</v>
       </c>
       <c r="N41">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O41">
-        <f t="shared" si="21"/>
-        <v>20</v>
+        <f t="shared" si="25"/>
+        <v>10</v>
       </c>
       <c r="P41">
-        <f>_xlfn.CEILING.MATH(O41/D41)</f>
-        <v>20</v>
+        <f t="shared" si="26"/>
+        <v>10</v>
       </c>
       <c r="Q41" s="4">
-        <f>P41*H41</f>
-        <v>2.2149999999999999</v>
+        <f t="shared" si="27"/>
+        <v>1.1074999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.4">
@@ -2547,41 +2547,41 @@
         <v>0</v>
       </c>
       <c r="G42" s="4">
-        <f t="shared" si="46"/>
+        <f t="shared" si="52"/>
         <v>0.23005</v>
       </c>
       <c r="H42" s="4">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>2.37005</v>
       </c>
       <c r="I42" s="4">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.23700499999999999</v>
       </c>
       <c r="J42">
         <v>10</v>
       </c>
       <c r="K42" s="4">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>2.37005</v>
       </c>
       <c r="M42">
-        <f>$D$1*J42</f>
+        <f t="shared" si="24"/>
         <v>200</v>
       </c>
       <c r="N42">
         <v>0</v>
       </c>
       <c r="O42">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>200</v>
       </c>
       <c r="P42">
-        <f>_xlfn.CEILING.MATH(O42/D42)</f>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="Q42" s="4">
-        <f>P42*H42</f>
+        <f t="shared" si="27"/>
         <v>47.400999999999996</v>
       </c>
     </row>
@@ -2602,42 +2602,42 @@
         <v>0</v>
       </c>
       <c r="G43" s="4">
-        <f t="shared" ref="G43" si="50">(C43+E43+F43)*0.1075</f>
+        <f t="shared" ref="G43" si="56">(C43+E43+F43)*0.1075</f>
         <v>0.12362499999999998</v>
       </c>
       <c r="H43" s="4">
-        <f t="shared" ref="H43" si="51">C43+E43+G43</f>
+        <f t="shared" ref="H43" si="57">C43+E43+G43</f>
         <v>1.273625</v>
       </c>
       <c r="I43" s="4">
-        <f t="shared" ref="I43" si="52">H43/D43</f>
+        <f t="shared" ref="I43" si="58">H43/D43</f>
         <v>0.25472499999999998</v>
       </c>
       <c r="J43">
         <v>5</v>
       </c>
       <c r="K43" s="4">
-        <f t="shared" ref="K43" si="53">I43*J43</f>
+        <f t="shared" ref="K43" si="59">I43*J43</f>
         <v>1.273625</v>
       </c>
       <c r="M43">
-        <f>$D$1*J43</f>
+        <f t="shared" si="24"/>
         <v>100</v>
       </c>
       <c r="N43">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O43">
-        <f t="shared" si="21"/>
-        <v>100</v>
+        <f t="shared" si="25"/>
+        <v>90</v>
       </c>
       <c r="P43">
-        <f>_xlfn.CEILING.MATH(O43/D43)</f>
-        <v>20</v>
+        <f t="shared" si="26"/>
+        <v>18</v>
       </c>
       <c r="Q43" s="4">
-        <f>P43*H43</f>
-        <v>25.4725</v>
+        <f t="shared" si="27"/>
+        <v>22.925249999999998</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.4">
@@ -2678,22 +2678,22 @@
       </c>
       <c r="L44" s="3"/>
       <c r="M44">
-        <f>$D$1*J44</f>
+        <f t="shared" si="24"/>
         <v>40</v>
       </c>
       <c r="N44">
         <v>0</v>
       </c>
       <c r="O44">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>40</v>
       </c>
       <c r="P44">
-        <f>_xlfn.CEILING.MATH(O44/D44)</f>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="Q44" s="4">
-        <f>P44*H44</f>
+        <f t="shared" si="27"/>
         <v>31.758299999999998</v>
       </c>
     </row>
@@ -2722,24 +2722,24 @@
       </c>
       <c r="L45" s="9"/>
       <c r="M45" s="5">
-        <f t="shared" ref="M45:P45" si="54">SUM(M27:M44)</f>
+        <f t="shared" ref="M45:P45" si="60">SUM(M27:M44)</f>
         <v>1120</v>
       </c>
       <c r="N45" s="5">
-        <f t="shared" si="54"/>
-        <v>70</v>
+        <f t="shared" si="60"/>
+        <v>120</v>
       </c>
       <c r="O45" s="5">
-        <f t="shared" si="54"/>
-        <v>1060</v>
+        <f t="shared" si="60"/>
+        <v>1010</v>
       </c>
       <c r="P45" s="5">
-        <f t="shared" si="54"/>
-        <v>634</v>
+        <f t="shared" si="60"/>
+        <v>592</v>
       </c>
       <c r="Q45" s="10">
         <f>SUM(Q27:Q44)</f>
-        <v>303.11075000000005</v>
+        <v>273.71577500000001</v>
       </c>
       <c r="S45" s="1">
         <v>218.6</v>
@@ -2788,18 +2788,18 @@
         <v>0</v>
       </c>
       <c r="H48" s="4">
-        <f t="shared" ref="H48" si="55">C48+E48+G48</f>
+        <f t="shared" ref="H48" si="61">C48+E48+G48</f>
         <v>60.55</v>
       </c>
       <c r="I48" s="4">
-        <f t="shared" ref="I48" si="56">H48/D48</f>
+        <f t="shared" ref="I48" si="62">H48/D48</f>
         <v>3.0274999999999999</v>
       </c>
       <c r="J48">
         <v>1</v>
       </c>
       <c r="K48" s="4">
-        <f t="shared" ref="K48" si="57">I48*J48</f>
+        <f t="shared" ref="K48" si="63">I48*J48</f>
         <v>3.0274999999999999</v>
       </c>
       <c r="L48" s="3"/>
@@ -2901,24 +2901,24 @@
         <v>49.771090999999998</v>
       </c>
       <c r="M51" s="11">
-        <f t="shared" ref="M51:P51" si="58">M13+M17+M24+M45+M49</f>
+        <f t="shared" ref="M51:P51" si="64">M13+M17+M24+M45+M49</f>
         <v>1540</v>
       </c>
       <c r="N51" s="11">
-        <f t="shared" si="58"/>
-        <v>248</v>
+        <f t="shared" si="64"/>
+        <v>298</v>
       </c>
       <c r="O51" s="11">
-        <f t="shared" si="58"/>
-        <v>1332</v>
+        <f t="shared" si="64"/>
+        <v>1282</v>
       </c>
       <c r="P51" s="11">
-        <f t="shared" si="58"/>
-        <v>771</v>
+        <f t="shared" si="64"/>
+        <v>729</v>
       </c>
       <c r="Q51" s="10">
         <f>Q13+Q17+Q24+Q45+Q49</f>
-        <v>894.68484999999998</v>
+        <v>865.28987499999994</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Updated bill of materials with Amazon order.
Added several columns to better track the final kit cost.  A few
Amazon items got more expensive since I selected the parts, but
that was more than offset by the DigiKey savings due to quantity
price breaks.
</commit_message>
<xml_diff>
--- a/parts/bill_of_materials.xlsx
+++ b/parts/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\laser_tunnel\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD140A74-FAF0-411A-97F3-179429EB834C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8164A0F9-030D-4361-B555-D6D13014B7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C7A15FB5-B248-4CA2-8E4B-B85C1BCDD779}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>Laser Tunnel</t>
   </si>
@@ -52,9 +52,6 @@
     <t>5V 5mW 650nm (red) dot laser diode</t>
   </si>
   <si>
-    <t>Noctua NF-R8 redux-1800 PWM fan</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/gp/product/B00KF7MVI2</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>10 kOhm trimpot</t>
   </si>
   <si>
-    <t>Purchase Price</t>
-  </si>
-  <si>
     <t>Purchase Qty</t>
   </si>
   <si>
@@ -211,12 +205,6 @@
     <t>Qty Needed</t>
   </si>
   <si>
-    <t>Purchase Units</t>
-  </si>
-  <si>
-    <t>Purchase Cost</t>
-  </si>
-  <si>
     <t>10 Ohm resistor</t>
   </si>
   <si>
@@ -256,7 +244,43 @@
     <t>15 degree mirror holder</t>
   </si>
   <si>
-    <t>Note that the DigiKey price for many parts drops significantly when ordered in modest quantities, so total cost may be several dollars lower per kit.</t>
+    <t>Actual Cost</t>
+  </si>
+  <si>
+    <t>Estimated Cost</t>
+  </si>
+  <si>
+    <t>Actual Tariff</t>
+  </si>
+  <si>
+    <t>Actual Price</t>
+  </si>
+  <si>
+    <t>Advertised Price</t>
+  </si>
+  <si>
+    <t>Purchase Blocks</t>
+  </si>
+  <si>
+    <t>Unit Qty Ordered</t>
+  </si>
+  <si>
+    <t>Actual Sales Tax</t>
+  </si>
+  <si>
+    <t>Actual Unit Cost</t>
+  </si>
+  <si>
+    <t>Actual Kit Cost</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>Note that the DigiKey price for many parts drops significantly when ordered in modest quantities, so actual cost may be several dollars lower per kit.</t>
+  </si>
+  <si>
+    <t>Noctua NF-R8 redux-1800 fan</t>
   </si>
 </sst>
 </file>
@@ -266,7 +290,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +327,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -329,19 +361,19 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -658,16 +690,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A265784A-A2E2-4F2C-B0D4-276F819350E1}">
-  <dimension ref="A1:S53"/>
+  <dimension ref="A1:Y54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.07421875" customWidth="1"/>
-    <col min="2" max="2" width="30.84375" customWidth="1"/>
+    <col min="1" max="1" width="10.3828125" customWidth="1"/>
+    <col min="2" max="2" width="25.3046875" customWidth="1"/>
     <col min="3" max="3" width="12.53515625" customWidth="1"/>
     <col min="4" max="4" width="12.23046875" customWidth="1"/>
     <col min="5" max="6" width="8.69140625" customWidth="1"/>
@@ -679,80 +712,110 @@
     <col min="15" max="15" width="11" customWidth="1"/>
     <col min="16" max="16" width="12.84375" customWidth="1"/>
     <col min="17" max="17" width="12.765625" customWidth="1"/>
+    <col min="18" max="18" width="15.15234375" customWidth="1"/>
+    <col min="19" max="19" width="12.15234375" customWidth="1"/>
+    <col min="20" max="20" width="11.07421875" customWidth="1"/>
+    <col min="21" max="21" width="13.921875" customWidth="1"/>
+    <col min="22" max="22" width="10.07421875" customWidth="1"/>
+    <col min="23" max="23" width="14.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
       </c>
       <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
         <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" t="s">
-        <v>29</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
       <c r="M2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" t="s">
         <v>56</v>
       </c>
-      <c r="N2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O2" t="s">
-        <v>58</v>
-      </c>
       <c r="P2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="Q2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>71</v>
+      </c>
+      <c r="R2" t="s">
+        <v>76</v>
+      </c>
+      <c r="S2" t="s">
+        <v>73</v>
+      </c>
+      <c r="T2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U2" t="s">
+        <v>77</v>
+      </c>
+      <c r="V2" t="s">
+        <v>70</v>
+      </c>
+      <c r="W2" t="s">
+        <v>78</v>
+      </c>
+      <c r="X2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B4" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="C4" s="1">
         <v>9.9499999999999993</v>
@@ -763,27 +826,27 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <f>(C4+E4+F4)*0.1075</f>
         <v>1.0696249999999998</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <f t="shared" ref="H4:H12" si="0">C4+E4+G4</f>
         <v>11.019625</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <f t="shared" ref="I4:I12" si="1">H4/D4</f>
         <v>11.019625</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <f t="shared" ref="K4:K12" si="2">I4*J4</f>
         <v>11.019625</v>
       </c>
       <c r="L4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M4">
         <f t="shared" ref="M4:M12" si="3">$D$1*J4</f>
@@ -800,12 +863,41 @@
         <f t="shared" ref="P4:P12" si="4">_xlfn.CEILING.MATH(O4/D4)</f>
         <v>19</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <f t="shared" ref="Q4:Q12" si="5">P4*H4</f>
         <v>209.37287499999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R4">
+        <v>19</v>
+      </c>
+      <c r="S4" s="1">
+        <v>189.05</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="3">
+        <f>ROUND(S4*0.1075, 2)</f>
+        <v>20.32</v>
+      </c>
+      <c r="V4" s="3">
+        <f>SUM(S4:U4)</f>
+        <v>209.37</v>
+      </c>
+      <c r="W4" s="3">
+        <f t="shared" ref="W4:W9" si="6">IF((R4&gt;0), V4/R4, I4)</f>
+        <v>11.019473684210526</v>
+      </c>
+      <c r="X4" s="3">
+        <f>J4*W4</f>
+        <v>11.019473684210526</v>
+      </c>
+      <c r="Y4" s="3">
+        <f>K4-X4</f>
+        <v>1.513157894734718E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -818,27 +910,27 @@
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="G5" s="4">
-        <f t="shared" ref="G5:G12" si="6">(C5+E5+F5)*0.1075</f>
+      <c r="G5" s="3">
+        <f t="shared" ref="G5:G12" si="7">(C5+E5+F5)*0.1075</f>
         <v>0.64392499999999997</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <f t="shared" si="0"/>
         <v>6.6339250000000005</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <f t="shared" si="1"/>
         <v>0.66339250000000005</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <f t="shared" si="2"/>
         <v>0.66339250000000005</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>8</v>
+      <c r="L5" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="M5">
         <f t="shared" si="3"/>
@@ -848,21 +940,50 @@
         <v>8</v>
       </c>
       <c r="O5">
-        <f t="shared" ref="O5:O12" si="7">MAX(0, M5-N5)</f>
+        <f t="shared" ref="O5:O12" si="8">MAX(0, M5-N5)</f>
         <v>12</v>
       </c>
       <c r="P5">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <f t="shared" si="5"/>
         <v>13.267850000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R5">
+        <v>20</v>
+      </c>
+      <c r="S5" s="1">
+        <v>12.58</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="3">
+        <f t="shared" ref="U5:U12" si="9">ROUND(S5*0.1075, 2)</f>
+        <v>1.35</v>
+      </c>
+      <c r="V5" s="3">
+        <f t="shared" ref="V5:V12" si="10">SUM(S5:U5)</f>
+        <v>13.93</v>
+      </c>
+      <c r="W5" s="3">
+        <f t="shared" si="6"/>
+        <v>0.69650000000000001</v>
+      </c>
+      <c r="X5" s="3">
+        <f t="shared" ref="X5:X12" si="11">J5*W5</f>
+        <v>0.69650000000000001</v>
+      </c>
+      <c r="Y5" s="3">
+        <f t="shared" ref="Y5:Y12" si="12">K5-X5</f>
+        <v>-3.3107499999999956E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C6" s="1">
         <v>7.99</v>
@@ -873,27 +994,27 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="G6" s="4">
-        <f t="shared" si="6"/>
+      <c r="G6" s="3">
+        <f t="shared" si="7"/>
         <v>0.85892500000000005</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <f t="shared" si="0"/>
         <v>8.8489249999999995</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <f t="shared" si="1"/>
         <v>0.17697849999999998</v>
       </c>
       <c r="J6">
         <v>3</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <f t="shared" si="2"/>
         <v>0.5309355</v>
       </c>
       <c r="L6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M6">
         <f t="shared" si="3"/>
@@ -903,21 +1024,50 @@
         <v>50</v>
       </c>
       <c r="O6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="P6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
         <f t="shared" si="5"/>
         <v>8.8489249999999995</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R6">
+        <v>50</v>
+      </c>
+      <c r="S6" s="1">
+        <v>7.99</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="3">
+        <f t="shared" si="9"/>
+        <v>0.86</v>
+      </c>
+      <c r="V6" s="3">
+        <f t="shared" si="10"/>
+        <v>8.85</v>
+      </c>
+      <c r="W6" s="3">
+        <f t="shared" si="6"/>
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="X6" s="3">
+        <f t="shared" si="11"/>
+        <v>0.53099999999999992</v>
+      </c>
+      <c r="Y6" s="3">
+        <f t="shared" si="12"/>
+        <v>-6.449999999991185E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1">
         <v>5.99</v>
@@ -928,27 +1078,27 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="G7" s="4">
-        <f t="shared" si="6"/>
+      <c r="G7" s="3">
+        <f t="shared" si="7"/>
         <v>0.64392499999999997</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <f t="shared" si="0"/>
         <v>6.6339250000000005</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <f t="shared" si="1"/>
         <v>4.4226166666666671E-2</v>
       </c>
       <c r="J7">
         <v>3</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <f t="shared" si="2"/>
         <v>0.1326785</v>
       </c>
       <c r="L7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M7">
         <f t="shared" si="3"/>
@@ -958,21 +1108,50 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>60</v>
       </c>
       <c r="P7">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <f t="shared" si="5"/>
         <v>6.6339250000000005</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R7">
+        <v>150</v>
+      </c>
+      <c r="S7" s="1">
+        <v>5.99</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="3">
+        <f t="shared" si="9"/>
+        <v>0.64</v>
+      </c>
+      <c r="V7" s="3">
+        <f t="shared" si="10"/>
+        <v>6.63</v>
+      </c>
+      <c r="W7" s="3">
+        <f t="shared" si="6"/>
+        <v>4.4199999999999996E-2</v>
+      </c>
+      <c r="X7" s="3">
+        <f t="shared" si="11"/>
+        <v>0.1326</v>
+      </c>
+      <c r="Y7" s="3">
+        <f t="shared" si="12"/>
+        <v>7.8500000000009118E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
         <v>18.989999999999998</v>
@@ -983,27 +1162,27 @@
       <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="G8" s="4">
-        <f t="shared" si="6"/>
+      <c r="G8" s="3">
+        <f t="shared" si="7"/>
         <v>2.0414249999999998</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <f t="shared" si="0"/>
         <v>21.031424999999999</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <f t="shared" si="1"/>
         <v>7.0104749999999996</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <f t="shared" si="2"/>
         <v>7.0104749999999996</v>
       </c>
       <c r="L8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M8">
         <f t="shared" si="3"/>
@@ -1013,21 +1192,50 @@
         <v>3</v>
       </c>
       <c r="O8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="P8">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8" s="3">
         <f t="shared" si="5"/>
         <v>126.18854999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R8">
+        <v>18</v>
+      </c>
+      <c r="S8" s="1">
+        <v>116.94</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="3">
+        <f t="shared" si="9"/>
+        <v>12.57</v>
+      </c>
+      <c r="V8" s="3">
+        <f t="shared" si="10"/>
+        <v>129.51</v>
+      </c>
+      <c r="W8" s="3">
+        <f t="shared" si="6"/>
+        <v>7.1949999999999994</v>
+      </c>
+      <c r="X8" s="3">
+        <f t="shared" si="11"/>
+        <v>7.1949999999999994</v>
+      </c>
+      <c r="Y8" s="3">
+        <f t="shared" si="12"/>
+        <v>-0.18452499999999983</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1">
         <v>12.99</v>
@@ -1038,27 +1246,27 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="G9" s="4">
-        <f t="shared" si="6"/>
+      <c r="G9" s="3">
+        <f t="shared" si="7"/>
         <v>1.396425</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <f t="shared" si="0"/>
         <v>14.386425000000001</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <f t="shared" si="1"/>
         <v>2.8772850000000001</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="3">
         <f t="shared" si="2"/>
         <v>2.8772850000000001</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>49</v>
+      <c r="L9" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="M9">
         <f t="shared" si="3"/>
@@ -1068,21 +1276,50 @@
         <v>6</v>
       </c>
       <c r="O9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="P9">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <f t="shared" si="5"/>
         <v>43.159275000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R9">
+        <v>15</v>
+      </c>
+      <c r="S9" s="1">
+        <v>37.47</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+      <c r="U9" s="3">
+        <f t="shared" si="9"/>
+        <v>4.03</v>
+      </c>
+      <c r="V9" s="3">
+        <f t="shared" si="10"/>
+        <v>41.5</v>
+      </c>
+      <c r="W9" s="3">
+        <f t="shared" si="6"/>
+        <v>2.7666666666666666</v>
+      </c>
+      <c r="X9" s="3">
+        <f t="shared" si="11"/>
+        <v>2.7666666666666666</v>
+      </c>
+      <c r="Y9" s="3">
+        <f t="shared" si="12"/>
+        <v>0.11061833333333349</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1">
         <v>14.49</v>
@@ -1093,27 +1330,27 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="G10" s="4">
-        <f t="shared" si="6"/>
+      <c r="G10" s="3">
+        <f t="shared" si="7"/>
         <v>1.5576749999999999</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <f t="shared" si="0"/>
         <v>16.047675000000002</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <f t="shared" si="1"/>
         <v>0.26746125000000004</v>
       </c>
       <c r="J10">
         <v>2</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <f t="shared" si="2"/>
         <v>0.53492250000000008</v>
       </c>
       <c r="L10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M10">
         <f t="shared" si="3"/>
@@ -1123,21 +1360,50 @@
         <v>60</v>
       </c>
       <c r="O10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
+      <c r="U10" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="V10" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W10" s="3">
+        <f>IF((R10&gt;0), V10/R10, I10)</f>
+        <v>0.26746125000000004</v>
+      </c>
+      <c r="X10" s="3">
+        <f t="shared" si="11"/>
+        <v>0.53492250000000008</v>
+      </c>
+      <c r="Y10" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1">
         <v>7.49</v>
@@ -1148,27 +1414,27 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="G11" s="4">
-        <f t="shared" si="6"/>
+      <c r="G11" s="3">
+        <f t="shared" si="7"/>
         <v>0.80517499999999997</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <f t="shared" si="0"/>
         <v>8.2951750000000004</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <f t="shared" si="1"/>
         <v>0.16590350000000001</v>
       </c>
       <c r="J11">
         <v>2</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <f t="shared" si="2"/>
         <v>0.33180700000000002</v>
       </c>
       <c r="L11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M11">
         <f t="shared" si="3"/>
@@ -1178,21 +1444,50 @@
         <v>50</v>
       </c>
       <c r="O11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0</v>
+      </c>
+      <c r="U11" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="3">
+        <f t="shared" ref="W11:W12" si="13">IF((R11&gt;0), V11/R11, I11)</f>
+        <v>0.16590350000000001</v>
+      </c>
+      <c r="X11" s="3">
+        <f t="shared" si="11"/>
+        <v>0.33180700000000002</v>
+      </c>
+      <c r="Y11" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1">
         <v>18.989999999999998</v>
@@ -1203,27 +1498,27 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="G12" s="4">
-        <f t="shared" si="6"/>
+      <c r="G12" s="3">
+        <f t="shared" si="7"/>
         <v>2.0414249999999998</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <f t="shared" si="0"/>
         <v>21.031424999999999</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <f t="shared" si="1"/>
         <v>4.2062849999999994</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="3">
         <f t="shared" si="2"/>
         <v>4.2062849999999994</v>
       </c>
       <c r="L12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M12">
         <f t="shared" si="3"/>
@@ -1233,81 +1528,142 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="P12">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12" s="3">
         <f t="shared" si="5"/>
         <v>84.125699999999995</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="7">
+      <c r="R12">
+        <v>20</v>
+      </c>
+      <c r="S12" s="1">
+        <v>79.959999999999994</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0</v>
+      </c>
+      <c r="U12" s="3">
+        <f t="shared" si="9"/>
+        <v>8.6</v>
+      </c>
+      <c r="V12" s="3">
+        <f t="shared" si="10"/>
+        <v>88.559999999999988</v>
+      </c>
+      <c r="W12" s="3">
+        <f t="shared" si="13"/>
+        <v>4.427999999999999</v>
+      </c>
+      <c r="X12" s="3">
+        <f t="shared" si="11"/>
+        <v>4.427999999999999</v>
+      </c>
+      <c r="Y12" s="3">
+        <f t="shared" si="12"/>
+        <v>-0.22171499999999966</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="6">
         <f>SUM(C4:C12)</f>
         <v>102.86999999999999</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="7">
+      <c r="G13" s="3"/>
+      <c r="H13" s="6">
         <f>SUM(H4:H12)</f>
         <v>113.92852499999999</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="12">
+      <c r="I13" s="3"/>
+      <c r="J13" s="10">
         <f>SUM(J4:J12)</f>
         <v>15</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="6">
         <f>SUM(K4:K12)</f>
         <v>27.307406</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="12">
-        <f t="shared" ref="M13:P13" si="8">SUM(M4:M12)</f>
+      <c r="L13" s="2"/>
+      <c r="M13" s="10">
+        <f t="shared" ref="M13:P13" si="14">SUM(M4:M12)</f>
         <v>300</v>
       </c>
-      <c r="N13" s="12">
-        <f t="shared" si="8"/>
+      <c r="N13" s="10">
+        <f t="shared" si="14"/>
         <v>178</v>
       </c>
-      <c r="O13" s="12">
-        <f t="shared" si="8"/>
+      <c r="O13" s="10">
+        <f t="shared" si="14"/>
         <v>152</v>
       </c>
-      <c r="P13" s="12">
-        <f t="shared" si="8"/>
+      <c r="P13" s="10">
+        <f t="shared" si="14"/>
         <v>36</v>
       </c>
-      <c r="Q13" s="7">
+      <c r="Q13" s="6">
         <f>SUM(Q4:Q12)</f>
         <v>491.59710000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="B14" s="5"/>
-      <c r="C14" s="7"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="3"/>
-      <c r="Q14" s="7"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A15" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R13" s="10">
+        <f t="shared" ref="R13:Y13" si="15">SUM(R4:R12)</f>
+        <v>292</v>
+      </c>
+      <c r="S13" s="6">
+        <f t="shared" si="15"/>
+        <v>449.98000000000008</v>
+      </c>
+      <c r="T13" s="6">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U13" s="6">
+        <f t="shared" si="15"/>
+        <v>48.370000000000005</v>
+      </c>
+      <c r="V13" s="6">
+        <f t="shared" si="15"/>
+        <v>498.34999999999997</v>
+      </c>
+      <c r="W13" s="6">
+        <f t="shared" si="15"/>
+        <v>26.760205100877187</v>
+      </c>
+      <c r="X13" s="6">
+        <f t="shared" si="15"/>
+        <v>27.635969850877196</v>
+      </c>
+      <c r="Y13" s="6">
+        <f t="shared" si="15"/>
+        <v>-0.32856385087719242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B14" s="4"/>
+      <c r="C14" s="6"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="2"/>
+      <c r="Q14" s="6"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A15" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1">
         <v>1.78</v>
@@ -1318,27 +1674,27 @@
       <c r="E16" s="1">
         <v>0</v>
       </c>
-      <c r="G16" s="4">
-        <f t="shared" ref="G16" si="9">(C16+E16+F16)*0.1075</f>
+      <c r="G16" s="3">
+        <f t="shared" ref="G16" si="16">(C16+E16+F16)*0.1075</f>
         <v>0.19134999999999999</v>
       </c>
-      <c r="H16" s="4">
-        <f t="shared" ref="H16" si="10">C16+E16+G16</f>
+      <c r="H16" s="3">
+        <f t="shared" ref="H16" si="17">C16+E16+G16</f>
         <v>1.9713499999999999</v>
       </c>
-      <c r="I16" s="4">
-        <f t="shared" ref="I16" si="11">H16/D16</f>
+      <c r="I16" s="3">
+        <f t="shared" ref="I16" si="18">H16/D16</f>
         <v>1.9713499999999999</v>
       </c>
       <c r="J16">
         <v>1</v>
       </c>
-      <c r="K16" s="4">
-        <f t="shared" ref="K16" si="12">I16*J16</f>
+      <c r="K16" s="3">
+        <f t="shared" ref="K16" si="19">I16*J16</f>
         <v>1.9713499999999999</v>
       </c>
-      <c r="L16" s="3" t="s">
-        <v>20</v>
+      <c r="L16" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="M16">
         <f>$D$1*J16</f>
@@ -1348,85 +1704,158 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <f t="shared" ref="O16" si="13">MAX(0, M16-N16)</f>
+        <f t="shared" ref="O16" si="20">MAX(0, M16-N16)</f>
         <v>20</v>
       </c>
       <c r="P16">
         <f>_xlfn.CEILING.MATH(O16/D16)</f>
         <v>20</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="Q16" s="3">
         <f>P16*H16</f>
         <v>39.427</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A17" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="7">
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16" s="3">
+        <f>S16*0.1075</f>
+        <v>0</v>
+      </c>
+      <c r="V16" s="3">
+        <f>SUM(S16:U16)</f>
+        <v>0</v>
+      </c>
+      <c r="W16" s="3">
+        <f t="shared" ref="W16" si="21">IF((R16&gt;0), V16/R16, I16)</f>
+        <v>1.9713499999999999</v>
+      </c>
+      <c r="X16" s="3">
+        <f>J16*W16</f>
+        <v>1.9713499999999999</v>
+      </c>
+      <c r="Y16" s="3">
+        <f>K16-X16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="6">
         <f>SUM(C16:C16)</f>
         <v>1.78</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="7">
+      <c r="D17" s="6">
+        <f t="shared" ref="D17:G17" si="22">SUM(D16:D16)</f>
+        <v>1</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="6">
+        <f t="shared" si="22"/>
+        <v>0.19134999999999999</v>
+      </c>
+      <c r="H17" s="6">
         <f>SUM(H16:H16)</f>
         <v>1.9713499999999999</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="12">
+      <c r="I17" s="6">
+        <f>SUM(I16:I16)</f>
+        <v>1.9713499999999999</v>
+      </c>
+      <c r="J17" s="10">
         <f>SUM(J16:J16)</f>
         <v>1</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="6">
         <f>SUM(K16:K16)</f>
         <v>1.9713499999999999</v>
       </c>
-      <c r="L17" s="3"/>
-      <c r="M17" s="12">
-        <f t="shared" ref="M17:P17" si="14">SUM(M16:M16)</f>
-        <v>20</v>
-      </c>
-      <c r="N17" s="12">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="12">
-        <f t="shared" si="14"/>
-        <v>20</v>
-      </c>
-      <c r="P17" s="12">
-        <f t="shared" si="14"/>
-        <v>20</v>
-      </c>
-      <c r="Q17" s="7">
+      <c r="L17" s="2"/>
+      <c r="M17" s="10">
+        <f t="shared" ref="M17:P17" si="23">SUM(M16:M16)</f>
+        <v>20</v>
+      </c>
+      <c r="N17" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="10">
+        <f t="shared" si="23"/>
+        <v>20</v>
+      </c>
+      <c r="P17" s="10">
+        <f t="shared" si="23"/>
+        <v>20</v>
+      </c>
+      <c r="Q17" s="6">
         <f>SUM(Q16:Q16)</f>
         <v>39.427</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R17" s="10">
+        <f>SUM(R16:R16)</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="6">
+        <f t="shared" ref="S17:Y17" si="24">SUM(S16:S16)</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="6">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U17" s="6">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V17" s="6">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W17" s="6">
+        <f t="shared" si="24"/>
+        <v>1.9713499999999999</v>
+      </c>
+      <c r="X17" s="6">
+        <f t="shared" si="24"/>
+        <v>1.9713499999999999</v>
+      </c>
+      <c r="Y17" s="6">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
       <c r="C18" s="1"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A19" s="5" t="s">
-        <v>38</v>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A19" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -1437,48 +1866,48 @@
       <c r="E20" s="1">
         <v>0</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <f>(C20+E20+F20)*0.1075</f>
         <v>0</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <f>C20+E20+G20</f>
         <v>0</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="3">
         <f>H20/D20</f>
         <v>0</v>
       </c>
       <c r="J20">
         <v>1</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="3">
         <f>I20*J20</f>
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" ref="M20:M23" si="15">$D$1*J20</f>
+        <f t="shared" ref="M20:M23" si="25">$D$1*J20</f>
         <v>20</v>
       </c>
       <c r="N20">
         <v>0</v>
       </c>
       <c r="O20">
-        <f t="shared" ref="O20:O23" si="16">MAX(0, M20-N20)</f>
+        <f t="shared" ref="O20:O23" si="26">MAX(0, M20-N20)</f>
         <v>20</v>
       </c>
       <c r="P20">
-        <f t="shared" ref="P20:P23" si="17">_xlfn.CEILING.MATH(O20/D20)</f>
-        <v>20</v>
-      </c>
-      <c r="Q20" s="4">
-        <f t="shared" ref="Q20:Q23" si="18">P20*H20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.4">
+        <f t="shared" ref="P20:P23" si="27">_xlfn.CEILING.MATH(O20/D20)</f>
+        <v>20</v>
+      </c>
+      <c r="Q20" s="3">
+        <f t="shared" ref="Q20:Q23" si="28">P20*H20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
@@ -1489,48 +1918,48 @@
       <c r="E21" s="1">
         <v>0</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <f>(C21+E21+F21)*0.1075</f>
         <v>0</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <f>C21+E21+G21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="3">
         <f>H21/D21</f>
         <v>0</v>
       </c>
       <c r="J21">
         <v>1</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="3">
         <f>I21*J21</f>
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="25"/>
         <v>20</v>
       </c>
       <c r="N21">
         <v>0</v>
       </c>
       <c r="O21">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="P21">
-        <f t="shared" si="17"/>
-        <v>20</v>
-      </c>
-      <c r="Q21" s="4">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.4">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="Q21" s="3">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
@@ -1541,48 +1970,48 @@
       <c r="E22" s="1">
         <v>0</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <f>(C22+E22+F22)*0.1075</f>
         <v>0</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="3">
         <f>C22+E22+G22</f>
         <v>0</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="3">
         <f>H22/D22</f>
         <v>0</v>
       </c>
       <c r="J22">
         <v>1</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="3">
         <f>I22*J22</f>
         <v>0</v>
       </c>
       <c r="M22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="25"/>
         <v>20</v>
       </c>
       <c r="N22">
         <v>0</v>
       </c>
       <c r="O22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="P22">
-        <f t="shared" si="17"/>
-        <v>20</v>
-      </c>
-      <c r="Q22" s="4">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.4">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="Q22" s="3">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
@@ -1593,113 +2022,113 @@
       <c r="E23" s="1">
         <v>0</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <f>(C23+E23+F23)*0.1075</f>
         <v>0</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="3">
         <f>C23+E23+G23</f>
         <v>0</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="3">
         <f>H23/D23</f>
         <v>0</v>
       </c>
       <c r="J23">
         <v>1</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="3">
         <f>I23*J23</f>
         <v>0</v>
       </c>
       <c r="M23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="25"/>
         <v>20</v>
       </c>
       <c r="N23">
         <v>0</v>
       </c>
       <c r="O23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="P23">
-        <f t="shared" si="17"/>
-        <v>20</v>
-      </c>
-      <c r="Q23" s="4">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="7">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="Q23" s="3">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="6">
         <f>SUM(C20:C23)</f>
         <v>0</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="7">
+      <c r="G24" s="3"/>
+      <c r="H24" s="6">
         <f>SUM(H20:H23)</f>
         <v>0</v>
       </c>
-      <c r="I24" s="4"/>
-      <c r="J24" s="12">
+      <c r="I24" s="3"/>
+      <c r="J24" s="10">
         <f>SUM(J20:J23)</f>
         <v>4</v>
       </c>
-      <c r="K24" s="7">
+      <c r="K24" s="6">
         <f>SUM(K20:K23)</f>
         <v>0</v>
       </c>
-      <c r="M24" s="12">
-        <f t="shared" ref="M24:P24" si="19">SUM(M20:M23)</f>
+      <c r="M24" s="10">
+        <f t="shared" ref="M24:P24" si="29">SUM(M20:M23)</f>
         <v>80</v>
       </c>
-      <c r="N24" s="12">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="O24" s="12">
-        <f t="shared" si="19"/>
+      <c r="N24" s="10">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="10">
+        <f t="shared" si="29"/>
         <v>80</v>
       </c>
-      <c r="P24" s="12">
-        <f t="shared" si="19"/>
+      <c r="P24" s="10">
+        <f t="shared" si="29"/>
         <v>80</v>
       </c>
-      <c r="Q24" s="7">
+      <c r="Q24" s="6">
         <f>SUM(Q20:Q23)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
       <c r="C25" s="1"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A26" s="5" t="s">
-        <v>35</v>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A26" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="K26" s="3"/>
       <c r="L26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" s="1">
         <v>0.53</v>
@@ -1710,52 +2139,81 @@
       <c r="E27" s="1">
         <v>0</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="3">
         <f>C27*0.1</f>
         <v>5.3000000000000005E-2</v>
       </c>
-      <c r="G27" s="4">
-        <f t="shared" ref="G27" si="20">(C27+E27+F27)*0.1075</f>
+      <c r="G27" s="3">
+        <f t="shared" ref="G27" si="30">(C27+E27+F27)*0.1075</f>
         <v>6.2672500000000006E-2</v>
       </c>
-      <c r="H27" s="4">
-        <f t="shared" ref="H27" si="21">C27+E27+G27</f>
+      <c r="H27" s="3">
+        <f t="shared" ref="H27" si="31">C27+E27+G27</f>
         <v>0.59267250000000005</v>
       </c>
-      <c r="I27" s="4">
-        <f t="shared" ref="I27" si="22">H27/D27</f>
+      <c r="I27" s="3">
+        <f t="shared" ref="I27" si="32">H27/D27</f>
         <v>0.59267250000000005</v>
       </c>
       <c r="J27">
         <v>1</v>
       </c>
-      <c r="K27" s="4">
-        <f t="shared" ref="K27" si="23">I27*J27</f>
+      <c r="K27" s="3">
+        <f t="shared" ref="K27" si="33">I27*J27</f>
         <v>0.59267250000000005</v>
       </c>
       <c r="M27">
-        <f t="shared" ref="M27:M44" si="24">$D$1*J27</f>
+        <f t="shared" ref="M27:M45" si="34">$D$1*J27</f>
         <v>20</v>
       </c>
       <c r="N27">
         <v>20</v>
       </c>
       <c r="O27">
-        <f t="shared" ref="O27:O44" si="25">MAX(0, M27-N27)</f>
+        <f t="shared" ref="O27:O45" si="35">MAX(0, M27-N27)</f>
         <v>0</v>
       </c>
       <c r="P27">
-        <f t="shared" ref="P27:P44" si="26">_xlfn.CEILING.MATH(O27/D27)</f>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="4">
-        <f t="shared" ref="Q27:Q44" si="27">P27*H27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.4">
+        <f t="shared" ref="P27:P44" si="36">_xlfn.CEILING.MATH(O27/D27)</f>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="3">
+        <f t="shared" ref="Q27:Q44" si="37">P27*H27</f>
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>10</v>
+      </c>
+      <c r="S27" s="1">
+        <v>4.45</v>
+      </c>
+      <c r="T27" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="U27" s="3">
+        <f>S27*0.1075</f>
+        <v>0.47837499999999999</v>
+      </c>
+      <c r="V27" s="3">
+        <f>SUM(S27:U27)</f>
+        <v>5.3783750000000001</v>
+      </c>
+      <c r="W27" s="3">
+        <f t="shared" ref="W27:W45" si="38">IF((R27&gt;0), V27/R27, I27)</f>
+        <v>0.53783749999999997</v>
+      </c>
+      <c r="X27" s="3">
+        <f>J27*W27</f>
+        <v>0.53783749999999997</v>
+      </c>
+      <c r="Y27" s="3">
+        <f>K27-X27</f>
+        <v>5.4835000000000078E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="1">
         <v>1.7</v>
@@ -1766,52 +2224,81 @@
       <c r="E28" s="1">
         <v>0</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="3">
         <f>C28*0.1</f>
         <v>0.17</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <f>(C28+E28+F28)*0.1075</f>
         <v>0.20102499999999998</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="3">
         <f>C28+E28+G28</f>
         <v>1.901025</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="3">
         <f>H28/D28</f>
         <v>0.95051249999999998</v>
       </c>
       <c r="J28">
         <v>2</v>
       </c>
-      <c r="K28" s="4">
+      <c r="K28" s="3">
         <f>I28*J28</f>
         <v>1.901025</v>
       </c>
       <c r="M28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>40</v>
       </c>
       <c r="N28">
         <v>0</v>
       </c>
       <c r="O28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>40</v>
       </c>
       <c r="P28">
-        <f t="shared" si="26"/>
-        <v>20</v>
-      </c>
-      <c r="Q28" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
+        <v>20</v>
+      </c>
+      <c r="Q28" s="3">
+        <f t="shared" si="37"/>
         <v>38.020499999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R28">
+        <v>50</v>
+      </c>
+      <c r="S28" s="1">
+        <v>15.53</v>
+      </c>
+      <c r="T28" s="1">
+        <v>1.55</v>
+      </c>
+      <c r="U28" s="3">
+        <f t="shared" ref="U28:U44" si="39">S28*0.1075</f>
+        <v>1.6694749999999998</v>
+      </c>
+      <c r="V28" s="3">
+        <f t="shared" ref="V28:V45" si="40">SUM(S28:U28)</f>
+        <v>18.749474999999997</v>
+      </c>
+      <c r="W28" s="3">
+        <f t="shared" si="38"/>
+        <v>0.37498949999999992</v>
+      </c>
+      <c r="X28" s="3">
+        <f t="shared" ref="X28:X45" si="41">J28*W28</f>
+        <v>0.74997899999999984</v>
+      </c>
+      <c r="Y28" s="3">
+        <f t="shared" ref="Y28:Y45" si="42">K28-X28</f>
+        <v>1.151046</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29" s="1">
         <v>0.81</v>
@@ -1822,51 +2309,78 @@
       <c r="E29" s="1">
         <v>0</v>
       </c>
-      <c r="F29" s="4">
-        <v>0</v>
-      </c>
-      <c r="G29" s="4">
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
         <f>(C29+E29+F29)*0.1075</f>
         <v>8.7075E-2</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29" s="3">
         <f>C29+E29+G29</f>
         <v>0.89707500000000007</v>
       </c>
-      <c r="I29" s="4">
+      <c r="I29" s="3">
         <f>H29/D29</f>
         <v>0.89707500000000007</v>
       </c>
       <c r="J29">
         <v>1</v>
       </c>
-      <c r="K29" s="4">
+      <c r="K29" s="3">
         <f>I29*J29</f>
         <v>0.89707500000000007</v>
       </c>
       <c r="M29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>20</v>
       </c>
       <c r="N29">
         <v>10</v>
       </c>
       <c r="O29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>10</v>
       </c>
       <c r="P29">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>10</v>
       </c>
-      <c r="Q29" s="4">
-        <f t="shared" si="27"/>
+      <c r="Q29" s="3">
+        <f t="shared" si="37"/>
         <v>8.9707500000000007</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R29">
+        <v>10</v>
+      </c>
+      <c r="S29" s="1">
+        <v>6.86</v>
+      </c>
+      <c r="T29" s="1"/>
+      <c r="U29" s="3">
+        <f t="shared" si="39"/>
+        <v>0.73745000000000005</v>
+      </c>
+      <c r="V29" s="3">
+        <f t="shared" si="40"/>
+        <v>7.5974500000000003</v>
+      </c>
+      <c r="W29" s="3">
+        <f t="shared" si="38"/>
+        <v>0.759745</v>
+      </c>
+      <c r="X29" s="3">
+        <f t="shared" si="41"/>
+        <v>0.759745</v>
+      </c>
+      <c r="Y29" s="3">
+        <f t="shared" si="42"/>
+        <v>0.13733000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C30" s="1">
         <v>1.38</v>
@@ -1877,52 +2391,81 @@
       <c r="E30" s="1">
         <v>0</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="3">
         <f>C33*0.1</f>
         <v>0.03</v>
       </c>
-      <c r="G30" s="4">
-        <f t="shared" ref="G30" si="28">(C30+E30+F30)*0.1075</f>
+      <c r="G30" s="3">
+        <f t="shared" ref="G30" si="43">(C30+E30+F30)*0.1075</f>
         <v>0.15157499999999999</v>
       </c>
-      <c r="H30" s="4">
-        <f t="shared" ref="H30" si="29">C30+E30+G30</f>
+      <c r="H30" s="3">
+        <f t="shared" ref="H30" si="44">C30+E30+G30</f>
         <v>1.5315749999999999</v>
       </c>
-      <c r="I30" s="4">
-        <f t="shared" ref="I30" si="30">H30/D30</f>
+      <c r="I30" s="3">
+        <f t="shared" ref="I30" si="45">H30/D30</f>
         <v>1.5315749999999999</v>
       </c>
       <c r="J30">
         <v>1</v>
       </c>
-      <c r="K30" s="4">
-        <f t="shared" ref="K30" si="31">I30*J30</f>
+      <c r="K30" s="3">
+        <f t="shared" ref="K30" si="46">I30*J30</f>
         <v>1.5315749999999999</v>
       </c>
       <c r="M30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>20</v>
       </c>
       <c r="N30">
         <v>10</v>
       </c>
       <c r="O30">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>10</v>
       </c>
       <c r="P30">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>10</v>
       </c>
-      <c r="Q30" s="4">
-        <f t="shared" si="27"/>
+      <c r="Q30" s="3">
+        <f t="shared" si="37"/>
         <v>15.31575</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R30">
+        <v>15</v>
+      </c>
+      <c r="S30" s="1">
+        <v>17.54</v>
+      </c>
+      <c r="T30" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="U30" s="3">
+        <f t="shared" si="39"/>
+        <v>1.8855499999999998</v>
+      </c>
+      <c r="V30" s="3">
+        <f t="shared" si="40"/>
+        <v>21.175549999999998</v>
+      </c>
+      <c r="W30" s="3">
+        <f t="shared" si="38"/>
+        <v>1.4117033333333331</v>
+      </c>
+      <c r="X30" s="3">
+        <f t="shared" si="41"/>
+        <v>1.4117033333333331</v>
+      </c>
+      <c r="Y30" s="3">
+        <f t="shared" si="42"/>
+        <v>0.11987166666666682</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1">
         <v>0.44</v>
@@ -1933,51 +2476,78 @@
       <c r="E31" s="1">
         <v>0</v>
       </c>
-      <c r="F31" s="4">
-        <v>0</v>
-      </c>
-      <c r="G31" s="4">
-        <f t="shared" ref="G31:G34" si="32">(C31+E31+F31)*0.1075</f>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <f t="shared" ref="G31:G34" si="47">(C31+E31+F31)*0.1075</f>
         <v>4.7300000000000002E-2</v>
       </c>
-      <c r="H31" s="4">
-        <f t="shared" ref="H31:H34" si="33">C31+E31+G31</f>
+      <c r="H31" s="3">
+        <f t="shared" ref="H31:H34" si="48">C31+E31+G31</f>
         <v>0.48730000000000001</v>
       </c>
-      <c r="I31" s="4">
-        <f t="shared" ref="I31:I34" si="34">H31/D31</f>
+      <c r="I31" s="3">
+        <f t="shared" ref="I31:I34" si="49">H31/D31</f>
         <v>0.48730000000000001</v>
       </c>
       <c r="J31">
         <v>1</v>
       </c>
-      <c r="K31" s="4">
-        <f t="shared" ref="K31:K34" si="35">I31*J31</f>
+      <c r="K31" s="3">
+        <f t="shared" ref="K31:K34" si="50">I31*J31</f>
         <v>0.48730000000000001</v>
       </c>
       <c r="M31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>20</v>
       </c>
       <c r="N31">
         <v>0</v>
       </c>
       <c r="O31">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>20</v>
       </c>
       <c r="P31">
-        <f t="shared" si="26"/>
-        <v>20</v>
-      </c>
-      <c r="Q31" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
+        <v>20</v>
+      </c>
+      <c r="Q31" s="3">
+        <f t="shared" si="37"/>
         <v>9.7460000000000004</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R31">
+        <v>20</v>
+      </c>
+      <c r="S31" s="1">
+        <v>6.66</v>
+      </c>
+      <c r="T31" s="1"/>
+      <c r="U31" s="3">
+        <f t="shared" si="39"/>
+        <v>0.71594999999999998</v>
+      </c>
+      <c r="V31" s="3">
+        <f t="shared" si="40"/>
+        <v>7.3759500000000005</v>
+      </c>
+      <c r="W31" s="3">
+        <f t="shared" si="38"/>
+        <v>0.3687975</v>
+      </c>
+      <c r="X31" s="3">
+        <f t="shared" si="41"/>
+        <v>0.3687975</v>
+      </c>
+      <c r="Y31" s="3">
+        <f t="shared" si="42"/>
+        <v>0.11850250000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C32" s="1">
         <v>0.1</v>
@@ -1988,51 +2558,78 @@
       <c r="E32" s="1">
         <v>0</v>
       </c>
-      <c r="F32" s="4">
-        <v>0</v>
-      </c>
-      <c r="G32" s="4">
-        <f t="shared" si="32"/>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <f t="shared" si="47"/>
         <v>1.0750000000000001E-2</v>
       </c>
-      <c r="H32" s="4">
-        <f t="shared" si="33"/>
+      <c r="H32" s="3">
+        <f t="shared" si="48"/>
         <v>0.11075</v>
       </c>
-      <c r="I32" s="4">
-        <f t="shared" si="34"/>
+      <c r="I32" s="3">
+        <f t="shared" si="49"/>
         <v>0.11075</v>
       </c>
       <c r="J32">
         <v>9</v>
       </c>
-      <c r="K32" s="4">
+      <c r="K32" s="3">
+        <f t="shared" si="50"/>
+        <v>0.99675000000000002</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="34"/>
+        <v>180</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
         <f t="shared" si="35"/>
-        <v>0.99675000000000002</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="24"/>
         <v>180</v>
       </c>
-      <c r="N32">
-        <v>0</v>
-      </c>
-      <c r="O32">
-        <f t="shared" si="25"/>
+      <c r="P32">
+        <f t="shared" si="36"/>
         <v>180</v>
       </c>
-      <c r="P32">
-        <f t="shared" si="26"/>
-        <v>180</v>
-      </c>
-      <c r="Q32" s="4">
-        <f t="shared" si="27"/>
+      <c r="Q32" s="3">
+        <f t="shared" si="37"/>
         <v>19.934999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="R32">
+        <v>250</v>
+      </c>
+      <c r="S32" s="1">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="T32" s="1"/>
+      <c r="U32" s="3">
+        <f t="shared" si="39"/>
+        <v>0.53964999999999996</v>
+      </c>
+      <c r="V32" s="3">
+        <f t="shared" si="40"/>
+        <v>5.5596499999999995</v>
+      </c>
+      <c r="W32" s="3">
+        <f t="shared" si="38"/>
+        <v>2.2238599999999997E-2</v>
+      </c>
+      <c r="X32" s="3">
+        <f t="shared" si="41"/>
+        <v>0.20014739999999998</v>
+      </c>
+      <c r="Y32" s="3">
+        <f t="shared" si="42"/>
+        <v>0.79660260000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C33" s="1">
         <v>0.3</v>
@@ -2043,51 +2640,78 @@
       <c r="E33" s="1">
         <v>0</v>
       </c>
-      <c r="F33" s="4">
-        <v>0</v>
-      </c>
-      <c r="G33" s="4">
-        <f t="shared" si="32"/>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
+        <f t="shared" si="47"/>
         <v>3.2250000000000001E-2</v>
       </c>
-      <c r="H33" s="4">
-        <f t="shared" si="33"/>
+      <c r="H33" s="3">
+        <f t="shared" si="48"/>
         <v>0.33224999999999999</v>
       </c>
-      <c r="I33" s="4">
-        <f t="shared" si="34"/>
+      <c r="I33" s="3">
+        <f t="shared" si="49"/>
         <v>0.11075</v>
       </c>
       <c r="J33">
         <v>2</v>
       </c>
-      <c r="K33" s="4">
+      <c r="K33" s="3">
+        <f t="shared" si="50"/>
+        <v>0.2215</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="34"/>
+        <v>40</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
         <f t="shared" si="35"/>
-        <v>0.2215</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="24"/>
         <v>40</v>
       </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
-      <c r="O33">
-        <f t="shared" si="25"/>
-        <v>40</v>
-      </c>
       <c r="P33">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>14</v>
       </c>
-      <c r="Q33" s="4">
-        <f t="shared" si="27"/>
+      <c r="Q33" s="3">
+        <f t="shared" si="37"/>
         <v>4.6514999999999995</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="R33">
+        <v>50</v>
+      </c>
+      <c r="S33" s="1">
+        <v>1.82</v>
+      </c>
+      <c r="T33" s="1"/>
+      <c r="U33" s="3">
+        <f t="shared" si="39"/>
+        <v>0.19564999999999999</v>
+      </c>
+      <c r="V33" s="3">
+        <f t="shared" si="40"/>
+        <v>2.0156499999999999</v>
+      </c>
+      <c r="W33" s="3">
+        <f t="shared" si="38"/>
+        <v>4.0313000000000002E-2</v>
+      </c>
+      <c r="X33" s="3">
+        <f t="shared" si="41"/>
+        <v>8.0626000000000003E-2</v>
+      </c>
+      <c r="Y33" s="3">
+        <f t="shared" si="42"/>
+        <v>0.140874</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C34" s="1">
         <v>0.5</v>
@@ -2098,51 +2722,78 @@
       <c r="E34" s="1">
         <v>0</v>
       </c>
-      <c r="F34" s="4">
-        <v>0</v>
-      </c>
-      <c r="G34" s="4">
-        <f t="shared" si="32"/>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <f t="shared" si="47"/>
         <v>5.3749999999999999E-2</v>
       </c>
-      <c r="H34" s="4">
-        <f t="shared" si="33"/>
+      <c r="H34" s="3">
+        <f t="shared" si="48"/>
         <v>0.55374999999999996</v>
       </c>
-      <c r="I34" s="4">
-        <f t="shared" si="34"/>
+      <c r="I34" s="3">
+        <f t="shared" si="49"/>
         <v>0.11074999999999999</v>
       </c>
       <c r="J34">
         <v>5</v>
       </c>
-      <c r="K34" s="4">
+      <c r="K34" s="3">
+        <f t="shared" si="50"/>
+        <v>0.55374999999999996</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="34"/>
+        <v>100</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
         <f t="shared" si="35"/>
-        <v>0.55374999999999996</v>
-      </c>
-      <c r="M34">
-        <f t="shared" si="24"/>
         <v>100</v>
       </c>
-      <c r="N34">
-        <v>0</v>
-      </c>
-      <c r="O34">
-        <f t="shared" si="25"/>
+      <c r="P34">
+        <f t="shared" si="36"/>
+        <v>20</v>
+      </c>
+      <c r="Q34" s="3">
+        <f t="shared" si="37"/>
+        <v>11.074999999999999</v>
+      </c>
+      <c r="R34">
         <v>100</v>
       </c>
-      <c r="P34">
-        <f t="shared" si="26"/>
-        <v>20</v>
-      </c>
-      <c r="Q34" s="4">
-        <f t="shared" si="27"/>
-        <v>11.074999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="S34" s="1">
+        <v>2.58</v>
+      </c>
+      <c r="T34" s="1"/>
+      <c r="U34" s="3">
+        <f t="shared" si="39"/>
+        <v>0.27734999999999999</v>
+      </c>
+      <c r="V34" s="3">
+        <f t="shared" si="40"/>
+        <v>2.8573500000000003</v>
+      </c>
+      <c r="W34" s="3">
+        <f t="shared" si="38"/>
+        <v>2.8573500000000002E-2</v>
+      </c>
+      <c r="X34" s="3">
+        <f t="shared" si="41"/>
+        <v>0.14286750000000001</v>
+      </c>
+      <c r="Y34" s="3">
+        <f t="shared" si="42"/>
+        <v>0.41088249999999993</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C35" s="1">
         <v>0.1</v>
@@ -2153,51 +2804,80 @@
       <c r="E35" s="1">
         <v>0</v>
       </c>
-      <c r="F35" s="4">
-        <v>0</v>
-      </c>
-      <c r="G35" s="4">
-        <f t="shared" ref="G35" si="36">(C35+E35+F35)*0.1075</f>
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3">
+        <f t="shared" ref="G35" si="51">(C35+E35+F35)*0.1075</f>
         <v>1.0750000000000001E-2</v>
       </c>
-      <c r="H35" s="4">
-        <f t="shared" ref="H35" si="37">C35+E35+G35</f>
+      <c r="H35" s="3">
+        <f t="shared" ref="H35" si="52">C35+E35+G35</f>
         <v>0.11075</v>
       </c>
-      <c r="I35" s="4">
-        <f t="shared" ref="I35" si="38">H35/D35</f>
+      <c r="I35" s="3">
+        <f t="shared" ref="I35" si="53">H35/D35</f>
         <v>0.11075</v>
       </c>
       <c r="J35">
         <v>5</v>
       </c>
-      <c r="K35" s="4">
-        <f t="shared" ref="K35" si="39">I35*J35</f>
+      <c r="K35" s="3">
+        <f t="shared" ref="K35" si="54">I35*J35</f>
         <v>0.55374999999999996</v>
       </c>
       <c r="M35">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>100</v>
       </c>
       <c r="N35">
         <v>0</v>
       </c>
       <c r="O35">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>100</v>
       </c>
       <c r="P35">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>100</v>
       </c>
-      <c r="Q35" s="4">
-        <f t="shared" si="27"/>
+      <c r="Q35" s="3">
+        <f t="shared" si="37"/>
         <v>11.074999999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="R35">
+        <v>25</v>
+      </c>
+      <c r="S35" s="1">
+        <v>1.59</v>
+      </c>
+      <c r="T35" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="U35" s="3">
+        <f t="shared" si="39"/>
+        <v>0.17092499999999999</v>
+      </c>
+      <c r="V35" s="3">
+        <f t="shared" si="40"/>
+        <v>1.920925</v>
+      </c>
+      <c r="W35" s="3">
+        <f t="shared" si="38"/>
+        <v>7.6837000000000003E-2</v>
+      </c>
+      <c r="X35" s="3">
+        <f t="shared" si="41"/>
+        <v>0.384185</v>
+      </c>
+      <c r="Y35" s="3">
+        <f t="shared" si="42"/>
+        <v>0.16956499999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C36" s="1">
         <v>0.1</v>
@@ -2208,51 +2888,80 @@
       <c r="E36" s="1">
         <v>0</v>
       </c>
-      <c r="F36" s="4">
-        <v>0</v>
-      </c>
-      <c r="G36" s="4">
-        <f t="shared" ref="G36" si="40">(C36+E36+F36)*0.1075</f>
+      <c r="F36" s="3">
+        <v>0</v>
+      </c>
+      <c r="G36" s="3">
+        <f t="shared" ref="G36" si="55">(C36+E36+F36)*0.1075</f>
         <v>1.0750000000000001E-2</v>
       </c>
-      <c r="H36" s="4">
-        <f t="shared" ref="H36" si="41">C36+E36+G36</f>
+      <c r="H36" s="3">
+        <f t="shared" ref="H36" si="56">C36+E36+G36</f>
         <v>0.11075</v>
       </c>
-      <c r="I36" s="4">
-        <f t="shared" ref="I36" si="42">H36/D36</f>
+      <c r="I36" s="3">
+        <f t="shared" ref="I36" si="57">H36/D36</f>
         <v>0.11075</v>
       </c>
       <c r="J36">
         <v>5</v>
       </c>
-      <c r="K36" s="4">
-        <f t="shared" ref="K36" si="43">I36*J36</f>
+      <c r="K36" s="3">
+        <f t="shared" ref="K36" si="58">I36*J36</f>
         <v>0.55374999999999996</v>
       </c>
       <c r="M36">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>100</v>
       </c>
       <c r="N36">
         <v>0</v>
       </c>
       <c r="O36">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>100</v>
       </c>
       <c r="P36">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>100</v>
       </c>
-      <c r="Q36" s="4">
-        <f t="shared" si="27"/>
+      <c r="Q36" s="3">
+        <f t="shared" si="37"/>
         <v>11.074999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="R36">
+        <v>25</v>
+      </c>
+      <c r="S36" s="1">
+        <v>1.59</v>
+      </c>
+      <c r="T36" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="U36" s="3">
+        <f t="shared" si="39"/>
+        <v>0.17092499999999999</v>
+      </c>
+      <c r="V36" s="3">
+        <f t="shared" si="40"/>
+        <v>1.920925</v>
+      </c>
+      <c r="W36" s="3">
+        <f t="shared" si="38"/>
+        <v>7.6837000000000003E-2</v>
+      </c>
+      <c r="X36" s="3">
+        <f t="shared" si="41"/>
+        <v>0.384185</v>
+      </c>
+      <c r="Y36" s="3">
+        <f t="shared" si="42"/>
+        <v>0.16956499999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C37" s="1">
         <v>0.13</v>
@@ -2263,53 +2972,82 @@
       <c r="E37" s="1">
         <v>0</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="3">
         <f>C37*0.1</f>
         <v>1.3000000000000001E-2</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="3">
         <f>(C37+E37+F37)*0.1075</f>
         <v>1.5372500000000001E-2</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="3">
         <f>C37+E37+G37</f>
         <v>0.14537250000000002</v>
       </c>
-      <c r="I37" s="4">
+      <c r="I37" s="3">
         <f>H37/D37</f>
         <v>0.14537250000000002</v>
       </c>
       <c r="J37">
         <v>1</v>
       </c>
-      <c r="K37" s="4">
+      <c r="K37" s="3">
         <f>I37*J37</f>
         <v>0.14537250000000002</v>
       </c>
-      <c r="L37" s="3"/>
+      <c r="L37" s="2"/>
       <c r="M37">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>20</v>
       </c>
       <c r="N37">
         <v>10</v>
       </c>
       <c r="O37">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>10</v>
       </c>
       <c r="P37">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>10</v>
       </c>
-      <c r="Q37" s="4">
-        <f t="shared" si="27"/>
+      <c r="Q37" s="3">
+        <f t="shared" si="37"/>
         <v>1.4537250000000002</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="R37">
+        <v>25</v>
+      </c>
+      <c r="S37" s="1">
+        <v>2.99</v>
+      </c>
+      <c r="T37" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="U37" s="3">
+        <f t="shared" si="39"/>
+        <v>0.32142500000000002</v>
+      </c>
+      <c r="V37" s="3">
+        <f t="shared" si="40"/>
+        <v>3.6114250000000001</v>
+      </c>
+      <c r="W37" s="3">
+        <f t="shared" si="38"/>
+        <v>0.144457</v>
+      </c>
+      <c r="X37" s="3">
+        <f t="shared" si="41"/>
+        <v>0.144457</v>
+      </c>
+      <c r="Y37" s="3">
+        <f t="shared" si="42"/>
+        <v>9.1550000000001353E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C38" s="1">
         <v>1.56</v>
@@ -2320,51 +3058,78 @@
       <c r="E38" s="1">
         <v>0</v>
       </c>
-      <c r="F38" s="4">
-        <v>0</v>
-      </c>
-      <c r="G38" s="4">
+      <c r="F38" s="3">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
         <f>(C38+E38+F38)*0.1075</f>
         <v>0.16770000000000002</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="3">
         <f>C38+E38+G38</f>
         <v>1.7277</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38" s="3">
         <f>H38/D38</f>
         <v>0.86385000000000001</v>
       </c>
       <c r="J38">
         <v>2</v>
       </c>
-      <c r="K38" s="4">
+      <c r="K38" s="3">
         <f>I38*J38</f>
         <v>1.7277</v>
       </c>
       <c r="M38">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>40</v>
       </c>
       <c r="N38">
         <v>50</v>
       </c>
       <c r="O38">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="P38">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="Q38" s="4">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.4">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="3">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38" s="1">
+        <v>0</v>
+      </c>
+      <c r="T38" s="1"/>
+      <c r="U38" s="3">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="V38" s="3">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="W38" s="3">
+        <f t="shared" si="38"/>
+        <v>0.86385000000000001</v>
+      </c>
+      <c r="X38" s="3">
+        <f t="shared" si="41"/>
+        <v>1.7277</v>
+      </c>
+      <c r="Y38" s="3">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C39" s="1">
         <v>1.3</v>
@@ -2375,52 +3140,79 @@
       <c r="E39" s="1">
         <v>0</v>
       </c>
-      <c r="F39" s="4">
-        <v>0</v>
-      </c>
-      <c r="G39" s="4">
-        <f t="shared" ref="G39" si="44">(C39+E39+F39)*0.1075</f>
+      <c r="F39" s="3">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" ref="G39" si="59">(C39+E39+F39)*0.1075</f>
         <v>0.13975000000000001</v>
       </c>
-      <c r="H39" s="4">
-        <f t="shared" ref="H39" si="45">C39+E39+G39</f>
+      <c r="H39" s="3">
+        <f t="shared" ref="H39" si="60">C39+E39+G39</f>
         <v>1.4397500000000001</v>
       </c>
-      <c r="I39" s="4">
-        <f t="shared" ref="I39" si="46">H39/D39</f>
+      <c r="I39" s="3">
+        <f t="shared" ref="I39" si="61">H39/D39</f>
         <v>0.71987500000000004</v>
       </c>
       <c r="J39">
         <v>2</v>
       </c>
-      <c r="K39" s="4">
-        <f t="shared" ref="K39" si="47">I39*J39</f>
+      <c r="K39" s="3">
+        <f t="shared" ref="K39" si="62">I39*J39</f>
         <v>1.4397500000000001</v>
       </c>
-      <c r="L39" s="3"/>
+      <c r="L39" s="2"/>
       <c r="M39">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>40</v>
       </c>
       <c r="N39">
         <v>0</v>
       </c>
       <c r="O39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>40</v>
       </c>
       <c r="P39">
-        <f t="shared" si="26"/>
-        <v>20</v>
-      </c>
-      <c r="Q39" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
+        <v>20</v>
+      </c>
+      <c r="Q39" s="3">
+        <f t="shared" si="37"/>
         <v>28.795000000000002</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="R39">
+        <v>40</v>
+      </c>
+      <c r="S39" s="1">
+        <v>22.6</v>
+      </c>
+      <c r="T39" s="1"/>
+      <c r="U39" s="3">
+        <f t="shared" si="39"/>
+        <v>2.4295</v>
+      </c>
+      <c r="V39" s="3">
+        <f t="shared" si="40"/>
+        <v>25.029500000000002</v>
+      </c>
+      <c r="W39" s="3">
+        <f t="shared" si="38"/>
+        <v>0.62573750000000006</v>
+      </c>
+      <c r="X39" s="3">
+        <f t="shared" si="41"/>
+        <v>1.2514750000000001</v>
+      </c>
+      <c r="Y39" s="3">
+        <f t="shared" si="42"/>
+        <v>0.18827499999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C40" s="1">
         <v>0.47</v>
@@ -2431,52 +3223,79 @@
       <c r="E40" s="1">
         <v>0</v>
       </c>
-      <c r="F40" s="4">
-        <v>0</v>
-      </c>
-      <c r="G40" s="4">
-        <f t="shared" ref="G40" si="48">(C40+E40+F40)*0.1075</f>
+      <c r="F40" s="3">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
+        <f t="shared" ref="G40" si="63">(C40+E40+F40)*0.1075</f>
         <v>5.0524999999999994E-2</v>
       </c>
-      <c r="H40" s="4">
-        <f t="shared" ref="H40" si="49">C40+E40+G40</f>
+      <c r="H40" s="3">
+        <f t="shared" ref="H40" si="64">C40+E40+G40</f>
         <v>0.52052500000000002</v>
       </c>
-      <c r="I40" s="4">
-        <f t="shared" ref="I40" si="50">H40/D40</f>
+      <c r="I40" s="3">
+        <f t="shared" ref="I40" si="65">H40/D40</f>
         <v>0.52052500000000002</v>
       </c>
       <c r="J40">
         <v>1</v>
       </c>
-      <c r="K40" s="4">
-        <f t="shared" ref="K40" si="51">I40*J40</f>
+      <c r="K40" s="3">
+        <f t="shared" ref="K40" si="66">I40*J40</f>
         <v>0.52052500000000002</v>
       </c>
-      <c r="L40" s="3"/>
+      <c r="L40" s="2"/>
       <c r="M40">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>20</v>
       </c>
       <c r="N40">
         <v>0</v>
       </c>
       <c r="O40">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>20</v>
       </c>
       <c r="P40">
-        <f t="shared" si="26"/>
-        <v>20</v>
-      </c>
-      <c r="Q40" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
+        <v>20</v>
+      </c>
+      <c r="Q40" s="3">
+        <f t="shared" si="37"/>
         <v>10.410500000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="R40">
+        <v>20</v>
+      </c>
+      <c r="S40" s="1">
+        <v>8.24</v>
+      </c>
+      <c r="T40" s="1"/>
+      <c r="U40" s="3">
+        <f t="shared" si="39"/>
+        <v>0.88580000000000003</v>
+      </c>
+      <c r="V40" s="3">
+        <f t="shared" si="40"/>
+        <v>9.1257999999999999</v>
+      </c>
+      <c r="W40" s="3">
+        <f t="shared" si="38"/>
+        <v>0.45628999999999997</v>
+      </c>
+      <c r="X40" s="3">
+        <f t="shared" si="41"/>
+        <v>0.45628999999999997</v>
+      </c>
+      <c r="Y40" s="3">
+        <f t="shared" si="42"/>
+        <v>6.4235000000000042E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C41" s="1">
         <v>0.1</v>
@@ -2487,52 +3306,79 @@
       <c r="E41" s="1">
         <v>0</v>
       </c>
-      <c r="F41" s="4">
-        <v>0</v>
-      </c>
-      <c r="G41" s="4">
-        <f t="shared" ref="G41:G42" si="52">(C41+E41+F41)*0.1075</f>
+      <c r="F41" s="3">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3">
+        <f t="shared" ref="G41:G42" si="67">(C41+E41+F41)*0.1075</f>
         <v>1.0750000000000001E-2</v>
       </c>
-      <c r="H41" s="4">
-        <f t="shared" ref="H41:H42" si="53">C41+E41+G41</f>
+      <c r="H41" s="3">
+        <f t="shared" ref="H41:H42" si="68">C41+E41+G41</f>
         <v>0.11075</v>
       </c>
-      <c r="I41" s="4">
-        <f t="shared" ref="I41:I42" si="54">H41/D41</f>
+      <c r="I41" s="3">
+        <f t="shared" ref="I41:I42" si="69">H41/D41</f>
         <v>0.11075</v>
       </c>
       <c r="J41">
         <v>1</v>
       </c>
-      <c r="K41" s="4">
-        <f t="shared" ref="K41:K42" si="55">I41*J41</f>
+      <c r="K41" s="3">
+        <f t="shared" ref="K41:K42" si="70">I41*J41</f>
         <v>0.11075</v>
       </c>
-      <c r="L41" s="3"/>
+      <c r="L41" s="2"/>
       <c r="M41">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>20</v>
       </c>
       <c r="N41">
         <v>10</v>
       </c>
       <c r="O41">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>10</v>
       </c>
       <c r="P41">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>10</v>
       </c>
-      <c r="Q41" s="4">
-        <f t="shared" si="27"/>
+      <c r="Q41" s="3">
+        <f t="shared" si="37"/>
         <v>1.1074999999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="R41">
+        <v>25</v>
+      </c>
+      <c r="S41" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="T41" s="1"/>
+      <c r="U41" s="3">
+        <f t="shared" si="39"/>
+        <v>0.10965</v>
+      </c>
+      <c r="V41" s="3">
+        <f t="shared" si="40"/>
+        <v>1.12965</v>
+      </c>
+      <c r="W41" s="3">
+        <f t="shared" si="38"/>
+        <v>4.5186000000000004E-2</v>
+      </c>
+      <c r="X41" s="3">
+        <f t="shared" si="41"/>
+        <v>4.5186000000000004E-2</v>
+      </c>
+      <c r="Y41" s="3">
+        <f t="shared" si="42"/>
+        <v>6.5563999999999997E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C42" s="1">
         <v>2.14</v>
@@ -2543,51 +3389,80 @@
       <c r="E42" s="1">
         <v>0</v>
       </c>
-      <c r="F42" s="4">
-        <v>0</v>
-      </c>
-      <c r="G42" s="4">
-        <f t="shared" si="52"/>
+      <c r="F42" s="3">
+        <v>0</v>
+      </c>
+      <c r="G42" s="3">
+        <f t="shared" si="67"/>
         <v>0.23005</v>
       </c>
-      <c r="H42" s="4">
-        <f t="shared" si="53"/>
+      <c r="H42" s="3">
+        <f t="shared" si="68"/>
         <v>2.37005</v>
       </c>
-      <c r="I42" s="4">
-        <f t="shared" si="54"/>
+      <c r="I42" s="3">
+        <f t="shared" si="69"/>
         <v>0.23700499999999999</v>
       </c>
       <c r="J42">
         <v>10</v>
       </c>
-      <c r="K42" s="4">
-        <f t="shared" si="55"/>
+      <c r="K42" s="3">
+        <f t="shared" si="70"/>
         <v>2.37005</v>
       </c>
       <c r="M42">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>200</v>
       </c>
       <c r="N42">
         <v>0</v>
       </c>
       <c r="O42">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>200</v>
       </c>
       <c r="P42">
-        <f t="shared" si="26"/>
-        <v>20</v>
-      </c>
-      <c r="Q42" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
+        <v>20</v>
+      </c>
+      <c r="Q42" s="3">
+        <f t="shared" si="37"/>
         <v>47.400999999999996</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="R42">
+        <v>200</v>
+      </c>
+      <c r="S42" s="1">
+        <v>22.7</v>
+      </c>
+      <c r="T42" s="1">
+        <v>2.27</v>
+      </c>
+      <c r="U42" s="3">
+        <f t="shared" si="39"/>
+        <v>2.4402499999999998</v>
+      </c>
+      <c r="V42" s="3">
+        <f t="shared" si="40"/>
+        <v>27.410249999999998</v>
+      </c>
+      <c r="W42" s="3">
+        <f t="shared" si="38"/>
+        <v>0.13705124999999999</v>
+      </c>
+      <c r="X42" s="3">
+        <f t="shared" si="41"/>
+        <v>1.3705124999999998</v>
+      </c>
+      <c r="Y42" s="3">
+        <f t="shared" si="42"/>
+        <v>0.99953750000000019</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C43" s="1">
         <v>1.1499999999999999</v>
@@ -2598,51 +3473,80 @@
       <c r="E43" s="1">
         <v>0</v>
       </c>
-      <c r="F43" s="4">
-        <v>0</v>
-      </c>
-      <c r="G43" s="4">
-        <f t="shared" ref="G43" si="56">(C43+E43+F43)*0.1075</f>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
+        <f t="shared" ref="G43" si="71">(C43+E43+F43)*0.1075</f>
         <v>0.12362499999999998</v>
       </c>
-      <c r="H43" s="4">
-        <f t="shared" ref="H43" si="57">C43+E43+G43</f>
+      <c r="H43" s="3">
+        <f t="shared" ref="H43" si="72">C43+E43+G43</f>
         <v>1.273625</v>
       </c>
-      <c r="I43" s="4">
-        <f t="shared" ref="I43" si="58">H43/D43</f>
+      <c r="I43" s="3">
+        <f t="shared" ref="I43" si="73">H43/D43</f>
         <v>0.25472499999999998</v>
       </c>
       <c r="J43">
         <v>5</v>
       </c>
-      <c r="K43" s="4">
-        <f t="shared" ref="K43" si="59">I43*J43</f>
+      <c r="K43" s="3">
+        <f t="shared" ref="K43" si="74">I43*J43</f>
         <v>1.273625</v>
       </c>
       <c r="M43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>100</v>
       </c>
       <c r="N43">
         <v>10</v>
       </c>
       <c r="O43">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>90</v>
       </c>
       <c r="P43">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>18</v>
       </c>
-      <c r="Q43" s="4">
-        <f t="shared" si="27"/>
+      <c r="Q43" s="3">
+        <f t="shared" si="37"/>
         <v>22.925249999999998</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="R43">
+        <v>110</v>
+      </c>
+      <c r="S43" s="1">
+        <v>8.73</v>
+      </c>
+      <c r="T43" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="U43" s="3">
+        <f t="shared" si="39"/>
+        <v>0.93847500000000006</v>
+      </c>
+      <c r="V43" s="3">
+        <f t="shared" si="40"/>
+        <v>10.538475</v>
+      </c>
+      <c r="W43" s="3">
+        <f t="shared" si="38"/>
+        <v>9.5804318181818185E-2</v>
+      </c>
+      <c r="X43" s="3">
+        <f t="shared" si="41"/>
+        <v>0.47902159090909091</v>
+      </c>
+      <c r="Y43" s="3">
+        <f t="shared" si="42"/>
+        <v>0.7946034090909091</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C44" s="1">
         <v>1.42</v>
@@ -2653,277 +3557,556 @@
       <c r="E44" s="1">
         <v>0</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F44" s="3">
         <f>C44*0.1</f>
         <v>0.14199999999999999</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44" s="3">
         <f>(C44+E44+F44)*0.1075</f>
         <v>0.16791499999999998</v>
       </c>
-      <c r="H44" s="4">
+      <c r="H44" s="3">
         <f>C44+E44+G44</f>
         <v>1.587915</v>
       </c>
-      <c r="I44" s="4">
+      <c r="I44" s="3">
         <f>H44/D44</f>
         <v>0.79395749999999998</v>
       </c>
       <c r="J44">
         <v>2</v>
       </c>
-      <c r="K44" s="4">
+      <c r="K44" s="3">
         <f>I44*J44</f>
         <v>1.587915</v>
       </c>
-      <c r="L44" s="3"/>
+      <c r="L44" s="2"/>
       <c r="M44">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>40</v>
       </c>
       <c r="N44">
         <v>0</v>
       </c>
       <c r="O44">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>40</v>
       </c>
       <c r="P44">
-        <f t="shared" si="26"/>
-        <v>20</v>
-      </c>
-      <c r="Q44" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
+        <v>20</v>
+      </c>
+      <c r="Q44" s="3">
+        <f t="shared" si="37"/>
         <v>31.758299999999998</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" s="7">
-        <f>SUM(C27:C44)</f>
+      <c r="R44">
+        <v>50</v>
+      </c>
+      <c r="S44" s="1">
+        <v>28.3</v>
+      </c>
+      <c r="T44" s="1"/>
+      <c r="U44" s="3">
+        <f t="shared" si="39"/>
+        <v>3.0422500000000001</v>
+      </c>
+      <c r="V44" s="3">
+        <f t="shared" si="40"/>
+        <v>31.34225</v>
+      </c>
+      <c r="W44" s="3">
+        <f t="shared" si="38"/>
+        <v>0.62684499999999999</v>
+      </c>
+      <c r="X44" s="3">
+        <f t="shared" si="41"/>
+        <v>1.25369</v>
+      </c>
+      <c r="Y44" s="3">
+        <f t="shared" si="42"/>
+        <v>0.33422499999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B45" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1">
+        <v>4.99</v>
+      </c>
+      <c r="F45" s="3">
+        <f>C45*0.1</f>
+        <v>0</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0</v>
+      </c>
+      <c r="H45" s="3">
+        <f>C45+E45+G45</f>
+        <v>4.99</v>
+      </c>
+      <c r="I45" s="3">
+        <f>H45/D45</f>
+        <v>4.99</v>
+      </c>
+      <c r="J45">
+        <f>1/$D$1</f>
+        <v>0.05</v>
+      </c>
+      <c r="K45" s="3">
+        <f>I45*J45</f>
+        <v>0.24950000000000003</v>
+      </c>
+      <c r="L45" s="2"/>
+      <c r="M45">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+      <c r="P45">
+        <f t="shared" ref="P45" si="75">_xlfn.CEILING.MATH(O45/D45)</f>
+        <v>1</v>
+      </c>
+      <c r="Q45" s="3">
+        <f t="shared" ref="Q45" si="76">P45*H45</f>
+        <v>4.99</v>
+      </c>
+      <c r="R45">
+        <v>1</v>
+      </c>
+      <c r="S45" s="1">
+        <v>6.99</v>
+      </c>
+      <c r="T45" s="1">
+        <v>0</v>
+      </c>
+      <c r="U45" s="1">
+        <v>0</v>
+      </c>
+      <c r="V45" s="3">
+        <f t="shared" si="40"/>
+        <v>6.99</v>
+      </c>
+      <c r="W45" s="3">
+        <f t="shared" si="38"/>
+        <v>6.99</v>
+      </c>
+      <c r="X45" s="3">
+        <f>W45/$D$1</f>
+        <v>0.34950000000000003</v>
+      </c>
+      <c r="Y45" s="3">
+        <f t="shared" si="42"/>
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" s="6">
+        <f>SUM(C27:C45)</f>
         <v>14.23</v>
       </c>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="7">
+      <c r="E46" s="6">
+        <f>SUM(E27:E45)</f>
+        <v>4.99</v>
+      </c>
+      <c r="F46" s="6">
+        <f>SUM(F27:F44)</f>
+        <v>0.40800000000000003</v>
+      </c>
+      <c r="G46" s="6">
+        <f>SUM(G27:G44)</f>
+        <v>1.5735850000000002</v>
+      </c>
+      <c r="H46" s="6">
         <f>SUM(H27:H44)</f>
         <v>15.803585</v>
       </c>
-      <c r="I45" s="8"/>
-      <c r="J45" s="5">
-        <f>SUM(J27:J44)</f>
+      <c r="I46" s="6">
+        <f>SUM(I27:I45)</f>
+        <v>13.648945000000003</v>
+      </c>
+      <c r="J46" s="4">
+        <f>TRUNC(SUM(J27:J45))</f>
         <v>56</v>
       </c>
-      <c r="K45" s="10">
+      <c r="K46" s="8">
         <f>SUM(K27:K44)</f>
         <v>17.464834999999997</v>
       </c>
-      <c r="L45" s="9"/>
-      <c r="M45" s="5">
-        <f t="shared" ref="M45:P45" si="60">SUM(M27:M44)</f>
-        <v>1120</v>
-      </c>
-      <c r="N45" s="5">
-        <f t="shared" si="60"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="4">
+        <f>SUM(M27:M45)</f>
+        <v>1121</v>
+      </c>
+      <c r="N46" s="4">
+        <f>SUM(N27:N45)</f>
         <v>120</v>
       </c>
-      <c r="O45" s="5">
-        <f t="shared" si="60"/>
+      <c r="O46" s="4">
+        <f t="shared" ref="M46:P46" si="77">SUM(O27:O44)</f>
         <v>1010</v>
       </c>
-      <c r="P45" s="5">
-        <f t="shared" si="60"/>
+      <c r="P46" s="4">
+        <f t="shared" si="77"/>
         <v>592</v>
       </c>
-      <c r="Q45" s="10">
+      <c r="Q46" s="8">
         <f>SUM(Q27:Q44)</f>
         <v>273.71577500000001</v>
       </c>
-      <c r="S45" s="1">
-        <v>218.6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="B46" s="5"/>
-      <c r="C46" s="1"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="3"/>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A47" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="R46" s="4">
+        <f>SUM(R27:R45)</f>
+        <v>1026</v>
+      </c>
+      <c r="S46" s="6">
+        <f t="shared" ref="S46:Y46" si="78">SUM(S27:S45)</f>
+        <v>165.21</v>
+      </c>
+      <c r="T46" s="6">
+        <f t="shared" si="78"/>
+        <v>7.5100000000000007</v>
+      </c>
+      <c r="U46" s="6">
+        <f t="shared" si="78"/>
+        <v>17.008649999999999</v>
+      </c>
+      <c r="V46" s="6">
+        <f t="shared" si="78"/>
+        <v>189.72864999999999</v>
+      </c>
+      <c r="W46" s="6">
+        <f t="shared" si="78"/>
+        <v>13.68309300151515</v>
+      </c>
+      <c r="X46" s="6">
+        <f t="shared" si="78"/>
+        <v>12.097905324242422</v>
+      </c>
+      <c r="Y46" s="6">
+        <f t="shared" si="78"/>
+        <v>5.6164296757575771</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B47" s="4"/>
       <c r="C47" s="1"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="3"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="B48" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C48" s="1">
+      <c r="I47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A48" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B49" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="1">
         <v>30.66</v>
       </c>
-      <c r="D48">
+      <c r="D49">
         <f>$D$1</f>
         <v>20</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E49" s="1">
         <v>29.89</v>
       </c>
-      <c r="F48" s="4">
-        <v>0</v>
-      </c>
-      <c r="G48" s="4">
-        <v>0</v>
-      </c>
-      <c r="H48" s="4">
-        <f t="shared" ref="H48" si="61">C48+E48+G48</f>
+      <c r="F49" s="3">
+        <v>0</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3">
+        <f t="shared" ref="H49" si="79">C49+E49+G49</f>
         <v>60.55</v>
       </c>
-      <c r="I48" s="4">
-        <f t="shared" ref="I48" si="62">H48/D48</f>
+      <c r="I49" s="3">
+        <f t="shared" ref="I49" si="80">H49/D49</f>
         <v>3.0274999999999999</v>
       </c>
-      <c r="J48">
-        <v>1</v>
-      </c>
-      <c r="K48" s="4">
-        <f t="shared" ref="K48" si="63">I48*J48</f>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49" s="3">
+        <f t="shared" ref="K49" si="81">I49*J49</f>
         <v>3.0274999999999999</v>
       </c>
-      <c r="L48" s="3"/>
-      <c r="M48">
-        <f>$D$1*J48</f>
-        <v>20</v>
-      </c>
-      <c r="N48">
-        <v>0</v>
-      </c>
-      <c r="O48">
-        <f>MAX(0, M48-N48)</f>
-        <v>20</v>
-      </c>
-      <c r="P48">
-        <f>_xlfn.CEILING.MATH(O48/D48)</f>
-        <v>1</v>
-      </c>
-      <c r="Q48" s="4">
-        <f>P48*H48</f>
+      <c r="L49" s="2"/>
+      <c r="M49">
+        <f>$D$1*J49</f>
+        <v>20</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <f>MAX(0, M49-N49)</f>
+        <v>20</v>
+      </c>
+      <c r="P49">
+        <f>_xlfn.CEILING.MATH(O49/D49)</f>
+        <v>1</v>
+      </c>
+      <c r="Q49" s="3">
+        <f>P49*H49</f>
         <v>60.55</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A49" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" s="7">
-        <f>SUM(C48:C48)</f>
+      <c r="R49">
+        <v>20</v>
+      </c>
+      <c r="S49" s="1">
+        <v>60.55</v>
+      </c>
+      <c r="T49" s="1">
+        <v>0</v>
+      </c>
+      <c r="U49" s="1">
+        <v>0</v>
+      </c>
+      <c r="V49" s="1">
+        <f t="shared" ref="V49" si="82">SUM(S49:U49)</f>
+        <v>60.55</v>
+      </c>
+      <c r="W49" s="1">
+        <f t="shared" ref="W49" si="83">V49/R49</f>
+        <v>3.0274999999999999</v>
+      </c>
+      <c r="X49" s="1">
+        <f t="shared" ref="X49" si="84">J49*W49</f>
+        <v>3.0274999999999999</v>
+      </c>
+      <c r="Y49" s="1">
+        <f t="shared" ref="Y49" si="85">K49-X49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A50" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="6">
+        <f>SUM(C49:C49)</f>
         <v>30.66</v>
       </c>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="7">
-        <f>SUM(H48:H48)</f>
+      <c r="E50" s="6">
+        <f>SUM(E49:E49)</f>
+        <v>29.89</v>
+      </c>
+      <c r="F50" s="6">
+        <f>SUM(F49:F49)</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="6">
+        <f>SUM(G49:G49)</f>
+        <v>0</v>
+      </c>
+      <c r="H50" s="6">
+        <f>SUM(H49:H49)</f>
         <v>60.55</v>
       </c>
-      <c r="I49" s="4"/>
-      <c r="J49" s="5">
-        <f>SUM(J48:J48)</f>
-        <v>1</v>
-      </c>
-      <c r="K49" s="7">
-        <f>SUM(K48:K48)</f>
+      <c r="I50" s="6">
+        <f>SUM(I49:I49)</f>
         <v>3.0274999999999999</v>
       </c>
-      <c r="M49" s="5">
-        <f>SUM(M48:M48)</f>
-        <v>20</v>
-      </c>
-      <c r="N49" s="5">
-        <f>SUM(N48:N48)</f>
-        <v>0</v>
-      </c>
-      <c r="O49" s="5">
-        <f>SUM(O48:O48)</f>
-        <v>20</v>
-      </c>
-      <c r="P49" s="5">
-        <f>SUM(P48:P48)</f>
-        <v>1</v>
-      </c>
-      <c r="Q49" s="7">
-        <f>SUM(Q48:Q48)</f>
+      <c r="J50" s="4">
+        <f>SUM(J49:J49)</f>
+        <v>1</v>
+      </c>
+      <c r="K50" s="6">
+        <f>SUM(K49:K49)</f>
+        <v>3.0274999999999999</v>
+      </c>
+      <c r="M50" s="4">
+        <f>SUM(M49:M49)</f>
+        <v>20</v>
+      </c>
+      <c r="N50" s="4">
+        <f>SUM(N49:N49)</f>
+        <v>0</v>
+      </c>
+      <c r="O50" s="4">
+        <f>SUM(O49:O49)</f>
+        <v>20</v>
+      </c>
+      <c r="P50" s="4">
+        <f>SUM(P49:P49)</f>
+        <v>1</v>
+      </c>
+      <c r="Q50" s="6">
+        <f>SUM(Q49:Q49)</f>
         <v>60.55</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="B50" s="5"/>
-      <c r="C50" s="1"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="K50" s="4"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A51" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51">
-        <f>COUNTA(B3:B50)</f>
-        <v>33</v>
-      </c>
-      <c r="C51" s="10">
-        <f>C13+C17+C24+C45+C49</f>
+      <c r="R50" s="4">
+        <f>SUM(R49:R49)</f>
+        <v>20</v>
+      </c>
+      <c r="S50" s="6">
+        <f t="shared" ref="S50:Y50" si="86">SUM(S49:S49)</f>
+        <v>60.55</v>
+      </c>
+      <c r="T50" s="6">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+      <c r="U50" s="6">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+      <c r="V50" s="6">
+        <f t="shared" si="86"/>
+        <v>60.55</v>
+      </c>
+      <c r="W50" s="6">
+        <f t="shared" si="86"/>
+        <v>3.0274999999999999</v>
+      </c>
+      <c r="X50" s="6">
+        <f t="shared" si="86"/>
+        <v>3.0274999999999999</v>
+      </c>
+      <c r="Y50" s="6">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B51" s="4"/>
+      <c r="C51" s="1"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A52" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52">
+        <f>COUNTA(B3:B51)</f>
+        <v>34</v>
+      </c>
+      <c r="C52" s="8">
+        <f>C13+C17+C24+C46+C50</f>
         <v>149.54</v>
       </c>
-      <c r="H51" s="10">
-        <f>H13+H17+H24+H45+H49</f>
+      <c r="D52" s="8">
+        <f>D13+D17+D24+D46+D50</f>
+        <v>1</v>
+      </c>
+      <c r="E52" s="8">
+        <f>E13+E17+E24+E46+E50</f>
+        <v>34.880000000000003</v>
+      </c>
+      <c r="F52" s="8">
+        <f>F13+F17+F24+F46+F50</f>
+        <v>0.40800000000000003</v>
+      </c>
+      <c r="G52" s="8">
+        <f>G13+G17+G24+G46+G50</f>
+        <v>1.7649350000000001</v>
+      </c>
+      <c r="H52" s="8">
+        <f>H13+H17+H24+H46+H50</f>
         <v>192.25346000000002</v>
       </c>
-      <c r="J51" s="11">
-        <f>J13+J17+J24+J45+J49</f>
+      <c r="I52" s="8">
+        <f>I13+I17+I24+I46+I50</f>
+        <v>18.647795000000002</v>
+      </c>
+      <c r="J52" s="9">
+        <f>J13+J17+J24+J46+J50</f>
         <v>77</v>
       </c>
-      <c r="K51" s="10">
-        <f>K13+K17+K24+K45+K49</f>
+      <c r="K52" s="8">
+        <f>K13+K17+K24+K46+K50</f>
         <v>49.771090999999998</v>
       </c>
-      <c r="M51" s="11">
-        <f t="shared" ref="M51:P51" si="64">M13+M17+M24+M45+M49</f>
-        <v>1540</v>
-      </c>
-      <c r="N51" s="11">
-        <f t="shared" si="64"/>
+      <c r="M52" s="9">
+        <f t="shared" ref="M52:P52" si="87">M13+M17+M24+M46+M50</f>
+        <v>1541</v>
+      </c>
+      <c r="N52" s="9">
+        <f t="shared" si="87"/>
         <v>298</v>
       </c>
-      <c r="O51" s="11">
-        <f t="shared" si="64"/>
+      <c r="O52" s="9">
+        <f t="shared" si="87"/>
         <v>1282</v>
       </c>
-      <c r="P51" s="11">
-        <f t="shared" si="64"/>
+      <c r="P52" s="9">
+        <f t="shared" si="87"/>
         <v>729</v>
       </c>
-      <c r="Q51" s="10">
-        <f>Q13+Q17+Q24+Q45+Q49</f>
+      <c r="Q52" s="8">
+        <f>Q13+Q17+Q24+Q46+Q50</f>
         <v>865.28987499999994</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
-        <v>74</v>
+      <c r="R52" s="9">
+        <f t="shared" ref="R52:Y52" si="88">R13+R17+R24+R46+R50</f>
+        <v>1338</v>
+      </c>
+      <c r="S52" s="8">
+        <f t="shared" si="88"/>
+        <v>675.74</v>
+      </c>
+      <c r="T52" s="8">
+        <f t="shared" si="88"/>
+        <v>7.5100000000000007</v>
+      </c>
+      <c r="U52" s="8">
+        <f t="shared" si="88"/>
+        <v>65.378650000000007</v>
+      </c>
+      <c r="V52" s="8">
+        <f t="shared" si="88"/>
+        <v>748.62864999999988</v>
+      </c>
+      <c r="W52" s="8">
+        <f t="shared" si="88"/>
+        <v>45.442148102392338</v>
+      </c>
+      <c r="X52" s="8">
+        <f t="shared" si="88"/>
+        <v>44.732725175119626</v>
+      </c>
+      <c r="Y52" s="8">
+        <f t="shared" si="88"/>
+        <v>5.2878658248803845</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM upon receipt of ordered parts.
</commit_message>
<xml_diff>
--- a/parts/bill_of_materials.xlsx
+++ b/parts/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\laser_tunnel\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93D4078-F14F-4223-8CC0-D26D856A39BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365C360E-49A4-48C9-B9D2-A501179332B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C7A15FB5-B248-4CA2-8E4B-B85C1BCDD779}"/>
   </bookViews>
@@ -438,7 +438,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -470,6 +470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -792,7 +793,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G22" sqref="G22:G25"/>
+      <selection pane="bottomRight" activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -834,7 +835,9 @@
       <c r="R1" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="Z1" s="17"/>
+      <c r="Z1" s="27">
+        <v>44612</v>
+      </c>
     </row>
     <row r="2" spans="1:26" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
@@ -964,7 +967,7 @@
         <v>11.019625</v>
       </c>
       <c r="M4" s="15">
-        <f>$N$1*K4</f>
+        <f t="shared" ref="M4:M14" si="3">$N$1*K4</f>
         <v>20</v>
       </c>
       <c r="N4">
@@ -975,11 +978,11 @@
         <v>19</v>
       </c>
       <c r="P4">
-        <f>_xlfn.CEILING.MATH(O4/E4)</f>
+        <f t="shared" ref="P4:P14" si="4">_xlfn.CEILING.MATH(O4/E4)</f>
         <v>19</v>
       </c>
       <c r="Q4" s="3">
-        <f>P4*I4</f>
+        <f t="shared" ref="Q4:Q14" si="5">P4*I4</f>
         <v>209.37287499999999</v>
       </c>
       <c r="R4" s="15">
@@ -1000,18 +1003,20 @@
         <v>209.37</v>
       </c>
       <c r="W4" s="3">
-        <f>IF((R4&gt;0), V4/R4, J4)</f>
+        <f t="shared" ref="W4:W14" si="6">IF((R4&gt;0), V4/R4, J4)</f>
         <v>11.019473684210526</v>
       </c>
       <c r="X4" s="3">
-        <f>K4*W4</f>
+        <f t="shared" ref="X4:X14" si="7">K4*W4</f>
         <v>11.019473684210526</v>
       </c>
       <c r="Y4" s="3">
-        <f>L4-X4</f>
+        <f t="shared" ref="Y4:Y14" si="8">L4-X4</f>
         <v>1.513157894734718E-4</v>
       </c>
-      <c r="Z4" s="15"/>
+      <c r="Z4" s="15">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
@@ -1033,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" ref="H5:H14" si="3">(D5+F5+G5)*0.1075</f>
+        <f t="shared" ref="H5:H14" si="9">(D5+F5+G5)*0.1075</f>
         <v>0.64392499999999997</v>
       </c>
       <c r="I5" s="3">
@@ -1052,22 +1057,22 @@
         <v>0.66339250000000005</v>
       </c>
       <c r="M5" s="15">
-        <f>$N$1*K5</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="N5">
         <v>8</v>
       </c>
       <c r="O5">
-        <f t="shared" ref="O5:O14" si="4">MAX(0, M5-N5)</f>
+        <f t="shared" ref="O5:O14" si="10">MAX(0, M5-N5)</f>
         <v>12</v>
       </c>
       <c r="P5">
-        <f>_xlfn.CEILING.MATH(O5/E5)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="Q5" s="3">
-        <f>P5*I5</f>
+        <f t="shared" si="5"/>
         <v>13.267850000000001</v>
       </c>
       <c r="R5" s="15">
@@ -1080,23 +1085,23 @@
         <v>0</v>
       </c>
       <c r="U5" s="3">
-        <f t="shared" ref="U5:U14" si="5">ROUND(S5*0.1075, 2)</f>
+        <f t="shared" ref="U5:U14" si="11">ROUND(S5*0.1075, 2)</f>
         <v>1.35</v>
       </c>
       <c r="V5" s="3">
-        <f t="shared" ref="V5:V14" si="6">SUM(S5:U5)</f>
+        <f t="shared" ref="V5:V14" si="12">SUM(S5:U5)</f>
         <v>13.93</v>
       </c>
       <c r="W5" s="3">
-        <f>IF((R5&gt;0), V5/R5, J5)</f>
+        <f t="shared" si="6"/>
         <v>0.69650000000000001</v>
       </c>
       <c r="X5" s="3">
-        <f>K5*W5</f>
+        <f t="shared" si="7"/>
         <v>0.69650000000000001</v>
       </c>
       <c r="Y5" s="3">
-        <f>L5-X5</f>
+        <f t="shared" si="8"/>
         <v>-3.3107499999999956E-2</v>
       </c>
       <c r="Z5" s="15"/>
@@ -1121,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.85892500000000005</v>
       </c>
       <c r="I6" s="3">
@@ -1140,22 +1145,22 @@
         <v>0.5309355</v>
       </c>
       <c r="M6" s="15">
-        <f>$N$1*K6</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="N6">
         <v>50</v>
       </c>
       <c r="O6">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="P6">
-        <f>_xlfn.CEILING.MATH(O6/E6)</f>
         <v>1</v>
       </c>
       <c r="Q6" s="3">
-        <f>P6*I6</f>
+        <f t="shared" si="5"/>
         <v>8.8489249999999995</v>
       </c>
       <c r="R6" s="15">
@@ -1168,26 +1173,28 @@
         <v>0</v>
       </c>
       <c r="U6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.86</v>
       </c>
       <c r="V6" s="3">
+        <f t="shared" si="12"/>
+        <v>8.85</v>
+      </c>
+      <c r="W6" s="3">
         <f t="shared" si="6"/>
-        <v>8.85</v>
-      </c>
-      <c r="W6" s="3">
-        <f>IF((R6&gt;0), V6/R6, J6)</f>
         <v>0.17699999999999999</v>
       </c>
       <c r="X6" s="3">
-        <f>K6*W6</f>
+        <f t="shared" si="7"/>
         <v>0.53099999999999992</v>
       </c>
       <c r="Y6" s="3">
-        <f>L6-X6</f>
+        <f t="shared" si="8"/>
         <v>-6.449999999991185E-5</v>
       </c>
-      <c r="Z6" s="15"/>
+      <c r="Z6" s="15">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
@@ -1209,7 +1216,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.64392499999999997</v>
       </c>
       <c r="I7" s="3">
@@ -1228,22 +1235,22 @@
         <v>0.1326785</v>
       </c>
       <c r="M7" s="15">
-        <f>$N$1*K7</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7">
+        <f t="shared" si="10"/>
+        <v>60</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-      <c r="P7">
-        <f>_xlfn.CEILING.MATH(O7/E7)</f>
         <v>1</v>
       </c>
       <c r="Q7" s="3">
-        <f>P7*I7</f>
+        <f t="shared" si="5"/>
         <v>6.6339250000000005</v>
       </c>
       <c r="R7" s="15">
@@ -1256,23 +1263,23 @@
         <v>0</v>
       </c>
       <c r="U7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.64</v>
       </c>
       <c r="V7" s="3">
+        <f t="shared" si="12"/>
+        <v>6.63</v>
+      </c>
+      <c r="W7" s="3">
         <f t="shared" si="6"/>
-        <v>6.63</v>
-      </c>
-      <c r="W7" s="3">
-        <f>IF((R7&gt;0), V7/R7, J7)</f>
         <v>4.4199999999999996E-2</v>
       </c>
       <c r="X7" s="3">
-        <f>K7*W7</f>
+        <f t="shared" si="7"/>
         <v>0.1326</v>
       </c>
       <c r="Y7" s="3">
-        <f>L7-X7</f>
+        <f t="shared" si="8"/>
         <v>7.8500000000009118E-5</v>
       </c>
       <c r="Z7" s="15"/>
@@ -1297,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.0414249999999998</v>
       </c>
       <c r="I8" s="3">
@@ -1316,22 +1323,22 @@
         <v>7.0104749999999996</v>
       </c>
       <c r="M8" s="15">
-        <f>$N$1*K8</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="N8">
         <v>3</v>
       </c>
       <c r="O8">
+        <f t="shared" si="10"/>
+        <v>17</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="4"/>
-        <v>17</v>
-      </c>
-      <c r="P8">
-        <f>_xlfn.CEILING.MATH(O8/E8)</f>
         <v>6</v>
       </c>
       <c r="Q8" s="3">
-        <f>P8*I8</f>
+        <f t="shared" si="5"/>
         <v>126.18854999999999</v>
       </c>
       <c r="R8" s="15">
@@ -1344,26 +1351,28 @@
         <v>0</v>
       </c>
       <c r="U8" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>12.57</v>
       </c>
       <c r="V8" s="3">
+        <f t="shared" si="12"/>
+        <v>129.51</v>
+      </c>
+      <c r="W8" s="3">
         <f t="shared" si="6"/>
-        <v>129.51</v>
-      </c>
-      <c r="W8" s="3">
-        <f>IF((R8&gt;0), V8/R8, J8)</f>
         <v>7.1949999999999994</v>
       </c>
       <c r="X8" s="3">
-        <f>K8*W8</f>
+        <f t="shared" si="7"/>
         <v>7.1949999999999994</v>
       </c>
       <c r="Y8" s="3">
-        <f>L8-X8</f>
+        <f t="shared" si="8"/>
         <v>-0.18452499999999983</v>
       </c>
-      <c r="Z8" s="15"/>
+      <c r="Z8" s="15">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
@@ -1385,7 +1394,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.396425</v>
       </c>
       <c r="I9" s="3">
@@ -1404,22 +1413,22 @@
         <v>2.8772850000000001</v>
       </c>
       <c r="M9" s="15">
-        <f>$N$1*K9</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="N9">
         <v>6</v>
       </c>
       <c r="O9">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="P9">
-        <f>_xlfn.CEILING.MATH(O9/E9)</f>
         <v>3</v>
       </c>
       <c r="Q9" s="3">
-        <f>P9*I9</f>
+        <f t="shared" si="5"/>
         <v>43.159275000000001</v>
       </c>
       <c r="R9" s="15">
@@ -1432,26 +1441,28 @@
         <v>0</v>
       </c>
       <c r="U9" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>4.03</v>
       </c>
       <c r="V9" s="3">
+        <f t="shared" si="12"/>
+        <v>41.5</v>
+      </c>
+      <c r="W9" s="3">
         <f t="shared" si="6"/>
-        <v>41.5</v>
-      </c>
-      <c r="W9" s="3">
-        <f>IF((R9&gt;0), V9/R9, J9)</f>
         <v>2.7666666666666666</v>
       </c>
       <c r="X9" s="3">
-        <f>K9*W9</f>
+        <f t="shared" si="7"/>
         <v>2.7666666666666666</v>
       </c>
       <c r="Y9" s="3">
-        <f>L9-X9</f>
+        <f t="shared" si="8"/>
         <v>0.11061833333333349</v>
       </c>
-      <c r="Z9" s="15"/>
+      <c r="Z9" s="15">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
@@ -1473,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.5576749999999999</v>
       </c>
       <c r="I10" s="3">
@@ -1492,22 +1503,22 @@
         <v>0.53492250000000008</v>
       </c>
       <c r="M10" s="15">
-        <f>$N$1*K10</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="N10">
         <v>60</v>
       </c>
       <c r="O10">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P10">
-        <f>_xlfn.CEILING.MATH(O10/E10)</f>
-        <v>0</v>
-      </c>
       <c r="Q10" s="3">
-        <f>P10*I10</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R10" s="15">
@@ -1520,23 +1531,23 @@
         <v>0</v>
       </c>
       <c r="U10" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V10" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W10" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="W10" s="3">
-        <f>IF((R10&gt;0), V10/R10, J10)</f>
         <v>0.26746125000000004</v>
       </c>
       <c r="X10" s="3">
-        <f>K10*W10</f>
+        <f t="shared" si="7"/>
         <v>0.53492250000000008</v>
       </c>
       <c r="Y10" s="3">
-        <f>L10-X10</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z10" s="15"/>
@@ -1561,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.80517499999999997</v>
       </c>
       <c r="I11" s="3">
@@ -1580,22 +1591,22 @@
         <v>0.33180700000000002</v>
       </c>
       <c r="M11" s="15">
-        <f>$N$1*K11</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="N11">
         <v>50</v>
       </c>
       <c r="O11">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P11">
-        <f>_xlfn.CEILING.MATH(O11/E11)</f>
-        <v>0</v>
-      </c>
       <c r="Q11" s="3">
-        <f>P11*I11</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R11" s="15">
@@ -1608,23 +1619,23 @@
         <v>0</v>
       </c>
       <c r="U11" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V11" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="W11" s="3">
-        <f>IF((R11&gt;0), V11/R11, J11)</f>
         <v>0.16590350000000001</v>
       </c>
       <c r="X11" s="3">
-        <f>K11*W11</f>
+        <f t="shared" si="7"/>
         <v>0.33180700000000002</v>
       </c>
       <c r="Y11" s="3">
-        <f>L11-X11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z11" s="15"/>
@@ -1649,41 +1660,41 @@
         <v>0</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" ref="H12:H13" si="7">(D12+F12+G12)*0.1075</f>
+        <f t="shared" ref="H12:H13" si="13">(D12+F12+G12)*0.1075</f>
         <v>1.127675</v>
       </c>
       <c r="I12" s="3">
-        <f t="shared" ref="I12:I13" si="8">D12+F12+H12</f>
+        <f t="shared" ref="I12:I13" si="14">D12+F12+H12</f>
         <v>11.617675</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" ref="J12:J13" si="9">I12/E12</f>
+        <f t="shared" ref="J12:J13" si="15">I12/E12</f>
         <v>0.11617675</v>
       </c>
       <c r="K12">
         <v>3</v>
       </c>
       <c r="L12" s="3">
-        <f t="shared" ref="L12:L13" si="10">J12*K12</f>
+        <f t="shared" ref="L12:L13" si="16">J12*K12</f>
         <v>0.34853024999999999</v>
       </c>
       <c r="M12" s="15">
-        <f>$N$1*K12</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
-        <f t="shared" ref="O12:O13" si="11">MAX(0, M12-N12)</f>
+        <f t="shared" ref="O12:O13" si="17">MAX(0, M12-N12)</f>
         <v>60</v>
       </c>
       <c r="P12">
-        <f>_xlfn.CEILING.MATH(O12/E12)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q12" s="3">
-        <f>P12*I12</f>
+        <f t="shared" si="5"/>
         <v>11.617675</v>
       </c>
       <c r="R12" s="15">
@@ -1696,23 +1707,23 @@
         <v>0</v>
       </c>
       <c r="U12" s="3">
-        <f t="shared" ref="U12:U13" si="12">ROUND(S12*0.1075, 2)</f>
+        <f t="shared" ref="U12:U13" si="18">ROUND(S12*0.1075, 2)</f>
         <v>1.1299999999999999</v>
       </c>
       <c r="V12" s="3">
-        <f t="shared" ref="V12:V13" si="13">SUM(S12:U12)</f>
+        <f t="shared" ref="V12:V13" si="19">SUM(S12:U12)</f>
         <v>11.620000000000001</v>
       </c>
       <c r="W12" s="3">
-        <f>IF((R12&gt;0), V12/R12, J12)</f>
+        <f t="shared" si="6"/>
         <v>0.11620000000000001</v>
       </c>
       <c r="X12" s="3">
-        <f>K12*W12</f>
+        <f t="shared" si="7"/>
         <v>0.34860000000000002</v>
       </c>
       <c r="Y12" s="3">
-        <f>L12-X12</f>
+        <f t="shared" si="8"/>
         <v>-6.9750000000035062E-5</v>
       </c>
       <c r="Z12" s="15"/>
@@ -1737,41 +1748,41 @@
         <v>0</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.75035000000000007</v>
       </c>
       <c r="I13" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>7.7303500000000005</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>7.7303500000000011E-2</v>
       </c>
       <c r="K13">
         <v>3</v>
       </c>
       <c r="L13" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>0.23191050000000002</v>
       </c>
       <c r="M13" s="15">
-        <f>$N$1*K13</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="N13">
         <v>0</v>
       </c>
       <c r="O13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>60</v>
       </c>
       <c r="P13">
-        <f>_xlfn.CEILING.MATH(O13/E13)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q13" s="3">
-        <f>P13*I13</f>
+        <f t="shared" si="5"/>
         <v>7.7303500000000005</v>
       </c>
       <c r="R13" s="15">
@@ -1784,23 +1795,23 @@
         <v>0</v>
       </c>
       <c r="U13" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0.75</v>
       </c>
       <c r="V13" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>7.73</v>
       </c>
       <c r="W13" s="3">
-        <f>IF((R13&gt;0), V13/R13, J13)</f>
+        <f t="shared" si="6"/>
         <v>7.7300000000000008E-2</v>
       </c>
       <c r="X13" s="3">
-        <f>K13*W13</f>
+        <f t="shared" si="7"/>
         <v>0.23190000000000002</v>
       </c>
       <c r="Y13" s="3">
-        <f>L13-X13</f>
+        <f t="shared" si="8"/>
         <v>1.0499999999996623E-5</v>
       </c>
       <c r="Z13" s="15"/>
@@ -1825,7 +1836,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.0414249999999998</v>
       </c>
       <c r="I14" s="3">
@@ -1844,22 +1855,22 @@
         <v>4.2062849999999994</v>
       </c>
       <c r="M14" s="15">
-        <f>$N$1*K14</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="P14">
         <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="P14">
-        <f>_xlfn.CEILING.MATH(O14/E14)</f>
         <v>4</v>
       </c>
       <c r="Q14" s="3">
-        <f>P14*I14</f>
+        <f t="shared" si="5"/>
         <v>84.125699999999995</v>
       </c>
       <c r="R14" s="15">
@@ -1872,23 +1883,23 @@
         <v>0</v>
       </c>
       <c r="U14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>8.6</v>
       </c>
       <c r="V14" s="3">
+        <f t="shared" si="12"/>
+        <v>88.559999999999988</v>
+      </c>
+      <c r="W14" s="3">
         <f t="shared" si="6"/>
-        <v>88.559999999999988</v>
-      </c>
-      <c r="W14" s="3">
-        <f>IF((R14&gt;0), V14/R14, J14)</f>
         <v>4.427999999999999</v>
       </c>
       <c r="X14" s="3">
-        <f>K14*W14</f>
+        <f t="shared" si="7"/>
         <v>4.427999999999999</v>
       </c>
       <c r="Y14" s="3">
-        <f>L14-X14</f>
+        <f t="shared" si="8"/>
         <v>-0.22171499999999966</v>
       </c>
       <c r="Z14" s="15"/>
@@ -1909,66 +1920,68 @@
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="10">
-        <f>SUM(K4:K14)</f>
+        <f t="shared" ref="K15:Y15" si="20">SUM(K4:K14)</f>
         <v>21</v>
       </c>
       <c r="L15" s="6">
-        <f>SUM(L4:L14)</f>
+        <f t="shared" si="20"/>
         <v>27.887846750000001</v>
       </c>
       <c r="M15" s="23">
-        <f>SUM(M4:M14)</f>
+        <f t="shared" si="20"/>
         <v>420</v>
       </c>
       <c r="N15" s="10">
-        <f>SUM(N4:N14)</f>
+        <f t="shared" si="20"/>
         <v>178</v>
       </c>
       <c r="O15" s="10">
-        <f>SUM(O4:O14)</f>
+        <f t="shared" si="20"/>
         <v>272</v>
       </c>
       <c r="P15" s="10">
-        <f>SUM(P4:P14)</f>
+        <f t="shared" si="20"/>
         <v>38</v>
       </c>
       <c r="Q15" s="6">
-        <f>SUM(Q4:Q14)</f>
+        <f t="shared" si="20"/>
         <v>510.94512500000002</v>
       </c>
       <c r="R15" s="23">
-        <f>SUM(R4:R14)</f>
+        <f t="shared" si="20"/>
         <v>492</v>
       </c>
       <c r="S15" s="6">
-        <f>SUM(S4:S14)</f>
+        <f t="shared" si="20"/>
         <v>467.4500000000001</v>
       </c>
       <c r="T15" s="6">
-        <f>SUM(T4:T14)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="U15" s="6">
-        <f>SUM(U4:U14)</f>
+        <f t="shared" si="20"/>
         <v>50.250000000000007</v>
       </c>
       <c r="V15" s="6">
-        <f>SUM(V4:V14)</f>
+        <f t="shared" si="20"/>
         <v>517.69999999999993</v>
       </c>
       <c r="W15" s="6">
-        <f>SUM(W4:W14)</f>
+        <f t="shared" si="20"/>
         <v>26.953705100877187</v>
       </c>
       <c r="X15" s="6">
-        <f>SUM(X4:X14)</f>
+        <f t="shared" si="20"/>
         <v>28.216469850877196</v>
       </c>
       <c r="Y15" s="6">
-        <f>SUM(Y4:Y14)</f>
+        <f t="shared" si="20"/>
         <v>-0.32862310087719243</v>
       </c>
-      <c r="Z15" s="15"/>
+      <c r="Z15" s="15">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B16" s="4"/>
@@ -2010,22 +2023,22 @@
         <v>0</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" ref="H18" si="14">(D18+F18+G18)*0.1075</f>
+        <f t="shared" ref="H18" si="21">(D18+F18+G18)*0.1075</f>
         <v>0.19134999999999999</v>
       </c>
       <c r="I18" s="3">
-        <f t="shared" ref="I18" si="15">D18+F18+H18</f>
+        <f t="shared" ref="I18" si="22">D18+F18+H18</f>
         <v>1.9713499999999999</v>
       </c>
       <c r="J18" s="3">
-        <f t="shared" ref="J18" si="16">I18/E18</f>
+        <f t="shared" ref="J18" si="23">I18/E18</f>
         <v>1.9713499999999999</v>
       </c>
       <c r="K18">
         <v>1</v>
       </c>
       <c r="L18" s="3">
-        <f t="shared" ref="L18" si="17">J18*K18</f>
+        <f t="shared" ref="L18" si="24">J18*K18</f>
         <v>1.9713499999999999</v>
       </c>
       <c r="M18" s="15">
@@ -2036,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <f t="shared" ref="O18" si="18">MAX(0, M18-N18)</f>
+        <f t="shared" ref="O18" si="25">MAX(0, M18-N18)</f>
         <v>20</v>
       </c>
       <c r="P18">
@@ -2084,19 +2097,19 @@
         <v>1.78</v>
       </c>
       <c r="E19" s="19">
-        <f t="shared" ref="E19:H19" si="19">SUM(E18:E18)</f>
+        <f t="shared" ref="E19:H19" si="26">SUM(E18:E18)</f>
         <v>1</v>
       </c>
       <c r="F19" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="G19" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="H19" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0.19134999999999999</v>
       </c>
       <c r="I19" s="6">
@@ -2116,19 +2129,19 @@
         <v>1.9713499999999999</v>
       </c>
       <c r="M19" s="23">
-        <f t="shared" ref="M19:P19" si="20">SUM(M18:M18)</f>
+        <f t="shared" ref="M19:P19" si="27">SUM(M18:M18)</f>
         <v>20</v>
       </c>
       <c r="N19" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="O19" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>20</v>
       </c>
       <c r="P19" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>20</v>
       </c>
       <c r="Q19" s="6">
@@ -2140,31 +2153,31 @@
         <v>0</v>
       </c>
       <c r="S19" s="6">
-        <f t="shared" ref="S19:Y19" si="21">SUM(S18:S18)</f>
+        <f t="shared" ref="S19:Y19" si="28">SUM(S18:S18)</f>
         <v>0</v>
       </c>
       <c r="T19" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="U19" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="V19" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="W19" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>1.9713499999999999</v>
       </c>
       <c r="X19" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>1.9713499999999999</v>
       </c>
       <c r="Y19" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Z19" s="15"/>
@@ -2240,7 +2253,7 @@
         <v>0</v>
       </c>
       <c r="O22">
-        <f t="shared" ref="O22:O25" si="22">MAX(0, M22-N22)</f>
+        <f t="shared" ref="O22:O25" si="29">MAX(0, M22-N22)</f>
         <v>20</v>
       </c>
       <c r="P22">
@@ -2266,19 +2279,19 @@
         <v>0</v>
       </c>
       <c r="V22" s="3">
-        <f t="shared" ref="V22:V25" si="23">SUM(S22:U22)</f>
+        <f t="shared" ref="V22:V25" si="30">SUM(S22:U22)</f>
         <v>11.399999999999999</v>
       </c>
       <c r="W22" s="3">
-        <f t="shared" ref="W22:W25" si="24">IF((R22&gt;0), V22/R22, J22)</f>
+        <f t="shared" ref="W22:W25" si="31">IF((R22&gt;0), V22/R22, J22)</f>
         <v>0.56999999999999995</v>
       </c>
       <c r="X22" s="3">
-        <f t="shared" ref="X22:X25" si="25">K22*W22</f>
+        <f t="shared" ref="X22:X25" si="32">K22*W22</f>
         <v>0.56999999999999995</v>
       </c>
       <c r="Y22" s="3">
-        <f t="shared" ref="Y22:Y25" si="26">L22-X22</f>
+        <f t="shared" ref="Y22:Y25" si="33">L22-X22</f>
         <v>-0.56999999999999995</v>
       </c>
       <c r="Z22" s="15"/>
@@ -2326,7 +2339,7 @@
         <v>0</v>
       </c>
       <c r="O23">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>20</v>
       </c>
       <c r="P23">
@@ -2338,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="R23" s="15">
-        <f t="shared" ref="R23:R25" si="27">M23</f>
+        <f t="shared" ref="R23:R25" si="34">M23</f>
         <v>20</v>
       </c>
       <c r="S23" s="1">
@@ -2352,19 +2365,19 @@
         <v>0</v>
       </c>
       <c r="V23" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>0.6</v>
       </c>
       <c r="W23" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
       <c r="X23" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="32"/>
         <v>0.03</v>
       </c>
       <c r="Y23" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>-0.03</v>
       </c>
       <c r="Z23" s="15"/>
@@ -2412,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="O24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>20</v>
       </c>
       <c r="P24">
@@ -2424,11 +2437,11 @@
         <v>0</v>
       </c>
       <c r="R24" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="34"/>
         <v>20</v>
       </c>
       <c r="S24" s="1">
-        <f t="shared" ref="S24:S26" si="28">1*$C$21*R24</f>
+        <f t="shared" ref="S24:S25" si="35">1*$C$21*R24</f>
         <v>0.6</v>
       </c>
       <c r="T24" s="1">
@@ -2438,19 +2451,19 @@
         <v>0</v>
       </c>
       <c r="V24" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>0.6</v>
       </c>
       <c r="W24" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
       <c r="X24" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="32"/>
         <v>0.03</v>
       </c>
       <c r="Y24" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>-0.03</v>
       </c>
       <c r="Z24" s="15"/>
@@ -2498,7 +2511,7 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>20</v>
       </c>
       <c r="P25">
@@ -2510,11 +2523,11 @@
         <v>0</v>
       </c>
       <c r="R25" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="34"/>
         <v>20</v>
       </c>
       <c r="S25" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="35"/>
         <v>0.6</v>
       </c>
       <c r="T25" s="1">
@@ -2524,19 +2537,19 @@
         <v>0</v>
       </c>
       <c r="V25" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>0.6</v>
       </c>
       <c r="W25" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="31"/>
         <v>0.03</v>
       </c>
       <c r="X25" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="32"/>
         <v>0.03</v>
       </c>
       <c r="Y25" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>-0.03</v>
       </c>
       <c r="Z25" s="15"/>
@@ -2564,19 +2577,19 @@
         <v>0</v>
       </c>
       <c r="M26" s="23">
-        <f t="shared" ref="M26:P26" si="29">SUM(M22:M25)</f>
+        <f t="shared" ref="M26:P26" si="36">SUM(M22:M25)</f>
         <v>80</v>
       </c>
       <c r="N26" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O26" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>80</v>
       </c>
       <c r="P26" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>80</v>
       </c>
       <c r="Q26" s="6">
@@ -2584,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="R26" s="23">
-        <f t="shared" ref="R26" si="30">SUM(R22:R25)</f>
+        <f t="shared" ref="R26" si="37">SUM(R22:R25)</f>
         <v>80</v>
       </c>
       <c r="S26" s="1">
@@ -2600,19 +2613,19 @@
         <v>0</v>
       </c>
       <c r="V26" s="6">
-        <f t="shared" ref="V26:Y26" si="31">SUM(V22:V25)</f>
+        <f t="shared" ref="V26:Y26" si="38">SUM(V22:V25)</f>
         <v>13.199999999999998</v>
       </c>
       <c r="W26" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.66</v>
       </c>
       <c r="X26" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.66</v>
       </c>
       <c r="Y26" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>-0.66</v>
       </c>
       <c r="Z26" s="15"/>
@@ -2666,41 +2679,41 @@
         <v>5.3000000000000005E-2</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" ref="H29" si="32">(D29+F29+G29)*0.1075</f>
+        <f t="shared" ref="H29" si="39">(D29+F29+G29)*0.1075</f>
         <v>6.2672500000000006E-2</v>
       </c>
       <c r="I29" s="3">
-        <f t="shared" ref="I29" si="33">D29+F29+H29</f>
+        <f t="shared" ref="I29" si="40">D29+F29+H29</f>
         <v>0.59267250000000005</v>
       </c>
       <c r="J29" s="3">
-        <f t="shared" ref="J29" si="34">I29/E29</f>
+        <f t="shared" ref="J29" si="41">I29/E29</f>
         <v>0.59267250000000005</v>
       </c>
       <c r="K29">
         <v>1</v>
       </c>
       <c r="L29" s="3">
-        <f t="shared" ref="L29" si="35">J29*K29</f>
+        <f t="shared" ref="L29" si="42">J29*K29</f>
         <v>0.59267250000000005</v>
       </c>
       <c r="M29" s="15">
-        <f>$N$1*K29</f>
+        <f t="shared" ref="M29:M47" si="43">$N$1*K29</f>
         <v>20</v>
       </c>
       <c r="N29">
         <v>20</v>
       </c>
       <c r="O29">
-        <f t="shared" ref="O29:O47" si="36">MAX(0, M29-N29)</f>
+        <f t="shared" ref="O29:O47" si="44">MAX(0, M29-N29)</f>
         <v>0</v>
       </c>
       <c r="P29">
-        <f>_xlfn.CEILING.MATH(O29/E29)</f>
+        <f t="shared" ref="P29:P47" si="45">_xlfn.CEILING.MATH(O29/E29)</f>
         <v>0</v>
       </c>
       <c r="Q29" s="3">
-        <f>P29*I29</f>
+        <f t="shared" ref="Q29:Q47" si="46">P29*I29</f>
         <v>0</v>
       </c>
       <c r="R29" s="15">
@@ -2721,15 +2734,15 @@
         <v>5.3783750000000001</v>
       </c>
       <c r="W29" s="3">
-        <f>IF((R29&gt;0), V29/R29, J29)</f>
+        <f t="shared" ref="W29:W47" si="47">IF((R29&gt;0), V29/R29, J29)</f>
         <v>0.53783749999999997</v>
       </c>
       <c r="X29" s="3">
-        <f>K29*W29</f>
+        <f t="shared" ref="X29:X46" si="48">K29*W29</f>
         <v>0.53783749999999997</v>
       </c>
       <c r="Y29" s="3">
-        <f>L29-X29</f>
+        <f t="shared" ref="Y29:Y47" si="49">L29-X29</f>
         <v>5.4835000000000078E-2</v>
       </c>
       <c r="Z29" s="15"/>
@@ -2774,22 +2787,22 @@
         <v>1.901025</v>
       </c>
       <c r="M30" s="15">
-        <f>$N$1*K30</f>
+        <f t="shared" si="43"/>
         <v>40</v>
       </c>
       <c r="N30">
         <v>0</v>
       </c>
       <c r="O30">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>40</v>
       </c>
       <c r="P30">
-        <f>_xlfn.CEILING.MATH(O30/E30)</f>
+        <f t="shared" si="45"/>
         <v>20</v>
       </c>
       <c r="Q30" s="3">
-        <f>P30*I30</f>
+        <f t="shared" si="46"/>
         <v>38.020499999999998</v>
       </c>
       <c r="R30" s="15">
@@ -2802,23 +2815,23 @@
         <v>1.55</v>
       </c>
       <c r="U30" s="3">
-        <f t="shared" ref="U30:U46" si="37">S30*0.1075</f>
+        <f t="shared" ref="U30:U46" si="50">S30*0.1075</f>
         <v>1.6694749999999998</v>
       </c>
       <c r="V30" s="3">
-        <f t="shared" ref="V30:V47" si="38">SUM(S30:U30)</f>
+        <f t="shared" ref="V30:V47" si="51">SUM(S30:U30)</f>
         <v>18.749474999999997</v>
       </c>
       <c r="W30" s="3">
-        <f>IF((R30&gt;0), V30/R30, J30)</f>
+        <f t="shared" si="47"/>
         <v>0.37498949999999992</v>
       </c>
       <c r="X30" s="3">
-        <f>K30*W30</f>
+        <f t="shared" si="48"/>
         <v>0.74997899999999984</v>
       </c>
       <c r="Y30" s="3">
-        <f>L30-X30</f>
+        <f t="shared" si="49"/>
         <v>1.151046</v>
       </c>
       <c r="Z30" s="15"/>
@@ -2862,22 +2875,22 @@
         <v>0.89707500000000007</v>
       </c>
       <c r="M31" s="15">
-        <f>$N$1*K31</f>
+        <f t="shared" si="43"/>
         <v>20</v>
       </c>
       <c r="N31">
         <v>10</v>
       </c>
       <c r="O31">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>10</v>
       </c>
       <c r="P31">
-        <f>_xlfn.CEILING.MATH(O31/E31)</f>
+        <f t="shared" si="45"/>
         <v>10</v>
       </c>
       <c r="Q31" s="3">
-        <f>P31*I31</f>
+        <f t="shared" si="46"/>
         <v>8.9707500000000007</v>
       </c>
       <c r="R31" s="15">
@@ -2888,23 +2901,23 @@
       </c>
       <c r="T31" s="1"/>
       <c r="U31" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>0.73745000000000005</v>
       </c>
       <c r="V31" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>7.5974500000000003</v>
       </c>
       <c r="W31" s="3">
-        <f>IF((R31&gt;0), V31/R31, J31)</f>
+        <f t="shared" si="47"/>
         <v>0.759745</v>
       </c>
       <c r="X31" s="3">
-        <f>K31*W31</f>
+        <f t="shared" si="48"/>
         <v>0.759745</v>
       </c>
       <c r="Y31" s="3">
-        <f>L31-X31</f>
+        <f t="shared" si="49"/>
         <v>0.13733000000000006</v>
       </c>
       <c r="Z31" s="15"/>
@@ -2930,41 +2943,41 @@
         <v>0.03</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" ref="H32" si="39">(D32+F32+G32)*0.1075</f>
+        <f t="shared" ref="H32" si="52">(D32+F32+G32)*0.1075</f>
         <v>0.15157499999999999</v>
       </c>
       <c r="I32" s="3">
-        <f t="shared" ref="I32" si="40">D32+F32+H32</f>
+        <f t="shared" ref="I32" si="53">D32+F32+H32</f>
         <v>1.5315749999999999</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" ref="J32" si="41">I32/E32</f>
+        <f t="shared" ref="J32" si="54">I32/E32</f>
         <v>1.5315749999999999</v>
       </c>
       <c r="K32">
         <v>1</v>
       </c>
       <c r="L32" s="3">
-        <f t="shared" ref="L32" si="42">J32*K32</f>
+        <f t="shared" ref="L32" si="55">J32*K32</f>
         <v>1.5315749999999999</v>
       </c>
       <c r="M32" s="15">
-        <f>$N$1*K32</f>
+        <f t="shared" si="43"/>
         <v>20</v>
       </c>
       <c r="N32">
         <v>10</v>
       </c>
       <c r="O32">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>10</v>
       </c>
       <c r="P32">
-        <f>_xlfn.CEILING.MATH(O32/E32)</f>
+        <f t="shared" si="45"/>
         <v>10</v>
       </c>
       <c r="Q32" s="3">
-        <f>P32*I32</f>
+        <f t="shared" si="46"/>
         <v>15.31575</v>
       </c>
       <c r="R32" s="15">
@@ -2977,23 +2990,23 @@
         <v>1.75</v>
       </c>
       <c r="U32" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>1.8855499999999998</v>
       </c>
       <c r="V32" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>21.175549999999998</v>
       </c>
       <c r="W32" s="3">
-        <f>IF((R32&gt;0), V32/R32, J32)</f>
+        <f t="shared" si="47"/>
         <v>1.4117033333333331</v>
       </c>
       <c r="X32" s="3">
-        <f>K32*W32</f>
+        <f t="shared" si="48"/>
         <v>1.4117033333333331</v>
       </c>
       <c r="Y32" s="3">
-        <f>L32-X32</f>
+        <f t="shared" si="49"/>
         <v>0.11987166666666682</v>
       </c>
       <c r="Z32" s="15"/>
@@ -3018,41 +3031,41 @@
         <v>0</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" ref="H33:H36" si="43">(D33+F33+G33)*0.1075</f>
+        <f t="shared" ref="H33:H36" si="56">(D33+F33+G33)*0.1075</f>
         <v>4.7300000000000002E-2</v>
       </c>
       <c r="I33" s="3">
-        <f t="shared" ref="I33:I36" si="44">D33+F33+H33</f>
+        <f t="shared" ref="I33:I36" si="57">D33+F33+H33</f>
         <v>0.48730000000000001</v>
       </c>
       <c r="J33" s="3">
-        <f t="shared" ref="J33:J36" si="45">I33/E33</f>
+        <f t="shared" ref="J33:J36" si="58">I33/E33</f>
         <v>0.48730000000000001</v>
       </c>
       <c r="K33">
         <v>1</v>
       </c>
       <c r="L33" s="3">
-        <f t="shared" ref="L33:L36" si="46">J33*K33</f>
+        <f t="shared" ref="L33:L36" si="59">J33*K33</f>
         <v>0.48730000000000001</v>
       </c>
       <c r="M33" s="15">
-        <f>$N$1*K33</f>
+        <f t="shared" si="43"/>
         <v>20</v>
       </c>
       <c r="N33">
         <v>0</v>
       </c>
       <c r="O33">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>20</v>
       </c>
       <c r="P33">
-        <f>_xlfn.CEILING.MATH(O33/E33)</f>
+        <f t="shared" si="45"/>
         <v>20</v>
       </c>
       <c r="Q33" s="3">
-        <f>P33*I33</f>
+        <f t="shared" si="46"/>
         <v>9.7460000000000004</v>
       </c>
       <c r="R33" s="15">
@@ -3063,23 +3076,23 @@
       </c>
       <c r="T33" s="1"/>
       <c r="U33" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>0.71594999999999998</v>
       </c>
       <c r="V33" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>7.3759500000000005</v>
       </c>
       <c r="W33" s="3">
-        <f>IF((R33&gt;0), V33/R33, J33)</f>
+        <f t="shared" si="47"/>
         <v>0.3687975</v>
       </c>
       <c r="X33" s="3">
-        <f>K33*W33</f>
+        <f t="shared" si="48"/>
         <v>0.3687975</v>
       </c>
       <c r="Y33" s="3">
-        <f>L33-X33</f>
+        <f t="shared" si="49"/>
         <v>0.11850250000000001</v>
       </c>
       <c r="Z33" s="15"/>
@@ -3104,41 +3117,41 @@
         <v>0</v>
       </c>
       <c r="H34" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="56"/>
         <v>1.0750000000000001E-2</v>
       </c>
       <c r="I34" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="57"/>
         <v>0.11075</v>
       </c>
       <c r="J34" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="58"/>
         <v>0.11075</v>
       </c>
       <c r="K34">
         <v>9</v>
       </c>
       <c r="L34" s="3">
+        <f t="shared" si="59"/>
+        <v>0.99675000000000002</v>
+      </c>
+      <c r="M34" s="15">
+        <f t="shared" si="43"/>
+        <v>180</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="44"/>
+        <v>180</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="45"/>
+        <v>180</v>
+      </c>
+      <c r="Q34" s="3">
         <f t="shared" si="46"/>
-        <v>0.99675000000000002</v>
-      </c>
-      <c r="M34" s="15">
-        <f>$N$1*K34</f>
-        <v>180</v>
-      </c>
-      <c r="N34">
-        <v>0</v>
-      </c>
-      <c r="O34">
-        <f t="shared" si="36"/>
-        <v>180</v>
-      </c>
-      <c r="P34">
-        <f>_xlfn.CEILING.MATH(O34/E34)</f>
-        <v>180</v>
-      </c>
-      <c r="Q34" s="3">
-        <f>P34*I34</f>
         <v>19.934999999999999</v>
       </c>
       <c r="R34" s="15">
@@ -3149,23 +3162,23 @@
       </c>
       <c r="T34" s="1"/>
       <c r="U34" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>0.53964999999999996</v>
       </c>
       <c r="V34" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>5.5596499999999995</v>
       </c>
       <c r="W34" s="3">
-        <f>IF((R34&gt;0), V34/R34, J34)</f>
+        <f t="shared" si="47"/>
         <v>2.2238599999999997E-2</v>
       </c>
       <c r="X34" s="3">
-        <f>K34*W34</f>
+        <f t="shared" si="48"/>
         <v>0.20014739999999998</v>
       </c>
       <c r="Y34" s="3">
-        <f>L34-X34</f>
+        <f t="shared" si="49"/>
         <v>0.79660260000000005</v>
       </c>
       <c r="Z34" s="15"/>
@@ -3190,41 +3203,41 @@
         <v>0</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="56"/>
         <v>3.2250000000000001E-2</v>
       </c>
       <c r="I35" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="57"/>
         <v>0.33224999999999999</v>
       </c>
       <c r="J35" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="58"/>
         <v>0.11075</v>
       </c>
       <c r="K35">
         <v>2</v>
       </c>
       <c r="L35" s="3">
+        <f t="shared" si="59"/>
+        <v>0.2215</v>
+      </c>
+      <c r="M35" s="15">
+        <f t="shared" si="43"/>
+        <v>40</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="44"/>
+        <v>40</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="45"/>
+        <v>14</v>
+      </c>
+      <c r="Q35" s="3">
         <f t="shared" si="46"/>
-        <v>0.2215</v>
-      </c>
-      <c r="M35" s="15">
-        <f>$N$1*K35</f>
-        <v>40</v>
-      </c>
-      <c r="N35">
-        <v>0</v>
-      </c>
-      <c r="O35">
-        <f t="shared" si="36"/>
-        <v>40</v>
-      </c>
-      <c r="P35">
-        <f>_xlfn.CEILING.MATH(O35/E35)</f>
-        <v>14</v>
-      </c>
-      <c r="Q35" s="3">
-        <f>P35*I35</f>
         <v>4.6514999999999995</v>
       </c>
       <c r="R35" s="15">
@@ -3235,23 +3248,23 @@
       </c>
       <c r="T35" s="1"/>
       <c r="U35" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>0.19564999999999999</v>
       </c>
       <c r="V35" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>2.0156499999999999</v>
       </c>
       <c r="W35" s="3">
-        <f>IF((R35&gt;0), V35/R35, J35)</f>
+        <f t="shared" si="47"/>
         <v>4.0313000000000002E-2</v>
       </c>
       <c r="X35" s="3">
-        <f>K35*W35</f>
+        <f t="shared" si="48"/>
         <v>8.0626000000000003E-2</v>
       </c>
       <c r="Y35" s="3">
-        <f>L35-X35</f>
+        <f t="shared" si="49"/>
         <v>0.140874</v>
       </c>
       <c r="Z35" s="15"/>
@@ -3276,41 +3289,41 @@
         <v>0</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="56"/>
         <v>5.3749999999999999E-2</v>
       </c>
       <c r="I36" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="57"/>
         <v>0.55374999999999996</v>
       </c>
       <c r="J36" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="58"/>
         <v>0.11074999999999999</v>
       </c>
       <c r="K36">
         <v>5</v>
       </c>
       <c r="L36" s="3">
+        <f t="shared" si="59"/>
+        <v>0.55374999999999996</v>
+      </c>
+      <c r="M36" s="15">
+        <f t="shared" si="43"/>
+        <v>100</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="44"/>
+        <v>100</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="45"/>
+        <v>20</v>
+      </c>
+      <c r="Q36" s="3">
         <f t="shared" si="46"/>
-        <v>0.55374999999999996</v>
-      </c>
-      <c r="M36" s="15">
-        <f>$N$1*K36</f>
-        <v>100</v>
-      </c>
-      <c r="N36">
-        <v>0</v>
-      </c>
-      <c r="O36">
-        <f t="shared" si="36"/>
-        <v>100</v>
-      </c>
-      <c r="P36">
-        <f>_xlfn.CEILING.MATH(O36/E36)</f>
-        <v>20</v>
-      </c>
-      <c r="Q36" s="3">
-        <f>P36*I36</f>
         <v>11.074999999999999</v>
       </c>
       <c r="R36" s="15">
@@ -3321,23 +3334,23 @@
       </c>
       <c r="T36" s="1"/>
       <c r="U36" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>0.27734999999999999</v>
       </c>
       <c r="V36" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>2.8573500000000003</v>
       </c>
       <c r="W36" s="3">
-        <f>IF((R36&gt;0), V36/R36, J36)</f>
+        <f t="shared" si="47"/>
         <v>2.8573500000000002E-2</v>
       </c>
       <c r="X36" s="3">
-        <f>K36*W36</f>
+        <f t="shared" si="48"/>
         <v>0.14286750000000001</v>
       </c>
       <c r="Y36" s="3">
-        <f>L36-X36</f>
+        <f t="shared" si="49"/>
         <v>0.41088249999999993</v>
       </c>
       <c r="Z36" s="15"/>
@@ -3362,41 +3375,41 @@
         <v>0</v>
       </c>
       <c r="H37" s="3">
-        <f t="shared" ref="H37" si="47">(D37+F37+G37)*0.1075</f>
+        <f t="shared" ref="H37" si="60">(D37+F37+G37)*0.1075</f>
         <v>1.0750000000000001E-2</v>
       </c>
       <c r="I37" s="3">
-        <f t="shared" ref="I37" si="48">D37+F37+H37</f>
+        <f t="shared" ref="I37" si="61">D37+F37+H37</f>
         <v>0.11075</v>
       </c>
       <c r="J37" s="3">
-        <f t="shared" ref="J37" si="49">I37/E37</f>
+        <f t="shared" ref="J37" si="62">I37/E37</f>
         <v>0.11075</v>
       </c>
       <c r="K37">
         <v>5</v>
       </c>
       <c r="L37" s="3">
-        <f t="shared" ref="L37" si="50">J37*K37</f>
+        <f t="shared" ref="L37" si="63">J37*K37</f>
         <v>0.55374999999999996</v>
       </c>
       <c r="M37" s="15">
-        <f>$N$1*K37</f>
+        <f t="shared" si="43"/>
         <v>100</v>
       </c>
       <c r="N37">
         <v>0</v>
       </c>
       <c r="O37">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>100</v>
       </c>
       <c r="P37">
-        <f>_xlfn.CEILING.MATH(O37/E37)</f>
+        <f t="shared" si="45"/>
         <v>100</v>
       </c>
       <c r="Q37" s="3">
-        <f>P37*I37</f>
+        <f t="shared" si="46"/>
         <v>11.074999999999999</v>
       </c>
       <c r="R37" s="15">
@@ -3409,23 +3422,23 @@
         <v>0.16</v>
       </c>
       <c r="U37" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>0.17092499999999999</v>
       </c>
       <c r="V37" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>1.920925</v>
       </c>
       <c r="W37" s="3">
-        <f>IF((R37&gt;0), V37/R37, J37)</f>
+        <f t="shared" si="47"/>
         <v>7.6837000000000003E-2</v>
       </c>
       <c r="X37" s="3">
-        <f>K37*W37</f>
+        <f t="shared" si="48"/>
         <v>0.384185</v>
       </c>
       <c r="Y37" s="3">
-        <f>L37-X37</f>
+        <f t="shared" si="49"/>
         <v>0.16956499999999997</v>
       </c>
       <c r="Z37" s="15"/>
@@ -3450,41 +3463,41 @@
         <v>0</v>
       </c>
       <c r="H38" s="3">
-        <f t="shared" ref="H38" si="51">(D38+F38+G38)*0.1075</f>
+        <f t="shared" ref="H38" si="64">(D38+F38+G38)*0.1075</f>
         <v>1.0750000000000001E-2</v>
       </c>
       <c r="I38" s="3">
-        <f t="shared" ref="I38" si="52">D38+F38+H38</f>
+        <f t="shared" ref="I38" si="65">D38+F38+H38</f>
         <v>0.11075</v>
       </c>
       <c r="J38" s="3">
-        <f t="shared" ref="J38" si="53">I38/E38</f>
+        <f t="shared" ref="J38" si="66">I38/E38</f>
         <v>0.11075</v>
       </c>
       <c r="K38">
         <v>5</v>
       </c>
       <c r="L38" s="3">
-        <f t="shared" ref="L38" si="54">J38*K38</f>
+        <f t="shared" ref="L38" si="67">J38*K38</f>
         <v>0.55374999999999996</v>
       </c>
       <c r="M38" s="15">
-        <f>$N$1*K38</f>
+        <f t="shared" si="43"/>
         <v>100</v>
       </c>
       <c r="N38">
         <v>0</v>
       </c>
       <c r="O38">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>100</v>
       </c>
       <c r="P38">
-        <f>_xlfn.CEILING.MATH(O38/E38)</f>
+        <f t="shared" si="45"/>
         <v>100</v>
       </c>
       <c r="Q38" s="3">
-        <f>P38*I38</f>
+        <f t="shared" si="46"/>
         <v>11.074999999999999</v>
       </c>
       <c r="R38" s="15">
@@ -3497,23 +3510,23 @@
         <v>0.16</v>
       </c>
       <c r="U38" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>0.17092499999999999</v>
       </c>
       <c r="V38" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>1.920925</v>
       </c>
       <c r="W38" s="3">
-        <f>IF((R38&gt;0), V38/R38, J38)</f>
+        <f t="shared" si="47"/>
         <v>7.6837000000000003E-2</v>
       </c>
       <c r="X38" s="3">
-        <f>K38*W38</f>
+        <f t="shared" si="48"/>
         <v>0.384185</v>
       </c>
       <c r="Y38" s="3">
-        <f>L38-X38</f>
+        <f t="shared" si="49"/>
         <v>0.16956499999999997</v>
       </c>
       <c r="Z38" s="15"/>
@@ -3558,22 +3571,22 @@
         <v>0.14537250000000002</v>
       </c>
       <c r="M39" s="15">
-        <f>$N$1*K39</f>
+        <f t="shared" si="43"/>
         <v>20</v>
       </c>
       <c r="N39">
         <v>10</v>
       </c>
       <c r="O39">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>10</v>
       </c>
       <c r="P39">
-        <f>_xlfn.CEILING.MATH(O39/E39)</f>
+        <f t="shared" si="45"/>
         <v>10</v>
       </c>
       <c r="Q39" s="3">
-        <f>P39*I39</f>
+        <f t="shared" si="46"/>
         <v>1.4537250000000002</v>
       </c>
       <c r="R39" s="15">
@@ -3586,23 +3599,23 @@
         <v>0.3</v>
       </c>
       <c r="U39" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>0.32142500000000002</v>
       </c>
       <c r="V39" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>3.6114250000000001</v>
       </c>
       <c r="W39" s="3">
-        <f>IF((R39&gt;0), V39/R39, J39)</f>
+        <f t="shared" si="47"/>
         <v>0.144457</v>
       </c>
       <c r="X39" s="3">
-        <f>K39*W39</f>
+        <f t="shared" si="48"/>
         <v>0.144457</v>
       </c>
       <c r="Y39" s="3">
-        <f>L39-X39</f>
+        <f t="shared" si="49"/>
         <v>9.1550000000001353E-4</v>
       </c>
       <c r="Z39" s="15"/>
@@ -3646,22 +3659,22 @@
         <v>1.7277</v>
       </c>
       <c r="M40" s="15">
-        <f>$N$1*K40</f>
+        <f t="shared" si="43"/>
         <v>40</v>
       </c>
       <c r="N40">
         <v>50</v>
       </c>
       <c r="O40">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="P40">
-        <f>_xlfn.CEILING.MATH(O40/E40)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Q40" s="3">
-        <f>P40*I40</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="R40" s="15">
@@ -3672,23 +3685,23 @@
       </c>
       <c r="T40" s="1"/>
       <c r="U40" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="V40" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="W40" s="3">
-        <f>IF((R40&gt;0), V40/R40, J40)</f>
+        <f t="shared" si="47"/>
         <v>0.86385000000000001</v>
       </c>
       <c r="X40" s="3">
-        <f>K40*W40</f>
+        <f t="shared" si="48"/>
         <v>1.7277</v>
       </c>
       <c r="Y40" s="3">
-        <f>L40-X40</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z40" s="15"/>
@@ -3713,41 +3726,41 @@
         <v>0</v>
       </c>
       <c r="H41" s="3">
-        <f t="shared" ref="H41" si="55">(D41+F41+G41)*0.1075</f>
+        <f t="shared" ref="H41" si="68">(D41+F41+G41)*0.1075</f>
         <v>0.13975000000000001</v>
       </c>
       <c r="I41" s="3">
-        <f t="shared" ref="I41" si="56">D41+F41+H41</f>
+        <f t="shared" ref="I41" si="69">D41+F41+H41</f>
         <v>1.4397500000000001</v>
       </c>
       <c r="J41" s="3">
-        <f t="shared" ref="J41" si="57">I41/E41</f>
+        <f t="shared" ref="J41" si="70">I41/E41</f>
         <v>0.71987500000000004</v>
       </c>
       <c r="K41">
         <v>2</v>
       </c>
       <c r="L41" s="3">
-        <f t="shared" ref="L41" si="58">J41*K41</f>
+        <f t="shared" ref="L41" si="71">J41*K41</f>
         <v>1.4397500000000001</v>
       </c>
       <c r="M41" s="15">
-        <f>$N$1*K41</f>
+        <f t="shared" si="43"/>
         <v>40</v>
       </c>
       <c r="N41">
         <v>0</v>
       </c>
       <c r="O41">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>40</v>
       </c>
       <c r="P41">
-        <f>_xlfn.CEILING.MATH(O41/E41)</f>
+        <f t="shared" si="45"/>
         <v>20</v>
       </c>
       <c r="Q41" s="3">
-        <f>P41*I41</f>
+        <f t="shared" si="46"/>
         <v>28.795000000000002</v>
       </c>
       <c r="R41" s="15">
@@ -3758,23 +3771,23 @@
       </c>
       <c r="T41" s="1"/>
       <c r="U41" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>2.4295</v>
       </c>
       <c r="V41" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>25.029500000000002</v>
       </c>
       <c r="W41" s="3">
-        <f>IF((R41&gt;0), V41/R41, J41)</f>
+        <f t="shared" si="47"/>
         <v>0.62573750000000006</v>
       </c>
       <c r="X41" s="3">
-        <f>K41*W41</f>
+        <f t="shared" si="48"/>
         <v>1.2514750000000001</v>
       </c>
       <c r="Y41" s="3">
-        <f>L41-X41</f>
+        <f t="shared" si="49"/>
         <v>0.18827499999999997</v>
       </c>
       <c r="Z41" s="15"/>
@@ -3799,41 +3812,41 @@
         <v>0</v>
       </c>
       <c r="H42" s="3">
-        <f t="shared" ref="H42" si="59">(D42+F42+G42)*0.1075</f>
+        <f t="shared" ref="H42" si="72">(D42+F42+G42)*0.1075</f>
         <v>5.0524999999999994E-2</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" ref="I42" si="60">D42+F42+H42</f>
+        <f t="shared" ref="I42" si="73">D42+F42+H42</f>
         <v>0.52052500000000002</v>
       </c>
       <c r="J42" s="3">
-        <f t="shared" ref="J42" si="61">I42/E42</f>
+        <f t="shared" ref="J42" si="74">I42/E42</f>
         <v>0.52052500000000002</v>
       </c>
       <c r="K42">
         <v>1</v>
       </c>
       <c r="L42" s="3">
-        <f t="shared" ref="L42" si="62">J42*K42</f>
+        <f t="shared" ref="L42" si="75">J42*K42</f>
         <v>0.52052500000000002</v>
       </c>
       <c r="M42" s="15">
-        <f>$N$1*K42</f>
+        <f t="shared" si="43"/>
         <v>20</v>
       </c>
       <c r="N42">
         <v>0</v>
       </c>
       <c r="O42">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>20</v>
       </c>
       <c r="P42">
-        <f>_xlfn.CEILING.MATH(O42/E42)</f>
+        <f t="shared" si="45"/>
         <v>20</v>
       </c>
       <c r="Q42" s="3">
-        <f>P42*I42</f>
+        <f t="shared" si="46"/>
         <v>10.410500000000001</v>
       </c>
       <c r="R42" s="15">
@@ -3844,23 +3857,23 @@
       </c>
       <c r="T42" s="1"/>
       <c r="U42" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>0.88580000000000003</v>
       </c>
       <c r="V42" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>9.1257999999999999</v>
       </c>
       <c r="W42" s="3">
-        <f>IF((R42&gt;0), V42/R42, J42)</f>
+        <f t="shared" si="47"/>
         <v>0.45628999999999997</v>
       </c>
       <c r="X42" s="3">
-        <f>K42*W42</f>
+        <f t="shared" si="48"/>
         <v>0.45628999999999997</v>
       </c>
       <c r="Y42" s="3">
-        <f>L42-X42</f>
+        <f t="shared" si="49"/>
         <v>6.4235000000000042E-2</v>
       </c>
       <c r="Z42" s="15"/>
@@ -3885,41 +3898,41 @@
         <v>0</v>
       </c>
       <c r="H43" s="3">
-        <f t="shared" ref="H43:H44" si="63">(D43+F43+G43)*0.1075</f>
+        <f t="shared" ref="H43:H44" si="76">(D43+F43+G43)*0.1075</f>
         <v>1.0750000000000001E-2</v>
       </c>
       <c r="I43" s="3">
-        <f t="shared" ref="I43:I44" si="64">D43+F43+H43</f>
+        <f t="shared" ref="I43:I44" si="77">D43+F43+H43</f>
         <v>0.11075</v>
       </c>
       <c r="J43" s="3">
-        <f t="shared" ref="J43:J44" si="65">I43/E43</f>
+        <f t="shared" ref="J43:J44" si="78">I43/E43</f>
         <v>0.11075</v>
       </c>
       <c r="K43">
         <v>1</v>
       </c>
       <c r="L43" s="3">
-        <f t="shared" ref="L43:L44" si="66">J43*K43</f>
+        <f t="shared" ref="L43:L44" si="79">J43*K43</f>
         <v>0.11075</v>
       </c>
       <c r="M43" s="15">
-        <f>$N$1*K43</f>
+        <f t="shared" si="43"/>
         <v>20</v>
       </c>
       <c r="N43">
         <v>10</v>
       </c>
       <c r="O43">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>10</v>
       </c>
       <c r="P43">
-        <f>_xlfn.CEILING.MATH(O43/E43)</f>
+        <f t="shared" si="45"/>
         <v>10</v>
       </c>
       <c r="Q43" s="3">
-        <f>P43*I43</f>
+        <f t="shared" si="46"/>
         <v>1.1074999999999999</v>
       </c>
       <c r="R43" s="15">
@@ -3930,23 +3943,23 @@
       </c>
       <c r="T43" s="1"/>
       <c r="U43" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>0.10965</v>
       </c>
       <c r="V43" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>1.12965</v>
       </c>
       <c r="W43" s="3">
-        <f>IF((R43&gt;0), V43/R43, J43)</f>
+        <f t="shared" si="47"/>
         <v>4.5186000000000004E-2</v>
       </c>
       <c r="X43" s="3">
-        <f>K43*W43</f>
+        <f t="shared" si="48"/>
         <v>4.5186000000000004E-2</v>
       </c>
       <c r="Y43" s="3">
-        <f>L43-X43</f>
+        <f t="shared" si="49"/>
         <v>6.5563999999999997E-2</v>
       </c>
       <c r="Z43" s="15"/>
@@ -3971,41 +3984,41 @@
         <v>0</v>
       </c>
       <c r="H44" s="3">
-        <f t="shared" si="63"/>
+        <f t="shared" si="76"/>
         <v>0.23005</v>
       </c>
       <c r="I44" s="3">
-        <f t="shared" si="64"/>
+        <f t="shared" si="77"/>
         <v>2.37005</v>
       </c>
       <c r="J44" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="78"/>
         <v>0.23700499999999999</v>
       </c>
       <c r="K44">
         <v>10</v>
       </c>
       <c r="L44" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="79"/>
         <v>2.37005</v>
       </c>
       <c r="M44" s="15">
-        <f>$N$1*K44</f>
+        <f t="shared" si="43"/>
         <v>200</v>
       </c>
       <c r="N44">
         <v>0</v>
       </c>
       <c r="O44">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>200</v>
       </c>
       <c r="P44">
-        <f>_xlfn.CEILING.MATH(O44/E44)</f>
+        <f t="shared" si="45"/>
         <v>20</v>
       </c>
       <c r="Q44" s="3">
-        <f>P44*I44</f>
+        <f t="shared" si="46"/>
         <v>47.400999999999996</v>
       </c>
       <c r="R44" s="15">
@@ -4018,23 +4031,23 @@
         <v>2.27</v>
       </c>
       <c r="U44" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>2.4402499999999998</v>
       </c>
       <c r="V44" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>27.410249999999998</v>
       </c>
       <c r="W44" s="3">
-        <f>IF((R44&gt;0), V44/R44, J44)</f>
+        <f t="shared" si="47"/>
         <v>0.13705124999999999</v>
       </c>
       <c r="X44" s="3">
-        <f>K44*W44</f>
+        <f t="shared" si="48"/>
         <v>1.3705124999999998</v>
       </c>
       <c r="Y44" s="3">
-        <f>L44-X44</f>
+        <f t="shared" si="49"/>
         <v>0.99953750000000019</v>
       </c>
       <c r="Z44" s="15"/>
@@ -4059,41 +4072,41 @@
         <v>0</v>
       </c>
       <c r="H45" s="3">
-        <f t="shared" ref="H45" si="67">(D45+F45+G45)*0.1075</f>
+        <f t="shared" ref="H45" si="80">(D45+F45+G45)*0.1075</f>
         <v>0.12362499999999998</v>
       </c>
       <c r="I45" s="3">
-        <f t="shared" ref="I45" si="68">D45+F45+H45</f>
+        <f t="shared" ref="I45" si="81">D45+F45+H45</f>
         <v>1.273625</v>
       </c>
       <c r="J45" s="3">
-        <f t="shared" ref="J45" si="69">I45/E45</f>
+        <f t="shared" ref="J45" si="82">I45/E45</f>
         <v>0.25472499999999998</v>
       </c>
       <c r="K45">
         <v>5</v>
       </c>
       <c r="L45" s="3">
-        <f t="shared" ref="L45" si="70">J45*K45</f>
+        <f t="shared" ref="L45" si="83">J45*K45</f>
         <v>1.273625</v>
       </c>
       <c r="M45" s="15">
-        <f>$N$1*K45</f>
+        <f t="shared" si="43"/>
         <v>100</v>
       </c>
       <c r="N45">
         <v>10</v>
       </c>
       <c r="O45">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>90</v>
       </c>
       <c r="P45">
-        <f>_xlfn.CEILING.MATH(O45/E45)</f>
+        <f t="shared" si="45"/>
         <v>18</v>
       </c>
       <c r="Q45" s="3">
-        <f>P45*I45</f>
+        <f t="shared" si="46"/>
         <v>22.925249999999998</v>
       </c>
       <c r="R45" s="15">
@@ -4106,23 +4119,23 @@
         <v>0.87</v>
       </c>
       <c r="U45" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>0.93847500000000006</v>
       </c>
       <c r="V45" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>10.538475</v>
       </c>
       <c r="W45" s="3">
-        <f>IF((R45&gt;0), V45/R45, J45)</f>
+        <f t="shared" si="47"/>
         <v>9.5804318181818185E-2</v>
       </c>
       <c r="X45" s="3">
-        <f>K45*W45</f>
+        <f t="shared" si="48"/>
         <v>0.47902159090909091</v>
       </c>
       <c r="Y45" s="3">
-        <f>L45-X45</f>
+        <f t="shared" si="49"/>
         <v>0.7946034090909091</v>
       </c>
       <c r="Z45" s="15"/>
@@ -4167,22 +4180,22 @@
         <v>1.587915</v>
       </c>
       <c r="M46" s="15">
-        <f>$N$1*K46</f>
+        <f t="shared" si="43"/>
         <v>40</v>
       </c>
       <c r="N46">
         <v>0</v>
       </c>
       <c r="O46">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>40</v>
       </c>
       <c r="P46">
-        <f>_xlfn.CEILING.MATH(O46/E46)</f>
+        <f t="shared" si="45"/>
         <v>20</v>
       </c>
       <c r="Q46" s="3">
-        <f>P46*I46</f>
+        <f t="shared" si="46"/>
         <v>31.758299999999998</v>
       </c>
       <c r="R46" s="15">
@@ -4193,23 +4206,23 @@
       </c>
       <c r="T46" s="1"/>
       <c r="U46" s="3">
-        <f t="shared" si="37"/>
+        <f t="shared" si="50"/>
         <v>3.0422500000000001</v>
       </c>
       <c r="V46" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>31.34225</v>
       </c>
       <c r="W46" s="3">
-        <f>IF((R46&gt;0), V46/R46, J46)</f>
+        <f t="shared" si="47"/>
         <v>0.62684499999999999</v>
       </c>
       <c r="X46" s="3">
-        <f>K46*W46</f>
+        <f t="shared" si="48"/>
         <v>1.25369</v>
       </c>
       <c r="Y46" s="3">
-        <f>L46-X46</f>
+        <f t="shared" si="49"/>
         <v>0.33422499999999999</v>
       </c>
       <c r="Z46" s="15"/>
@@ -4251,22 +4264,22 @@
         <v>0.24950000000000003</v>
       </c>
       <c r="M47" s="15">
-        <f>$N$1*K47</f>
+        <f t="shared" si="43"/>
         <v>1</v>
       </c>
       <c r="N47">
         <v>0</v>
       </c>
       <c r="O47">
-        <f t="shared" si="36"/>
+        <f t="shared" si="44"/>
         <v>1</v>
       </c>
       <c r="P47">
-        <f>_xlfn.CEILING.MATH(O47/E47)</f>
+        <f t="shared" si="45"/>
         <v>1</v>
       </c>
       <c r="Q47" s="3">
-        <f>P47*I47</f>
+        <f t="shared" si="46"/>
         <v>4.99</v>
       </c>
       <c r="R47" s="15">
@@ -4282,11 +4295,11 @@
         <v>0</v>
       </c>
       <c r="V47" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>6.99</v>
       </c>
       <c r="W47" s="3">
-        <f>IF((R47&gt;0), V47/R47, J47)</f>
+        <f t="shared" si="47"/>
         <v>6.99</v>
       </c>
       <c r="X47" s="3">
@@ -4294,7 +4307,7 @@
         <v>0.34950000000000003</v>
       </c>
       <c r="Y47" s="3">
-        <f>L47-X47</f>
+        <f t="shared" si="49"/>
         <v>-0.1</v>
       </c>
       <c r="Z47" s="15"/>
@@ -4345,11 +4358,11 @@
         <v>120</v>
       </c>
       <c r="O48" s="4">
-        <f t="shared" ref="O48:P48" si="71">SUM(O29:O46)</f>
+        <f t="shared" ref="O48:P48" si="84">SUM(O29:O46)</f>
         <v>1010</v>
       </c>
       <c r="P48" s="4">
-        <f t="shared" si="71"/>
+        <f t="shared" si="84"/>
         <v>592</v>
       </c>
       <c r="Q48" s="8">
@@ -4361,31 +4374,31 @@
         <v>1026</v>
       </c>
       <c r="S48" s="6">
-        <f t="shared" ref="S48:Y48" si="72">SUM(S29:S47)</f>
+        <f t="shared" ref="S48:Y48" si="85">SUM(S29:S47)</f>
         <v>165.21</v>
       </c>
       <c r="T48" s="6">
-        <f t="shared" si="72"/>
+        <f t="shared" si="85"/>
         <v>7.5100000000000007</v>
       </c>
       <c r="U48" s="6">
-        <f t="shared" si="72"/>
+        <f t="shared" si="85"/>
         <v>17.008649999999999</v>
       </c>
       <c r="V48" s="6">
-        <f t="shared" si="72"/>
+        <f t="shared" si="85"/>
         <v>189.72864999999999</v>
       </c>
       <c r="W48" s="6">
-        <f t="shared" si="72"/>
+        <f t="shared" si="85"/>
         <v>13.68309300151515</v>
       </c>
       <c r="X48" s="6">
-        <f t="shared" si="72"/>
+        <f t="shared" si="85"/>
         <v>12.097905324242422</v>
       </c>
       <c r="Y48" s="6">
-        <f t="shared" si="72"/>
+        <f t="shared" si="85"/>
         <v>5.6164296757575771</v>
       </c>
       <c r="Z48" s="25"/>
@@ -4440,18 +4453,18 @@
         <v>0</v>
       </c>
       <c r="I51" s="3">
-        <f t="shared" ref="I51" si="73">D51+F51+H51</f>
+        <f t="shared" ref="I51" si="86">D51+F51+H51</f>
         <v>60.55</v>
       </c>
       <c r="J51" s="3">
-        <f t="shared" ref="J51" si="74">I51/E51</f>
+        <f t="shared" ref="J51" si="87">I51/E51</f>
         <v>3.0274999999999999</v>
       </c>
       <c r="K51">
         <v>1</v>
       </c>
       <c r="L51" s="3">
-        <f t="shared" ref="L51" si="75">J51*K51</f>
+        <f t="shared" ref="L51" si="88">J51*K51</f>
         <v>3.0274999999999999</v>
       </c>
       <c r="M51" s="15">
@@ -4486,11 +4499,11 @@
         <v>0</v>
       </c>
       <c r="V51" s="1">
-        <f t="shared" ref="V51" si="76">SUM(S51:U51)</f>
+        <f t="shared" ref="V51" si="89">SUM(S51:U51)</f>
         <v>60.55</v>
       </c>
       <c r="W51" s="1">
-        <f t="shared" ref="W51" si="77">V51/R51</f>
+        <f t="shared" ref="W51" si="90">V51/R51</f>
         <v>3.0274999999999999</v>
       </c>
       <c r="X51" s="1">
@@ -4512,83 +4525,83 @@
         <v>30.66</v>
       </c>
       <c r="F52" s="6">
-        <f t="shared" ref="F52:L52" si="78">SUM(F51:F51)</f>
+        <f t="shared" ref="F52:L52" si="91">SUM(F51:F51)</f>
         <v>29.89</v>
       </c>
       <c r="G52" s="6">
-        <f t="shared" si="78"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="H52" s="6">
-        <f t="shared" si="78"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="I52" s="6">
-        <f t="shared" si="78"/>
+        <f t="shared" si="91"/>
         <v>60.55</v>
       </c>
       <c r="J52" s="6">
-        <f t="shared" si="78"/>
+        <f t="shared" si="91"/>
         <v>3.0274999999999999</v>
       </c>
       <c r="K52" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="91"/>
         <v>1</v>
       </c>
       <c r="L52" s="6">
-        <f t="shared" si="78"/>
+        <f t="shared" si="91"/>
         <v>3.0274999999999999</v>
       </c>
       <c r="M52" s="17">
-        <f t="shared" ref="M52:R52" si="79">SUM(M51:M51)</f>
+        <f t="shared" ref="M52:R52" si="92">SUM(M51:M51)</f>
         <v>20</v>
       </c>
       <c r="N52" s="4">
-        <f t="shared" si="79"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="O52" s="4">
-        <f t="shared" si="79"/>
+        <f t="shared" si="92"/>
         <v>20</v>
       </c>
       <c r="P52" s="4">
-        <f t="shared" si="79"/>
+        <f t="shared" si="92"/>
         <v>1</v>
       </c>
       <c r="Q52" s="6">
-        <f t="shared" si="79"/>
+        <f t="shared" si="92"/>
         <v>60.55</v>
       </c>
       <c r="R52" s="17">
-        <f t="shared" si="79"/>
+        <f t="shared" si="92"/>
         <v>20</v>
       </c>
       <c r="S52" s="6">
-        <f t="shared" ref="S52:Y52" si="80">SUM(S51:S51)</f>
+        <f t="shared" ref="S52:Y52" si="93">SUM(S51:S51)</f>
         <v>60.55</v>
       </c>
       <c r="T52" s="6">
-        <f t="shared" si="80"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="U52" s="6">
-        <f t="shared" si="80"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="V52" s="6">
-        <f t="shared" si="80"/>
+        <f t="shared" si="93"/>
         <v>60.55</v>
       </c>
       <c r="W52" s="6">
-        <f t="shared" si="80"/>
+        <f t="shared" si="93"/>
         <v>3.0274999999999999</v>
       </c>
       <c r="X52" s="6">
-        <f t="shared" si="80"/>
+        <f t="shared" si="93"/>
         <v>3.0274999999999999</v>
       </c>
       <c r="Y52" s="6">
-        <f t="shared" si="80"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="Z52" s="15"/>
@@ -4614,55 +4627,55 @@
         <v>36</v>
       </c>
       <c r="D54" s="22">
-        <f t="shared" ref="D54:L54" si="81">D15+D19+D26+D48+D52</f>
+        <f t="shared" ref="D54:L54" si="94">D15+D19+D26+D48+D52</f>
         <v>167.01</v>
       </c>
       <c r="E54" s="8">
-        <f t="shared" si="81"/>
+        <f t="shared" si="94"/>
         <v>1</v>
       </c>
       <c r="F54" s="8">
-        <f t="shared" si="81"/>
+        <f t="shared" si="94"/>
         <v>34.880000000000003</v>
       </c>
       <c r="G54" s="8">
-        <f t="shared" si="81"/>
+        <f t="shared" si="94"/>
         <v>0.40800000000000003</v>
       </c>
       <c r="H54" s="8">
-        <f t="shared" si="81"/>
+        <f t="shared" si="94"/>
         <v>1.7649350000000001</v>
       </c>
       <c r="I54" s="8">
-        <f t="shared" si="81"/>
+        <f t="shared" si="94"/>
         <v>211.60148499999997</v>
       </c>
       <c r="J54" s="8">
-        <f t="shared" si="81"/>
+        <f t="shared" si="94"/>
         <v>18.647795000000002</v>
       </c>
       <c r="K54" s="9">
-        <f t="shared" si="81"/>
+        <f t="shared" si="94"/>
         <v>83</v>
       </c>
       <c r="L54" s="8">
-        <f t="shared" si="81"/>
+        <f t="shared" si="94"/>
         <v>50.351531750000007</v>
       </c>
       <c r="M54" s="24">
-        <f t="shared" ref="M54:P54" si="82">M15+M19+M26+M48+M52</f>
+        <f t="shared" ref="M54:P54" si="95">M15+M19+M26+M48+M52</f>
         <v>1661</v>
       </c>
       <c r="N54" s="9">
-        <f t="shared" si="82"/>
+        <f t="shared" si="95"/>
         <v>298</v>
       </c>
       <c r="O54" s="9">
-        <f t="shared" si="82"/>
+        <f t="shared" si="95"/>
         <v>1402</v>
       </c>
       <c r="P54" s="9">
-        <f t="shared" si="82"/>
+        <f t="shared" si="95"/>
         <v>731</v>
       </c>
       <c r="Q54" s="8">
@@ -4670,35 +4683,35 @@
         <v>884.63789999999995</v>
       </c>
       <c r="R54" s="24">
-        <f t="shared" ref="R54:Y54" si="83">R15+R19+R26+R48+R52</f>
+        <f t="shared" ref="R54:Y54" si="96">R15+R19+R26+R48+R52</f>
         <v>1618</v>
       </c>
       <c r="S54" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="96"/>
         <v>706.41000000000008</v>
       </c>
       <c r="T54" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="96"/>
         <v>7.5100000000000007</v>
       </c>
       <c r="U54" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="96"/>
         <v>67.258650000000003</v>
       </c>
       <c r="V54" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="96"/>
         <v>781.17864999999995</v>
       </c>
       <c r="W54" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="96"/>
         <v>46.295648102392335</v>
       </c>
       <c r="X54" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="96"/>
         <v>45.973225175119623</v>
       </c>
       <c r="Y54" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="96"/>
         <v>4.6278065748803847</v>
       </c>
       <c r="Z54" s="15"/>

</xml_diff>

<commit_message>
Received final parts for Make & Take kits.
</commit_message>
<xml_diff>
--- a/parts/bill_of_materials.xlsx
+++ b/parts/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\laser_tunnel\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365C360E-49A4-48C9-B9D2-A501179332B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7AE4E7-5AE5-4FE7-B094-BC13AA200A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C7A15FB5-B248-4CA2-8E4B-B85C1BCDD779}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="100">
   <si>
     <t>Laser Tunnel</t>
   </si>
@@ -438,7 +438,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -467,10 +467,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -787,13 +788,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A265784A-A2E2-4F2C-B0D4-276F819350E1}">
-  <dimension ref="A1:Z57"/>
+  <dimension ref="A1:AB57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z17" sqref="Z17"/>
+      <selection pane="bottomRight" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -821,7 +822,7 @@
     <col min="24" max="24" width="10.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -835,11 +836,17 @@
       <c r="R1" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="Z1" s="27">
+      <c r="Z1" s="26">
         <v>44612</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="AA1" s="28">
+        <v>44613</v>
+      </c>
+      <c r="AB1" s="28">
+        <v>44614</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
         <v>62</v>
       </c>
@@ -918,8 +925,14 @@
       <c r="Z2" s="16" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="AA2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
@@ -928,7 +941,7 @@
       <c r="R3" s="15"/>
       <c r="Z3" s="15"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B4" s="12" t="s">
         <v>69</v>
       </c>
@@ -1018,7 +1031,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1105,8 +1118,11 @@
         <v>-3.3107499999999956E-2</v>
       </c>
       <c r="Z5" s="15"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>65</v>
       </c>
@@ -1196,7 +1212,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -1283,8 +1299,11 @@
         <v>7.8500000000009118E-5</v>
       </c>
       <c r="Z7" s="15"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -1373,8 +1392,11 @@
       <c r="Z8" s="15">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>45</v>
       </c>
@@ -1464,7 +1486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>15</v>
       </c>
@@ -1552,7 +1574,7 @@
       </c>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -1640,7 +1662,7 @@
       </c>
       <c r="Z11" s="15"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>70</v>
       </c>
@@ -1727,8 +1749,11 @@
         <v>-6.9750000000035062E-5</v>
       </c>
       <c r="Z12" s="15"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>71</v>
       </c>
@@ -1816,7 +1841,7 @@
       </c>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -1904,7 +1929,7 @@
       </c>
       <c r="Z14" s="15"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
@@ -1983,7 +2008,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B16" s="4"/>
       <c r="C16" s="2"/>
       <c r="D16" s="21"/>
@@ -1997,7 +2022,7 @@
       <c r="R16" s="15"/>
       <c r="Z16" s="15"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>63</v>
       </c>
@@ -2006,7 +2031,7 @@
       <c r="R17" s="15"/>
       <c r="Z17" s="15"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>18</v>
       </c>
@@ -2060,17 +2085,22 @@
         <f>P18*I18</f>
         <v>39.427</v>
       </c>
-      <c r="R18" s="15"/>
+      <c r="R18" s="15">
+        <v>20</v>
+      </c>
+      <c r="S18">
+        <v>35.6</v>
+      </c>
       <c r="T18" s="1">
         <v>0</v>
       </c>
       <c r="U18" s="3">
         <f>S18*0.1075</f>
-        <v>0</v>
+        <v>3.827</v>
       </c>
       <c r="V18" s="3">
         <f>SUM(S18:U18)</f>
-        <v>0</v>
+        <v>39.427</v>
       </c>
       <c r="W18" s="3">
         <f>IF((R18&gt;0), V18/R18, J18)</f>
@@ -2085,8 +2115,11 @@
         <v>0</v>
       </c>
       <c r="Z18" s="15"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>64</v>
       </c>
@@ -2150,11 +2183,11 @@
       </c>
       <c r="R19" s="23">
         <f>SUM(R18:R18)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S19" s="6">
         <f t="shared" ref="S19:Y19" si="28">SUM(S18:S18)</f>
-        <v>0</v>
+        <v>35.6</v>
       </c>
       <c r="T19" s="6">
         <f t="shared" si="28"/>
@@ -2162,11 +2195,11 @@
       </c>
       <c r="U19" s="6">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>3.827</v>
       </c>
       <c r="V19" s="6">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>39.427</v>
       </c>
       <c r="W19" s="6">
         <f t="shared" si="28"/>
@@ -2182,7 +2215,7 @@
       </c>
       <c r="Z19" s="15"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.4">
       <c r="D20" s="20"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -2193,7 +2226,7 @@
       <c r="R20" s="15"/>
       <c r="Z20" s="15"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>36</v>
       </c>
@@ -2210,7 +2243,7 @@
       <c r="R21" s="15"/>
       <c r="Z21" s="15"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
         <v>93</v>
       </c>
@@ -2296,7 +2329,7 @@
       </c>
       <c r="Z22" s="15"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>94</v>
       </c>
@@ -2382,7 +2415,7 @@
       </c>
       <c r="Z23" s="15"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>95</v>
       </c>
@@ -2468,7 +2501,7 @@
       </c>
       <c r="Z24" s="15"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>96</v>
       </c>
@@ -2554,7 +2587,7 @@
       </c>
       <c r="Z25" s="15"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>40</v>
       </c>
@@ -2630,7 +2663,7 @@
       </c>
       <c r="Z26" s="15"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.4">
       <c r="D27" s="20"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -2641,7 +2674,7 @@
       <c r="R27" s="15"/>
       <c r="Z27" s="15"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>33</v>
       </c>
@@ -2658,7 +2691,7 @@
       <c r="R28" s="15"/>
       <c r="Z28" s="15"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>37</v>
       </c>
@@ -2746,8 +2779,11 @@
         <v>5.4835000000000078E-2</v>
       </c>
       <c r="Z29" s="15"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>13</v>
       </c>
@@ -2835,8 +2871,11 @@
         <v>1.151046</v>
       </c>
       <c r="Z30" s="15"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB30">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>20</v>
       </c>
@@ -2921,8 +2960,11 @@
         <v>0.13733000000000006</v>
       </c>
       <c r="Z31" s="15"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>34</v>
       </c>
@@ -3010,8 +3052,11 @@
         <v>0.11987166666666682</v>
       </c>
       <c r="Z32" s="15"/>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>30</v>
       </c>
@@ -3096,8 +3141,11 @@
         <v>0.11850250000000001</v>
       </c>
       <c r="Z33" s="15"/>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
         <v>31</v>
       </c>
@@ -3182,8 +3230,11 @@
         <v>0.79660260000000005</v>
       </c>
       <c r="Z34" s="15"/>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB34">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>32</v>
       </c>
@@ -3268,8 +3319,11 @@
         <v>0.140874</v>
       </c>
       <c r="Z35" s="15"/>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>56</v>
       </c>
@@ -3354,8 +3408,11 @@
         <v>0.41088249999999993</v>
       </c>
       <c r="Z36" s="15"/>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>57</v>
       </c>
@@ -3442,8 +3499,11 @@
         <v>0.16956499999999997</v>
       </c>
       <c r="Z37" s="15"/>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB37">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>58</v>
       </c>
@@ -3530,8 +3590,11 @@
         <v>0.16956499999999997</v>
       </c>
       <c r="Z38" s="15"/>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB38">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -3619,8 +3682,11 @@
         <v>9.1550000000001353E-4</v>
       </c>
       <c r="Z39" s="15"/>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB39">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>49</v>
       </c>
@@ -3706,7 +3772,7 @@
       </c>
       <c r="Z40" s="15"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>48</v>
       </c>
@@ -3791,8 +3857,11 @@
         <v>0.18827499999999997</v>
       </c>
       <c r="Z41" s="15"/>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>59</v>
       </c>
@@ -3877,8 +3946,11 @@
         <v>6.4235000000000042E-2</v>
       </c>
       <c r="Z42" s="15"/>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
         <v>50</v>
       </c>
@@ -3963,8 +4035,11 @@
         <v>6.5563999999999997E-2</v>
       </c>
       <c r="Z43" s="15"/>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB43">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
         <v>60</v>
       </c>
@@ -4051,8 +4126,11 @@
         <v>0.99953750000000019</v>
       </c>
       <c r="Z44" s="15"/>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB44">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
         <v>61</v>
       </c>
@@ -4139,8 +4217,11 @@
         <v>0.7946034090909091</v>
       </c>
       <c r="Z45" s="15"/>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
         <v>23</v>
       </c>
@@ -4226,8 +4307,11 @@
         <v>0.33422499999999999</v>
       </c>
       <c r="Z46" s="15"/>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AB46">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B47" s="11" t="s">
         <v>2</v>
       </c>
@@ -4311,8 +4395,11 @@
         <v>-0.1</v>
       </c>
       <c r="Z47" s="15"/>
-    </row>
-    <row r="48" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="AB47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>41</v>
       </c>
@@ -4403,7 +4490,7 @@
       </c>
       <c r="Z48" s="25"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.4">
       <c r="B49" s="4"/>
       <c r="C49" s="2"/>
       <c r="D49" s="20"/>
@@ -4416,7 +4503,7 @@
       <c r="R49" s="15"/>
       <c r="Z49" s="15"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A50" s="4" t="s">
         <v>43</v>
       </c>
@@ -4431,7 +4518,7 @@
       <c r="R50" s="15"/>
       <c r="Z50" s="15"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.4">
       <c r="B51" s="5" t="s">
         <v>47</v>
       </c>
@@ -4515,8 +4602,11 @@
         <v>0</v>
       </c>
       <c r="Z51" s="15"/>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AA51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A52" s="4" t="s">
         <v>44</v>
       </c>
@@ -4606,7 +4696,7 @@
       </c>
       <c r="Z52" s="15"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.4">
       <c r="B53" s="4"/>
       <c r="D53" s="20"/>
       <c r="G53" s="3"/>
@@ -4618,7 +4708,7 @@
       <c r="R53" s="15"/>
       <c r="Z53" s="15"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A54" s="4" t="s">
         <v>42</v>
       </c>
@@ -4684,11 +4774,11 @@
       </c>
       <c r="R54" s="24">
         <f t="shared" ref="R54:Y54" si="96">R15+R19+R26+R48+R52</f>
-        <v>1618</v>
+        <v>1638</v>
       </c>
       <c r="S54" s="8">
         <f t="shared" si="96"/>
-        <v>706.41000000000008</v>
+        <v>742.0100000000001</v>
       </c>
       <c r="T54" s="8">
         <f t="shared" si="96"/>
@@ -4696,11 +4786,11 @@
       </c>
       <c r="U54" s="8">
         <f t="shared" si="96"/>
-        <v>67.258650000000003</v>
+        <v>71.085650000000001</v>
       </c>
       <c r="V54" s="8">
         <f t="shared" si="96"/>
-        <v>781.17864999999995</v>
+        <v>820.60564999999997</v>
       </c>
       <c r="W54" s="8">
         <f t="shared" si="96"/>
@@ -4716,17 +4806,17 @@
       </c>
       <c r="Z54" s="15"/>
     </row>
-    <row r="56" spans="1:26" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="26" t="s">
+    <row r="56" spans="1:27" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="26"/>
-    </row>
-    <row r="57" spans="1:26" ht="67.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="26" t="s">
+      <c r="B56" s="27"/>
+    </row>
+    <row r="57" spans="1:27" ht="67.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="26"/>
+      <c r="B57" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Updated BOM to reflect items received.
</commit_message>
<xml_diff>
--- a/parts/bill_of_materials.xlsx
+++ b/parts/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\laser_tunnel\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7AE4E7-5AE5-4FE7-B094-BC13AA200A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229C3AE6-B481-48FD-A9FC-08EB22E689BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C7A15FB5-B248-4CA2-8E4B-B85C1BCDD779}"/>
   </bookViews>
@@ -467,11 +467,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -791,10 +791,10 @@
   <dimension ref="A1:AB57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AC2" sqref="AC2"/>
+      <selection pane="bottomRight" activeCell="AB26" sqref="AB26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -836,13 +836,13 @@
       <c r="R1" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="Z1" s="26">
+      <c r="Z1" s="28">
         <v>44612</v>
       </c>
-      <c r="AA1" s="28">
+      <c r="AA1" s="26">
         <v>44613</v>
       </c>
-      <c r="AB1" s="28">
+      <c r="AB1" s="26">
         <v>44614</v>
       </c>
     </row>
@@ -2328,6 +2328,9 @@
         <v>-0.56999999999999995</v>
       </c>
       <c r="Z22" s="15"/>
+      <c r="AB22">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
@@ -2414,6 +2417,9 @@
         <v>-0.03</v>
       </c>
       <c r="Z23" s="15"/>
+      <c r="AB23">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
@@ -2500,6 +2506,9 @@
         <v>-0.03</v>
       </c>
       <c r="Z24" s="15"/>
+      <c r="AB24">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
@@ -2586,6 +2595,9 @@
         <v>-0.03</v>
       </c>
       <c r="Z25" s="15"/>
+      <c r="AB25">
+        <v>3</v>
+      </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">

</xml_diff>

<commit_message>
Updated bill of materials to switch Arduino Pro Mini version.
The cheaper ones from Hiletgo were unreliable to the voltage regulators.
Ended up switching to the actual SparkFun ones.  Unfortunately, those
may still take a few days to arrive, and the up the kit price by $4.

Fortunately, I figured out how to continue to develop the software
using an old Pro Mini with a blown voltage regulator:  I clipped off the
RAW pin on the Pro Mini and keep it connected to the FTDI cable.  That
way the Pro Mini (and other things powered by its VCC) get their 5V from
the USB hub, bypassing the voltage regulator.  Since we need the 12V for
the fan, that can be powered from the jack on the board (as intended).
</commit_message>
<xml_diff>
--- a/parts/bill_of_materials.xlsx
+++ b/parts/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\laser_tunnel\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229C3AE6-B481-48FD-A9FC-08EB22E689BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE1FA46-BBAB-4C26-9001-36F5C5FE0600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C7A15FB5-B248-4CA2-8E4B-B85C1BCDD779}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>https://www.amazon.com/gp/product/B014Q7AVKG</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B07X2JGS69</t>
-  </si>
-  <si>
     <t>5V 16MHz Arduino Pro Mini</t>
   </si>
   <si>
@@ -332,6 +329,9 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B004G53J5I</t>
   </si>
 </sst>
 </file>
@@ -468,10 +468,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -791,10 +791,10 @@
   <dimension ref="A1:AB57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AB26" sqref="AB26"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -828,15 +828,15 @@
       </c>
       <c r="D1" s="15"/>
       <c r="M1" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N1" s="18">
         <v>20</v>
       </c>
       <c r="R1" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z1" s="28">
+        <v>90</v>
+      </c>
+      <c r="Z1" s="27">
         <v>44612</v>
       </c>
       <c r="AA1" s="26">
@@ -848,7 +848,7 @@
     </row>
     <row r="2" spans="1:28" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>1</v>
@@ -857,84 +857,84 @@
         <v>4</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="M2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>28</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>29</v>
       </c>
       <c r="U2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="V2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="W2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="14" t="s">
+      <c r="X2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="X2" s="14" t="s">
-        <v>27</v>
-      </c>
       <c r="Y2" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Z2" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA2" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AB2" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="15"/>
       <c r="M3" s="15"/>
@@ -943,7 +943,7 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B4" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -1214,10 +1214,10 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="20">
         <v>5.99</v>
@@ -1305,10 +1305,10 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
         <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="D8" s="20">
         <v>18.989999999999998</v>
@@ -1346,62 +1346,58 @@
         <v>20</v>
       </c>
       <c r="N8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <f t="shared" si="10"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="P8">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q8" s="3">
         <f t="shared" si="5"/>
-        <v>126.18854999999999</v>
+        <v>147.21997499999998</v>
       </c>
       <c r="R8" s="15">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="S8" s="1">
-        <v>116.94</v>
+        <f>9.95*20</f>
+        <v>199</v>
       </c>
       <c r="T8" s="1">
         <v>0</v>
       </c>
       <c r="U8" s="3">
         <f t="shared" si="11"/>
-        <v>12.57</v>
+        <v>21.39</v>
       </c>
       <c r="V8" s="3">
         <f t="shared" si="12"/>
-        <v>129.51</v>
+        <v>220.39</v>
       </c>
       <c r="W8" s="3">
         <f t="shared" si="6"/>
-        <v>7.1949999999999994</v>
+        <v>11.019499999999999</v>
       </c>
       <c r="X8" s="3">
         <f t="shared" si="7"/>
-        <v>7.1949999999999994</v>
+        <v>11.019499999999999</v>
       </c>
       <c r="Y8" s="3">
         <f t="shared" si="8"/>
-        <v>-0.18452499999999983</v>
-      </c>
-      <c r="Z8" s="15">
-        <v>15</v>
-      </c>
-      <c r="AB8">
-        <v>3</v>
-      </c>
+        <v>-4.0090249999999994</v>
+      </c>
+      <c r="Z8" s="15"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D9" s="20">
         <v>12.99</v>
@@ -1488,10 +1484,10 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="20">
         <v>14.49</v>
@@ -1576,10 +1572,10 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="20">
         <v>7.49</v>
@@ -1664,10 +1660,10 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="20">
         <v>10.49</v>
@@ -1755,10 +1751,10 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="20">
         <v>6.98</v>
@@ -1843,10 +1839,10 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
         <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
       </c>
       <c r="D14" s="20">
         <v>18.989999999999998</v>
@@ -1931,7 +1927,7 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="21">
@@ -1958,27 +1954,27 @@
       </c>
       <c r="N15" s="10">
         <f t="shared" si="20"/>
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="O15" s="10">
         <f t="shared" si="20"/>
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="P15" s="10">
         <f t="shared" si="20"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q15" s="6">
         <f t="shared" si="20"/>
-        <v>510.94512500000002</v>
+        <v>531.97654999999997</v>
       </c>
       <c r="R15" s="23">
         <f t="shared" si="20"/>
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="S15" s="6">
         <f t="shared" si="20"/>
-        <v>467.4500000000001</v>
+        <v>549.5100000000001</v>
       </c>
       <c r="T15" s="6">
         <f t="shared" si="20"/>
@@ -1986,23 +1982,23 @@
       </c>
       <c r="U15" s="6">
         <f t="shared" si="20"/>
-        <v>50.250000000000007</v>
+        <v>59.070000000000007</v>
       </c>
       <c r="V15" s="6">
         <f t="shared" si="20"/>
-        <v>517.69999999999993</v>
+        <v>608.57999999999993</v>
       </c>
       <c r="W15" s="6">
         <f t="shared" si="20"/>
-        <v>26.953705100877187</v>
+        <v>30.778205100877187</v>
       </c>
       <c r="X15" s="6">
         <f t="shared" si="20"/>
-        <v>28.216469850877196</v>
+        <v>32.040969850877197</v>
       </c>
       <c r="Y15" s="6">
         <f t="shared" si="20"/>
-        <v>-0.32862310087719243</v>
+        <v>-4.1531231008771918</v>
       </c>
       <c r="Z15" s="15">
         <v>20</v>
@@ -2024,7 +2020,7 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" s="15"/>
       <c r="M17" s="15"/>
@@ -2033,10 +2029,10 @@
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D18" s="20">
         <v>1.78</v>
@@ -2121,7 +2117,7 @@
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="2"/>
@@ -2228,7 +2224,7 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1">
         <v>0.03</v>
@@ -2245,7 +2241,7 @@
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22" s="20">
         <v>0</v>
@@ -2334,7 +2330,7 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D23" s="20">
         <v>0</v>
@@ -2423,7 +2419,7 @@
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24" s="20">
         <v>0</v>
@@ -2512,7 +2508,7 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D25" s="20">
         <v>0</v>
@@ -2601,7 +2597,7 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" s="21">
         <f>SUM(D22:D25)</f>
@@ -2688,10 +2684,10 @@
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" s="20"/>
       <c r="G28" s="3"/>
@@ -2705,7 +2701,7 @@
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="13">
         <v>470531000</v>
@@ -2797,10 +2793,10 @@
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30" s="20">
         <v>1.7</v>
@@ -2889,10 +2885,10 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D31" s="20">
         <v>0.81</v>
@@ -2978,10 +2974,10 @@
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D32" s="20">
         <v>1.38</v>
@@ -3070,10 +3066,10 @@
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D33" s="20">
         <v>0.44</v>
@@ -3159,10 +3155,10 @@
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" s="20">
         <v>0.1</v>
@@ -3248,10 +3244,10 @@
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D35" s="20">
         <v>0.3</v>
@@ -3337,10 +3333,10 @@
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="20">
         <v>0.5</v>
@@ -3426,10 +3422,10 @@
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D37" s="20">
         <v>0.1</v>
@@ -3517,10 +3513,10 @@
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D38" s="20">
         <v>0.1</v>
@@ -3608,10 +3604,10 @@
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D39" s="20">
         <v>0.13</v>
@@ -3700,10 +3696,10 @@
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D40" s="20">
         <v>1.56</v>
@@ -3786,10 +3782,10 @@
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D41" s="20">
         <v>1.3</v>
@@ -3875,10 +3871,10 @@
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D42" s="20">
         <v>0.47</v>
@@ -3964,10 +3960,10 @@
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D43" s="20">
         <v>0.1</v>
@@ -4053,10 +4049,10 @@
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D44" s="20">
         <v>2.14</v>
@@ -4144,10 +4140,10 @@
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D45" s="20">
         <v>1.1499999999999999</v>
@@ -4235,10 +4231,10 @@
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D46" s="20">
         <v>1.42</v>
@@ -4413,7 +4409,7 @@
     </row>
     <row r="48" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="21">
@@ -4517,7 +4513,7 @@
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A50" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="20"/>
@@ -4532,7 +4528,7 @@
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.4">
       <c r="B51" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="20">
@@ -4620,7 +4616,7 @@
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A52" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D52" s="21">
         <f>SUM(D51:D51)</f>
@@ -4722,7 +4718,7 @@
     </row>
     <row r="54" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A54" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B54">
         <f>COUNTA(B3:B53)</f>
@@ -4770,27 +4766,27 @@
       </c>
       <c r="N54" s="9">
         <f t="shared" si="95"/>
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="O54" s="9">
         <f t="shared" si="95"/>
-        <v>1402</v>
+        <v>1405</v>
       </c>
       <c r="P54" s="9">
         <f t="shared" si="95"/>
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="Q54" s="8">
         <f>Q15+Q19+Q26+Q48+Q52</f>
-        <v>884.63789999999995</v>
+        <v>905.66932499999996</v>
       </c>
       <c r="R54" s="24">
         <f t="shared" ref="R54:Y54" si="96">R15+R19+R26+R48+R52</f>
-        <v>1638</v>
+        <v>1640</v>
       </c>
       <c r="S54" s="8">
         <f t="shared" si="96"/>
-        <v>742.0100000000001</v>
+        <v>824.07000000000016</v>
       </c>
       <c r="T54" s="8">
         <f t="shared" si="96"/>
@@ -4798,37 +4794,37 @@
       </c>
       <c r="U54" s="8">
         <f t="shared" si="96"/>
-        <v>71.085650000000001</v>
+        <v>79.905650000000009</v>
       </c>
       <c r="V54" s="8">
         <f t="shared" si="96"/>
-        <v>820.60564999999997</v>
+        <v>911.48564999999996</v>
       </c>
       <c r="W54" s="8">
         <f t="shared" si="96"/>
-        <v>46.295648102392335</v>
+        <v>50.120148102392335</v>
       </c>
       <c r="X54" s="8">
         <f t="shared" si="96"/>
-        <v>45.973225175119623</v>
+        <v>49.797725175119623</v>
       </c>
       <c r="Y54" s="8">
         <f t="shared" si="96"/>
-        <v>4.6278065748803847</v>
+        <v>0.80330657488038515</v>
       </c>
       <c r="Z54" s="15"/>
     </row>
     <row r="56" spans="1:27" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B56" s="27"/>
+      <c r="A56" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="28"/>
     </row>
     <row r="57" spans="1:27" ht="67.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B57" s="27"/>
+      <c r="A57" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4839,8 +4835,9 @@
     <hyperlink ref="C5" r:id="rId1" xr:uid="{ACAC5234-DDA0-4969-B5FE-D166D7000F40}"/>
     <hyperlink ref="C9" r:id="rId2" xr:uid="{AED873F4-67F0-430A-8DE3-7AABA9CDF44E}"/>
     <hyperlink ref="C18" r:id="rId3" xr:uid="{0FEF45BF-45A4-4B48-81CD-48A372ED4F15}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{BA25087D-F716-4915-9858-9E7D9D1E74A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>